<commit_message>
Reflection of corrections in the Japanese version
</commit_message>
<xml_diff>
--- a/en/Sample_Project/Design_Document/B1_Client_Management_System/030_Application_Design/030_Interface_Design/Web_Service_API_List_B1_Client_Management_System.xlsx
+++ b/en/Sample_Project/Design_Document/B1_Client_Management_System/030_Application_Design/030_Interface_Design/Web_Service_API_List_B1_Client_Management_System.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73D24EE-C5CC-4E53-A3AA-38B5136162B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985100E1-BDB4-4D1F-9B31-530BE73E4D3D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="3510" windowWidth="27090" windowHeight="10830" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="28" r:id="rId1"/>
@@ -27,9 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -129,9 +127,6 @@
   </si>
   <si>
     <t>GET</t>
-  </si>
-  <si>
-    <t>/Client?client_name=client name&amp;industry_code= industry code</t>
   </si>
   <si>
     <t>JSON</t>
@@ -314,6 +309,10 @@
       </rPr>
       <t>）</t>
     </r>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>/client?clientName=client name&amp;industryCode= industry code</t>
     <phoneticPr fontId="10"/>
   </si>
 </sst>
@@ -1335,248 +1334,8 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="11" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="12" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="10" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="11" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="12" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="32" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="32" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="14" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="24" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" xfId="41" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="25" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="24" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="25" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="17" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="18" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="32" fillId="0" borderId="10" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="32" fillId="0" borderId="11" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="177" fontId="32" fillId="0" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1597,6 +1356,56 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="24" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="25" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="10" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="11" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="32" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1606,6 +1415,24 @@
     <xf numFmtId="14" fontId="32" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1615,8 +1442,83 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="11" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="12" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="14" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="24" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" xfId="41" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="25" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="17" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="18" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="10" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="11" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="12" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1636,20 +1538,54 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="12" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="10" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="11" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="12" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="177" fontId="32" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="24" borderId="11" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="12" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="24" borderId="13" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1659,15 +1595,6 @@
     <xf numFmtId="0" fontId="33" fillId="24" borderId="15" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="10" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="11" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="12" xfId="41" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="24" borderId="24" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1685,6 +1612,78 @@
     </xf>
     <xf numFmtId="0" fontId="33" fillId="24" borderId="18" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -2434,7 +2433,9 @@
   </sheetPr>
   <dimension ref="A1:S513"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Y22" sqref="Y22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -2476,7 +2477,7 @@
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="J23" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="6:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2488,12 +2489,12 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="67">
+      <c r="I25" s="78">
         <f ca="1">IF(INDIRECT("'Revision history'!D8")="","",MAX(INDIRECT("'Revision history'!D8"):INDIRECT("'Revision history'!F33")))</f>
         <v>43404</v>
       </c>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
     </row>
     <row r="26" spans="6:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F26" s="5"/>
@@ -3087,1208 +3088,1363 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="4.83203125" style="169"/>
+    <col min="1" max="16384" width="4.83203125" style="76"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="105" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71" t="s">
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="110" t="s">
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="105" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="111"/>
-      <c r="Q1" s="111"/>
-      <c r="R1" s="112"/>
-      <c r="S1" s="113" t="s">
-        <v>60</v>
-      </c>
-      <c r="T1" s="114"/>
-      <c r="U1" s="114"/>
-      <c r="V1" s="114"/>
-      <c r="W1" s="114"/>
-      <c r="X1" s="114"/>
-      <c r="Y1" s="114"/>
-      <c r="Z1" s="115"/>
-      <c r="AA1" s="68" t="s">
+      <c r="AB1" s="107"/>
+      <c r="AC1" s="123" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="124"/>
+      <c r="AE1" s="124"/>
+      <c r="AF1" s="125"/>
+      <c r="AG1" s="88">
+        <v>43404</v>
+      </c>
+      <c r="AH1" s="89"/>
+      <c r="AI1" s="90"/>
+    </row>
+    <row r="2" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="75"/>
-      <c r="AF1" s="76"/>
-      <c r="AG1" s="142">
-        <v>43404</v>
-      </c>
-      <c r="AH1" s="143"/>
-      <c r="AI1" s="144"/>
-    </row>
-    <row r="2" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="68" t="s">
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="108" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71" t="s">
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="119"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="116"/>
-      <c r="P2" s="117"/>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="118"/>
-      <c r="S2" s="119"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="120"/>
-      <c r="X2" s="120"/>
-      <c r="Y2" s="120"/>
-      <c r="Z2" s="121"/>
-      <c r="AA2" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="145" t="str">
+      <c r="AB2" s="107"/>
+      <c r="AC2" s="111" t="str">
         <f ca="1">IF(COUNTA(AF9:AF33)&lt;&gt;0,INDIRECT("AF"&amp;(COUNTA(AF9:AF33)+8)),"")</f>
         <v/>
       </c>
-      <c r="AD2" s="146"/>
-      <c r="AE2" s="146"/>
-      <c r="AF2" s="147"/>
-      <c r="AG2" s="142" t="str">
+      <c r="AD2" s="112"/>
+      <c r="AE2" s="112"/>
+      <c r="AF2" s="113"/>
+      <c r="AG2" s="88" t="str">
         <f>IF(D9="","",MAX(D9:F33))</f>
         <v/>
       </c>
-      <c r="AH2" s="143"/>
-      <c r="AI2" s="144"/>
+      <c r="AH2" s="89"/>
+      <c r="AI2" s="90"/>
     </row>
     <row r="3" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="105" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="71" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="123"/>
-      <c r="Q3" s="123"/>
-      <c r="R3" s="124"/>
-      <c r="S3" s="125"/>
-      <c r="T3" s="126"/>
-      <c r="U3" s="126"/>
-      <c r="V3" s="126"/>
-      <c r="W3" s="126"/>
-      <c r="X3" s="126"/>
-      <c r="Y3" s="126"/>
-      <c r="Z3" s="127"/>
-      <c r="AA3" s="68"/>
-      <c r="AB3" s="70"/>
-      <c r="AC3" s="74"/>
-      <c r="AD3" s="75"/>
-      <c r="AE3" s="75"/>
-      <c r="AF3" s="76"/>
-      <c r="AG3" s="142"/>
-      <c r="AH3" s="143"/>
-      <c r="AI3" s="144"/>
-    </row>
-    <row r="5" spans="1:35" s="148" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N5" s="149" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA5" s="150"/>
-      <c r="AB5" s="150"/>
-      <c r="AC5" s="151"/>
-      <c r="AD5" s="152"/>
-      <c r="AE5" s="152"/>
-      <c r="AF5" s="152"/>
-      <c r="AG5" s="150"/>
-      <c r="AH5" s="150"/>
-      <c r="AI5" s="150"/>
-    </row>
-    <row r="6" spans="1:35" s="148" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="N6" s="149"/>
-      <c r="AA6" s="150"/>
-      <c r="AB6" s="150"/>
-      <c r="AC6" s="151"/>
-      <c r="AD6" s="152"/>
-      <c r="AE6" s="152"/>
-      <c r="AF6" s="152"/>
-      <c r="AG6" s="150"/>
-      <c r="AH6" s="150"/>
-      <c r="AI6" s="150"/>
-    </row>
-    <row r="7" spans="1:35" s="153" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="128" t="s">
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="110"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="121"/>
+      <c r="Q3" s="121"/>
+      <c r="R3" s="122"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="86"/>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="86"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="105"/>
+      <c r="AB3" s="107"/>
+      <c r="AC3" s="123"/>
+      <c r="AD3" s="124"/>
+      <c r="AE3" s="124"/>
+      <c r="AF3" s="125"/>
+      <c r="AG3" s="88"/>
+      <c r="AH3" s="89"/>
+      <c r="AI3" s="90"/>
+    </row>
+    <row r="5" spans="1:35" s="68" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA5" s="70"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="71"/>
+      <c r="AD5" s="72"/>
+      <c r="AE5" s="72"/>
+      <c r="AF5" s="72"/>
+      <c r="AG5" s="70"/>
+      <c r="AH5" s="70"/>
+      <c r="AI5" s="70"/>
+    </row>
+    <row r="6" spans="1:35" s="68" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N6" s="69"/>
+      <c r="AA6" s="70"/>
+      <c r="AB6" s="70"/>
+      <c r="AC6" s="71"/>
+      <c r="AD6" s="72"/>
+      <c r="AE6" s="72"/>
+      <c r="AF6" s="72"/>
+      <c r="AG6" s="70"/>
+      <c r="AH6" s="70"/>
+      <c r="AI6" s="70"/>
+    </row>
+    <row r="7" spans="1:35" s="73" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="129" t="s">
+      <c r="B7" s="126" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="127"/>
+      <c r="D7" s="128" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="130"/>
-      <c r="D7" s="131" t="s">
+      <c r="E7" s="129"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="132"/>
-      <c r="F7" s="133"/>
-      <c r="G7" s="131" t="s">
+      <c r="H7" s="129"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="128" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="132"/>
-      <c r="I7" s="133"/>
-      <c r="J7" s="131" t="s">
+      <c r="K7" s="129"/>
+      <c r="L7" s="129"/>
+      <c r="M7" s="129"/>
+      <c r="N7" s="129"/>
+      <c r="O7" s="129"/>
+      <c r="P7" s="130"/>
+      <c r="Q7" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="132"/>
-      <c r="L7" s="132"/>
-      <c r="M7" s="132"/>
-      <c r="N7" s="132"/>
-      <c r="O7" s="132"/>
-      <c r="P7" s="133"/>
-      <c r="Q7" s="131" t="s">
+      <c r="R7" s="129"/>
+      <c r="S7" s="129"/>
+      <c r="T7" s="129"/>
+      <c r="U7" s="129"/>
+      <c r="V7" s="129"/>
+      <c r="W7" s="129"/>
+      <c r="X7" s="129"/>
+      <c r="Y7" s="129"/>
+      <c r="Z7" s="129"/>
+      <c r="AA7" s="129"/>
+      <c r="AB7" s="129"/>
+      <c r="AC7" s="129"/>
+      <c r="AD7" s="129"/>
+      <c r="AE7" s="130"/>
+      <c r="AF7" s="128" t="s">
         <v>65</v>
       </c>
-      <c r="R7" s="132"/>
-      <c r="S7" s="132"/>
-      <c r="T7" s="132"/>
-      <c r="U7" s="132"/>
-      <c r="V7" s="132"/>
-      <c r="W7" s="132"/>
-      <c r="X7" s="132"/>
-      <c r="Y7" s="132"/>
-      <c r="Z7" s="132"/>
-      <c r="AA7" s="132"/>
-      <c r="AB7" s="132"/>
-      <c r="AC7" s="132"/>
-      <c r="AD7" s="132"/>
-      <c r="AE7" s="133"/>
-      <c r="AF7" s="131" t="s">
+      <c r="AG7" s="129"/>
+      <c r="AH7" s="129"/>
+      <c r="AI7" s="130"/>
+    </row>
+    <row r="8" spans="1:35" s="73" customFormat="1" ht="26.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="74">
+        <v>1</v>
+      </c>
+      <c r="B8" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="92"/>
+      <c r="D8" s="93">
+        <v>43404</v>
+      </c>
+      <c r="E8" s="94"/>
+      <c r="F8" s="95"/>
+      <c r="G8" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="AG7" s="132"/>
-      <c r="AH7" s="132"/>
-      <c r="AI7" s="133"/>
-    </row>
-    <row r="8" spans="1:35" s="153" customFormat="1" ht="26.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="154">
-        <v>1</v>
-      </c>
-      <c r="B8" s="134" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="135"/>
-      <c r="D8" s="155">
-        <v>43404</v>
-      </c>
-      <c r="E8" s="156"/>
-      <c r="F8" s="157"/>
-      <c r="G8" s="136" t="s">
+      <c r="H8" s="97"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="99" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="100"/>
+      <c r="N8" s="100"/>
+      <c r="O8" s="100"/>
+      <c r="P8" s="101"/>
+      <c r="Q8" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="H8" s="137"/>
-      <c r="I8" s="138"/>
-      <c r="J8" s="139" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="140"/>
-      <c r="L8" s="140"/>
-      <c r="M8" s="140"/>
-      <c r="N8" s="140"/>
-      <c r="O8" s="140"/>
-      <c r="P8" s="141"/>
-      <c r="Q8" s="139" t="s">
-        <v>68</v>
-      </c>
-      <c r="R8" s="140"/>
-      <c r="S8" s="140"/>
-      <c r="T8" s="140"/>
-      <c r="U8" s="140"/>
-      <c r="V8" s="140"/>
-      <c r="W8" s="140"/>
-      <c r="X8" s="140"/>
-      <c r="Y8" s="140"/>
-      <c r="Z8" s="140"/>
-      <c r="AA8" s="140"/>
-      <c r="AB8" s="140"/>
-      <c r="AC8" s="140"/>
-      <c r="AD8" s="140"/>
-      <c r="AE8" s="141"/>
-      <c r="AF8" s="158" t="s">
+      <c r="R8" s="100"/>
+      <c r="S8" s="100"/>
+      <c r="T8" s="100"/>
+      <c r="U8" s="100"/>
+      <c r="V8" s="100"/>
+      <c r="W8" s="100"/>
+      <c r="X8" s="100"/>
+      <c r="Y8" s="100"/>
+      <c r="Z8" s="100"/>
+      <c r="AA8" s="100"/>
+      <c r="AB8" s="100"/>
+      <c r="AC8" s="100"/>
+      <c r="AD8" s="100"/>
+      <c r="AE8" s="101"/>
+      <c r="AF8" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="AG8" s="159"/>
-      <c r="AH8" s="159"/>
-      <c r="AI8" s="160"/>
-    </row>
-    <row r="9" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="161"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="165"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="164"/>
-      <c r="H9" s="167"/>
-      <c r="I9" s="163"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="81"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="89"/>
-      <c r="R9" s="90"/>
-      <c r="S9" s="90"/>
-      <c r="T9" s="90"/>
-      <c r="U9" s="90"/>
-      <c r="V9" s="90"/>
-      <c r="W9" s="90"/>
-      <c r="X9" s="90"/>
-      <c r="Y9" s="90"/>
-      <c r="Z9" s="90"/>
-      <c r="AA9" s="90"/>
-      <c r="AB9" s="90"/>
-      <c r="AC9" s="90"/>
-      <c r="AD9" s="90"/>
-      <c r="AE9" s="91"/>
-      <c r="AF9" s="80"/>
-      <c r="AG9" s="81"/>
-      <c r="AH9" s="81"/>
-      <c r="AI9" s="82"/>
-    </row>
-    <row r="10" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="161"/>
-      <c r="B10" s="162"/>
-      <c r="C10" s="163"/>
-      <c r="D10" s="164"/>
-      <c r="E10" s="165"/>
-      <c r="F10" s="166"/>
-      <c r="G10" s="162"/>
-      <c r="H10" s="167"/>
-      <c r="I10" s="163"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="82"/>
-      <c r="Q10" s="89"/>
-      <c r="R10" s="90"/>
-      <c r="S10" s="90"/>
-      <c r="T10" s="90"/>
-      <c r="U10" s="90"/>
-      <c r="V10" s="90"/>
-      <c r="W10" s="90"/>
-      <c r="X10" s="90"/>
-      <c r="Y10" s="90"/>
-      <c r="Z10" s="90"/>
-      <c r="AA10" s="90"/>
-      <c r="AB10" s="90"/>
-      <c r="AC10" s="90"/>
-      <c r="AD10" s="90"/>
-      <c r="AE10" s="91"/>
-      <c r="AF10" s="80"/>
-      <c r="AG10" s="81"/>
-      <c r="AH10" s="81"/>
-      <c r="AI10" s="82"/>
-    </row>
-    <row r="11" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="161"/>
-      <c r="B11" s="162"/>
-      <c r="C11" s="163"/>
-      <c r="D11" s="164"/>
-      <c r="E11" s="165"/>
-      <c r="F11" s="166"/>
-      <c r="G11" s="162"/>
-      <c r="H11" s="167"/>
-      <c r="I11" s="163"/>
-      <c r="J11" s="80"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="82"/>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="90"/>
-      <c r="T11" s="90"/>
-      <c r="U11" s="90"/>
-      <c r="V11" s="90"/>
-      <c r="W11" s="90"/>
-      <c r="X11" s="90"/>
-      <c r="Y11" s="90"/>
-      <c r="Z11" s="90"/>
-      <c r="AA11" s="90"/>
-      <c r="AB11" s="90"/>
-      <c r="AC11" s="90"/>
-      <c r="AD11" s="90"/>
-      <c r="AE11" s="91"/>
-      <c r="AF11" s="80"/>
-      <c r="AG11" s="81"/>
-      <c r="AH11" s="81"/>
-      <c r="AI11" s="82"/>
-    </row>
-    <row r="12" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="161"/>
-      <c r="B12" s="162"/>
-      <c r="C12" s="163"/>
-      <c r="D12" s="164"/>
-      <c r="E12" s="165"/>
-      <c r="F12" s="166"/>
-      <c r="G12" s="162"/>
-      <c r="H12" s="167"/>
-      <c r="I12" s="163"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="81"/>
-      <c r="M12" s="81"/>
-      <c r="N12" s="81"/>
-      <c r="O12" s="81"/>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
-      <c r="T12" s="90"/>
-      <c r="U12" s="90"/>
-      <c r="V12" s="90"/>
-      <c r="W12" s="90"/>
-      <c r="X12" s="90"/>
-      <c r="Y12" s="90"/>
-      <c r="Z12" s="90"/>
-      <c r="AA12" s="90"/>
-      <c r="AB12" s="90"/>
-      <c r="AC12" s="90"/>
-      <c r="AD12" s="90"/>
-      <c r="AE12" s="91"/>
-      <c r="AF12" s="80"/>
-      <c r="AG12" s="81"/>
-      <c r="AH12" s="81"/>
-      <c r="AI12" s="82"/>
-    </row>
-    <row r="13" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="161"/>
-      <c r="B13" s="162"/>
-      <c r="C13" s="163"/>
-      <c r="D13" s="164"/>
-      <c r="E13" s="165"/>
-      <c r="F13" s="166"/>
-      <c r="G13" s="162"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="163"/>
-      <c r="J13" s="80"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="90"/>
-      <c r="S13" s="90"/>
-      <c r="T13" s="90"/>
-      <c r="U13" s="90"/>
-      <c r="V13" s="90"/>
-      <c r="W13" s="90"/>
-      <c r="X13" s="90"/>
-      <c r="Y13" s="90"/>
-      <c r="Z13" s="90"/>
-      <c r="AA13" s="90"/>
-      <c r="AB13" s="90"/>
-      <c r="AC13" s="90"/>
-      <c r="AD13" s="90"/>
-      <c r="AE13" s="91"/>
-      <c r="AF13" s="80"/>
-      <c r="AG13" s="81"/>
-      <c r="AH13" s="81"/>
-      <c r="AI13" s="82"/>
-    </row>
-    <row r="14" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="161"/>
-      <c r="B14" s="162"/>
-      <c r="C14" s="163"/>
-      <c r="D14" s="164"/>
-      <c r="E14" s="165"/>
-      <c r="F14" s="166"/>
-      <c r="G14" s="162"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="163"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="82"/>
-      <c r="Q14" s="89"/>
-      <c r="R14" s="90"/>
-      <c r="S14" s="90"/>
-      <c r="T14" s="90"/>
-      <c r="U14" s="90"/>
-      <c r="V14" s="90"/>
-      <c r="W14" s="90"/>
-      <c r="X14" s="90"/>
-      <c r="Y14" s="90"/>
-      <c r="Z14" s="90"/>
-      <c r="AA14" s="90"/>
-      <c r="AB14" s="90"/>
-      <c r="AC14" s="90"/>
-      <c r="AD14" s="90"/>
-      <c r="AE14" s="91"/>
-      <c r="AF14" s="80"/>
-      <c r="AG14" s="81"/>
-      <c r="AH14" s="81"/>
-      <c r="AI14" s="82"/>
-    </row>
-    <row r="15" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="161"/>
-      <c r="B15" s="162"/>
-      <c r="C15" s="163"/>
-      <c r="D15" s="164"/>
-      <c r="E15" s="165"/>
-      <c r="F15" s="166"/>
-      <c r="G15" s="162"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="163"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="81"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="82"/>
-      <c r="Q15" s="89"/>
-      <c r="R15" s="90"/>
-      <c r="S15" s="90"/>
-      <c r="T15" s="90"/>
-      <c r="U15" s="90"/>
-      <c r="V15" s="90"/>
-      <c r="W15" s="90"/>
-      <c r="X15" s="90"/>
-      <c r="Y15" s="90"/>
-      <c r="Z15" s="90"/>
-      <c r="AA15" s="90"/>
-      <c r="AB15" s="90"/>
-      <c r="AC15" s="90"/>
-      <c r="AD15" s="90"/>
-      <c r="AE15" s="91"/>
-      <c r="AF15" s="80"/>
-      <c r="AG15" s="81"/>
-      <c r="AH15" s="81"/>
-      <c r="AI15" s="82"/>
-    </row>
-    <row r="16" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="161"/>
-      <c r="B16" s="162"/>
-      <c r="C16" s="163"/>
-      <c r="D16" s="164"/>
-      <c r="E16" s="165"/>
-      <c r="F16" s="166"/>
-      <c r="G16" s="162"/>
-      <c r="H16" s="167"/>
-      <c r="I16" s="163"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="81"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="82"/>
-      <c r="Q16" s="89"/>
-      <c r="R16" s="90"/>
-      <c r="S16" s="90"/>
-      <c r="T16" s="90"/>
-      <c r="U16" s="90"/>
-      <c r="V16" s="90"/>
-      <c r="W16" s="90"/>
-      <c r="X16" s="90"/>
-      <c r="Y16" s="90"/>
-      <c r="Z16" s="90"/>
-      <c r="AA16" s="90"/>
-      <c r="AB16" s="90"/>
-      <c r="AC16" s="90"/>
-      <c r="AD16" s="90"/>
-      <c r="AE16" s="91"/>
-      <c r="AF16" s="80"/>
-      <c r="AG16" s="81"/>
-      <c r="AH16" s="81"/>
-      <c r="AI16" s="82"/>
-    </row>
-    <row r="17" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="161"/>
-      <c r="B17" s="162"/>
-      <c r="C17" s="163"/>
-      <c r="D17" s="164"/>
-      <c r="E17" s="165"/>
-      <c r="F17" s="166"/>
-      <c r="G17" s="162"/>
-      <c r="H17" s="167"/>
-      <c r="I17" s="163"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="81"/>
-      <c r="L17" s="81"/>
-      <c r="M17" s="81"/>
-      <c r="N17" s="81"/>
-      <c r="O17" s="81"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="89"/>
-      <c r="R17" s="90"/>
-      <c r="S17" s="90"/>
-      <c r="T17" s="90"/>
-      <c r="U17" s="90"/>
-      <c r="V17" s="90"/>
-      <c r="W17" s="90"/>
-      <c r="X17" s="90"/>
-      <c r="Y17" s="90"/>
-      <c r="Z17" s="90"/>
-      <c r="AA17" s="90"/>
-      <c r="AB17" s="90"/>
-      <c r="AC17" s="90"/>
-      <c r="AD17" s="90"/>
-      <c r="AE17" s="91"/>
-      <c r="AF17" s="80"/>
-      <c r="AG17" s="81"/>
-      <c r="AH17" s="81"/>
-      <c r="AI17" s="82"/>
-    </row>
-    <row r="18" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="161"/>
-      <c r="B18" s="162"/>
-      <c r="C18" s="163"/>
-      <c r="D18" s="164"/>
-      <c r="E18" s="165"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="162"/>
-      <c r="H18" s="167"/>
-      <c r="I18" s="163"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="81"/>
-      <c r="N18" s="81"/>
-      <c r="O18" s="81"/>
-      <c r="P18" s="82"/>
-      <c r="Q18" s="89"/>
-      <c r="R18" s="90"/>
-      <c r="S18" s="90"/>
-      <c r="T18" s="90"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="90"/>
-      <c r="W18" s="90"/>
-      <c r="X18" s="90"/>
-      <c r="Y18" s="90"/>
-      <c r="Z18" s="90"/>
-      <c r="AA18" s="90"/>
-      <c r="AB18" s="90"/>
-      <c r="AC18" s="90"/>
-      <c r="AD18" s="90"/>
-      <c r="AE18" s="91"/>
-      <c r="AF18" s="80"/>
-      <c r="AG18" s="81"/>
-      <c r="AH18" s="81"/>
-      <c r="AI18" s="82"/>
-    </row>
-    <row r="19" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="161"/>
-      <c r="B19" s="162"/>
-      <c r="C19" s="163"/>
-      <c r="D19" s="164"/>
-      <c r="E19" s="165"/>
-      <c r="F19" s="166"/>
-      <c r="G19" s="162"/>
-      <c r="H19" s="167"/>
-      <c r="I19" s="163"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="81"/>
-      <c r="O19" s="81"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="89"/>
-      <c r="R19" s="90"/>
-      <c r="S19" s="90"/>
-      <c r="T19" s="90"/>
-      <c r="U19" s="90"/>
-      <c r="V19" s="90"/>
-      <c r="W19" s="90"/>
-      <c r="X19" s="90"/>
-      <c r="Y19" s="90"/>
-      <c r="Z19" s="90"/>
-      <c r="AA19" s="90"/>
-      <c r="AB19" s="90"/>
-      <c r="AC19" s="90"/>
-      <c r="AD19" s="90"/>
-      <c r="AE19" s="91"/>
-      <c r="AF19" s="80"/>
-      <c r="AG19" s="81"/>
-      <c r="AH19" s="81"/>
-      <c r="AI19" s="82"/>
-    </row>
-    <row r="20" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="161"/>
-      <c r="B20" s="162"/>
-      <c r="C20" s="163"/>
-      <c r="D20" s="164"/>
-      <c r="E20" s="165"/>
-      <c r="F20" s="166"/>
-      <c r="G20" s="162"/>
-      <c r="H20" s="167"/>
-      <c r="I20" s="163"/>
-      <c r="J20" s="80"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="81"/>
-      <c r="N20" s="81"/>
-      <c r="O20" s="81"/>
-      <c r="P20" s="82"/>
-      <c r="Q20" s="89"/>
-      <c r="R20" s="90"/>
-      <c r="S20" s="90"/>
-      <c r="T20" s="90"/>
-      <c r="U20" s="90"/>
-      <c r="V20" s="90"/>
-      <c r="W20" s="90"/>
-      <c r="X20" s="90"/>
-      <c r="Y20" s="90"/>
-      <c r="Z20" s="90"/>
-      <c r="AA20" s="90"/>
-      <c r="AB20" s="90"/>
-      <c r="AC20" s="90"/>
-      <c r="AD20" s="90"/>
-      <c r="AE20" s="91"/>
-      <c r="AF20" s="80"/>
-      <c r="AG20" s="81"/>
-      <c r="AH20" s="81"/>
-      <c r="AI20" s="82"/>
-    </row>
-    <row r="21" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="161"/>
-      <c r="B21" s="162"/>
-      <c r="C21" s="163"/>
-      <c r="D21" s="164"/>
-      <c r="E21" s="165"/>
-      <c r="F21" s="166"/>
-      <c r="G21" s="162"/>
-      <c r="H21" s="167"/>
-      <c r="I21" s="163"/>
-      <c r="J21" s="80"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="81"/>
-      <c r="N21" s="81"/>
-      <c r="O21" s="81"/>
-      <c r="P21" s="82"/>
-      <c r="Q21" s="89"/>
-      <c r="R21" s="90"/>
-      <c r="S21" s="90"/>
-      <c r="T21" s="90"/>
-      <c r="U21" s="90"/>
-      <c r="V21" s="90"/>
-      <c r="W21" s="90"/>
-      <c r="X21" s="90"/>
-      <c r="Y21" s="90"/>
-      <c r="Z21" s="90"/>
-      <c r="AA21" s="90"/>
-      <c r="AB21" s="90"/>
-      <c r="AC21" s="90"/>
-      <c r="AD21" s="90"/>
-      <c r="AE21" s="91"/>
-      <c r="AF21" s="80"/>
-      <c r="AG21" s="81"/>
-      <c r="AH21" s="81"/>
-      <c r="AI21" s="82"/>
-    </row>
-    <row r="22" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="161"/>
-      <c r="B22" s="162"/>
-      <c r="C22" s="163"/>
-      <c r="D22" s="164"/>
-      <c r="E22" s="165"/>
-      <c r="F22" s="166"/>
-      <c r="G22" s="162"/>
-      <c r="H22" s="167"/>
-      <c r="I22" s="163"/>
-      <c r="J22" s="80"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="81"/>
-      <c r="P22" s="82"/>
-      <c r="Q22" s="89"/>
-      <c r="R22" s="90"/>
-      <c r="S22" s="90"/>
-      <c r="T22" s="90"/>
-      <c r="U22" s="90"/>
-      <c r="V22" s="90"/>
-      <c r="W22" s="90"/>
-      <c r="X22" s="90"/>
-      <c r="Y22" s="90"/>
-      <c r="Z22" s="90"/>
-      <c r="AA22" s="90"/>
-      <c r="AB22" s="90"/>
-      <c r="AC22" s="90"/>
-      <c r="AD22" s="90"/>
-      <c r="AE22" s="91"/>
-      <c r="AF22" s="80"/>
-      <c r="AG22" s="81"/>
-      <c r="AH22" s="81"/>
-      <c r="AI22" s="82"/>
-    </row>
-    <row r="23" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="161"/>
-      <c r="B23" s="162"/>
-      <c r="C23" s="163"/>
-      <c r="D23" s="164"/>
-      <c r="E23" s="165"/>
-      <c r="F23" s="166"/>
-      <c r="G23" s="162"/>
-      <c r="H23" s="167"/>
-      <c r="I23" s="163"/>
-      <c r="J23" s="80"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="81"/>
-      <c r="M23" s="81"/>
-      <c r="N23" s="81"/>
-      <c r="O23" s="81"/>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="89"/>
-      <c r="R23" s="90"/>
-      <c r="S23" s="90"/>
-      <c r="T23" s="90"/>
-      <c r="U23" s="90"/>
-      <c r="V23" s="90"/>
-      <c r="W23" s="90"/>
-      <c r="X23" s="90"/>
-      <c r="Y23" s="90"/>
-      <c r="Z23" s="90"/>
-      <c r="AA23" s="90"/>
-      <c r="AB23" s="90"/>
-      <c r="AC23" s="90"/>
-      <c r="AD23" s="90"/>
-      <c r="AE23" s="91"/>
-      <c r="AF23" s="80"/>
-      <c r="AG23" s="81"/>
-      <c r="AH23" s="81"/>
-      <c r="AI23" s="82"/>
-    </row>
-    <row r="24" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="161"/>
-      <c r="B24" s="162"/>
-      <c r="C24" s="163"/>
-      <c r="D24" s="164"/>
-      <c r="E24" s="165"/>
-      <c r="F24" s="166"/>
-      <c r="G24" s="162"/>
-      <c r="H24" s="167"/>
-      <c r="I24" s="163"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="81"/>
-      <c r="L24" s="81"/>
-      <c r="M24" s="81"/>
-      <c r="N24" s="81"/>
-      <c r="O24" s="81"/>
-      <c r="P24" s="82"/>
-      <c r="Q24" s="89"/>
-      <c r="R24" s="90"/>
-      <c r="S24" s="90"/>
-      <c r="T24" s="90"/>
-      <c r="U24" s="90"/>
-      <c r="V24" s="90"/>
-      <c r="W24" s="90"/>
-      <c r="X24" s="90"/>
-      <c r="Y24" s="90"/>
-      <c r="Z24" s="90"/>
-      <c r="AA24" s="90"/>
-      <c r="AB24" s="90"/>
-      <c r="AC24" s="90"/>
-      <c r="AD24" s="90"/>
-      <c r="AE24" s="91"/>
-      <c r="AF24" s="80"/>
-      <c r="AG24" s="81"/>
-      <c r="AH24" s="81"/>
-      <c r="AI24" s="82"/>
-    </row>
-    <row r="25" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="161"/>
-      <c r="B25" s="162"/>
-      <c r="C25" s="163"/>
-      <c r="D25" s="164"/>
-      <c r="E25" s="165"/>
-      <c r="F25" s="166"/>
-      <c r="G25" s="162"/>
-      <c r="H25" s="167"/>
-      <c r="I25" s="163"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="81"/>
-      <c r="L25" s="81"/>
-      <c r="M25" s="81"/>
-      <c r="N25" s="81"/>
-      <c r="O25" s="81"/>
-      <c r="P25" s="82"/>
-      <c r="Q25" s="89"/>
-      <c r="R25" s="90"/>
-      <c r="S25" s="90"/>
-      <c r="T25" s="90"/>
-      <c r="U25" s="90"/>
-      <c r="V25" s="90"/>
-      <c r="W25" s="90"/>
-      <c r="X25" s="90"/>
-      <c r="Y25" s="90"/>
-      <c r="Z25" s="90"/>
-      <c r="AA25" s="90"/>
-      <c r="AB25" s="90"/>
-      <c r="AC25" s="90"/>
-      <c r="AD25" s="90"/>
-      <c r="AE25" s="91"/>
-      <c r="AF25" s="80"/>
-      <c r="AG25" s="81"/>
-      <c r="AH25" s="81"/>
-      <c r="AI25" s="82"/>
-    </row>
-    <row r="26" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="161"/>
-      <c r="B26" s="162"/>
-      <c r="C26" s="163"/>
-      <c r="D26" s="164"/>
-      <c r="E26" s="165"/>
-      <c r="F26" s="166"/>
-      <c r="G26" s="162"/>
-      <c r="H26" s="167"/>
-      <c r="I26" s="163"/>
-      <c r="J26" s="80"/>
-      <c r="K26" s="81"/>
-      <c r="L26" s="81"/>
-      <c r="M26" s="81"/>
-      <c r="N26" s="81"/>
-      <c r="O26" s="81"/>
-      <c r="P26" s="82"/>
-      <c r="Q26" s="89"/>
-      <c r="R26" s="90"/>
-      <c r="S26" s="90"/>
-      <c r="T26" s="90"/>
-      <c r="U26" s="90"/>
-      <c r="V26" s="90"/>
-      <c r="W26" s="90"/>
-      <c r="X26" s="90"/>
-      <c r="Y26" s="90"/>
-      <c r="Z26" s="90"/>
-      <c r="AA26" s="90"/>
-      <c r="AB26" s="90"/>
-      <c r="AC26" s="90"/>
-      <c r="AD26" s="90"/>
-      <c r="AE26" s="91"/>
-      <c r="AF26" s="80"/>
-      <c r="AG26" s="81"/>
-      <c r="AH26" s="81"/>
-      <c r="AI26" s="82"/>
-    </row>
-    <row r="27" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="161"/>
-      <c r="B27" s="162"/>
-      <c r="C27" s="163"/>
-      <c r="D27" s="164"/>
-      <c r="E27" s="165"/>
-      <c r="F27" s="166"/>
-      <c r="G27" s="162"/>
-      <c r="H27" s="167"/>
-      <c r="I27" s="163"/>
-      <c r="J27" s="80"/>
-      <c r="K27" s="81"/>
-      <c r="L27" s="81"/>
-      <c r="M27" s="81"/>
-      <c r="N27" s="81"/>
-      <c r="O27" s="81"/>
-      <c r="P27" s="82"/>
-      <c r="Q27" s="89"/>
-      <c r="R27" s="90"/>
-      <c r="S27" s="90"/>
-      <c r="T27" s="90"/>
-      <c r="U27" s="90"/>
-      <c r="V27" s="90"/>
-      <c r="W27" s="90"/>
-      <c r="X27" s="90"/>
-      <c r="Y27" s="90"/>
-      <c r="Z27" s="90"/>
-      <c r="AA27" s="90"/>
-      <c r="AB27" s="90"/>
-      <c r="AC27" s="90"/>
-      <c r="AD27" s="90"/>
-      <c r="AE27" s="91"/>
-      <c r="AF27" s="80"/>
-      <c r="AG27" s="81"/>
-      <c r="AH27" s="81"/>
-      <c r="AI27" s="82"/>
-    </row>
-    <row r="28" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="161"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="164"/>
-      <c r="E28" s="165"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="162"/>
-      <c r="H28" s="167"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="81"/>
-      <c r="L28" s="81"/>
-      <c r="M28" s="81"/>
-      <c r="N28" s="81"/>
-      <c r="O28" s="81"/>
-      <c r="P28" s="82"/>
-      <c r="Q28" s="89"/>
-      <c r="R28" s="90"/>
-      <c r="S28" s="90"/>
-      <c r="T28" s="90"/>
-      <c r="U28" s="90"/>
-      <c r="V28" s="90"/>
-      <c r="W28" s="90"/>
-      <c r="X28" s="90"/>
-      <c r="Y28" s="90"/>
-      <c r="Z28" s="90"/>
-      <c r="AA28" s="90"/>
-      <c r="AB28" s="90"/>
-      <c r="AC28" s="90"/>
-      <c r="AD28" s="90"/>
-      <c r="AE28" s="91"/>
-      <c r="AF28" s="80"/>
-      <c r="AG28" s="81"/>
-      <c r="AH28" s="81"/>
-      <c r="AI28" s="82"/>
-    </row>
-    <row r="29" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="161"/>
-      <c r="B29" s="162"/>
-      <c r="C29" s="163"/>
-      <c r="D29" s="164"/>
-      <c r="E29" s="165"/>
-      <c r="F29" s="166"/>
-      <c r="G29" s="162"/>
-      <c r="H29" s="167"/>
-      <c r="I29" s="163"/>
-      <c r="J29" s="80"/>
-      <c r="K29" s="81"/>
-      <c r="L29" s="81"/>
-      <c r="M29" s="81"/>
-      <c r="N29" s="81"/>
-      <c r="O29" s="81"/>
-      <c r="P29" s="82"/>
-      <c r="Q29" s="89"/>
-      <c r="R29" s="90"/>
-      <c r="S29" s="90"/>
-      <c r="T29" s="90"/>
-      <c r="U29" s="90"/>
-      <c r="V29" s="90"/>
-      <c r="W29" s="90"/>
-      <c r="X29" s="90"/>
-      <c r="Y29" s="90"/>
-      <c r="Z29" s="90"/>
-      <c r="AA29" s="90"/>
-      <c r="AB29" s="90"/>
-      <c r="AC29" s="90"/>
-      <c r="AD29" s="90"/>
-      <c r="AE29" s="91"/>
-      <c r="AF29" s="80"/>
-      <c r="AG29" s="81"/>
-      <c r="AH29" s="81"/>
-      <c r="AI29" s="82"/>
-    </row>
-    <row r="30" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="161"/>
-      <c r="B30" s="162"/>
-      <c r="C30" s="163"/>
-      <c r="D30" s="164"/>
-      <c r="E30" s="165"/>
-      <c r="F30" s="166"/>
-      <c r="G30" s="162"/>
-      <c r="H30" s="167"/>
-      <c r="I30" s="163"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="81"/>
-      <c r="L30" s="81"/>
-      <c r="M30" s="81"/>
-      <c r="N30" s="81"/>
-      <c r="O30" s="81"/>
-      <c r="P30" s="82"/>
-      <c r="Q30" s="89"/>
-      <c r="R30" s="90"/>
-      <c r="S30" s="90"/>
-      <c r="T30" s="90"/>
-      <c r="U30" s="90"/>
-      <c r="V30" s="90"/>
-      <c r="W30" s="90"/>
-      <c r="X30" s="90"/>
-      <c r="Y30" s="90"/>
-      <c r="Z30" s="90"/>
-      <c r="AA30" s="90"/>
-      <c r="AB30" s="90"/>
-      <c r="AC30" s="90"/>
-      <c r="AD30" s="90"/>
-      <c r="AE30" s="91"/>
-      <c r="AF30" s="80"/>
-      <c r="AG30" s="81"/>
-      <c r="AH30" s="81"/>
-      <c r="AI30" s="82"/>
-    </row>
-    <row r="31" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="161"/>
-      <c r="B31" s="162"/>
-      <c r="C31" s="163"/>
-      <c r="D31" s="164"/>
-      <c r="E31" s="165"/>
-      <c r="F31" s="166"/>
-      <c r="G31" s="162"/>
-      <c r="H31" s="167"/>
-      <c r="I31" s="163"/>
-      <c r="J31" s="80"/>
-      <c r="K31" s="81"/>
-      <c r="L31" s="81"/>
-      <c r="M31" s="81"/>
-      <c r="N31" s="81"/>
-      <c r="O31" s="81"/>
-      <c r="P31" s="82"/>
-      <c r="Q31" s="89"/>
-      <c r="R31" s="90"/>
-      <c r="S31" s="90"/>
-      <c r="T31" s="90"/>
-      <c r="U31" s="90"/>
-      <c r="V31" s="90"/>
-      <c r="W31" s="90"/>
-      <c r="X31" s="90"/>
-      <c r="Y31" s="90"/>
-      <c r="Z31" s="90"/>
-      <c r="AA31" s="90"/>
-      <c r="AB31" s="90"/>
-      <c r="AC31" s="90"/>
-      <c r="AD31" s="90"/>
-      <c r="AE31" s="91"/>
-      <c r="AF31" s="80"/>
-      <c r="AG31" s="81"/>
-      <c r="AH31" s="81"/>
-      <c r="AI31" s="82"/>
-    </row>
-    <row r="32" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="161"/>
-      <c r="B32" s="162"/>
-      <c r="C32" s="163"/>
-      <c r="D32" s="164"/>
-      <c r="E32" s="165"/>
-      <c r="F32" s="166"/>
-      <c r="G32" s="162"/>
-      <c r="H32" s="167"/>
-      <c r="I32" s="163"/>
-      <c r="J32" s="80"/>
-      <c r="K32" s="168"/>
-      <c r="L32" s="81"/>
-      <c r="M32" s="81"/>
-      <c r="N32" s="81"/>
-      <c r="O32" s="81"/>
-      <c r="P32" s="82"/>
-      <c r="Q32" s="89"/>
-      <c r="R32" s="90"/>
-      <c r="S32" s="90"/>
-      <c r="T32" s="90"/>
-      <c r="U32" s="90"/>
-      <c r="V32" s="90"/>
-      <c r="W32" s="90"/>
-      <c r="X32" s="90"/>
-      <c r="Y32" s="90"/>
-      <c r="Z32" s="90"/>
-      <c r="AA32" s="90"/>
-      <c r="AB32" s="90"/>
-      <c r="AC32" s="90"/>
-      <c r="AD32" s="90"/>
-      <c r="AE32" s="91"/>
-      <c r="AF32" s="80"/>
-      <c r="AG32" s="81"/>
-      <c r="AH32" s="81"/>
-      <c r="AI32" s="82"/>
-    </row>
-    <row r="33" spans="1:35" s="153" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="161"/>
-      <c r="B33" s="162"/>
-      <c r="C33" s="163"/>
-      <c r="D33" s="164"/>
-      <c r="E33" s="165"/>
-      <c r="F33" s="166"/>
-      <c r="G33" s="162"/>
-      <c r="H33" s="167"/>
-      <c r="I33" s="163"/>
-      <c r="J33" s="80"/>
-      <c r="K33" s="81"/>
-      <c r="L33" s="81"/>
-      <c r="M33" s="81"/>
-      <c r="N33" s="81"/>
-      <c r="O33" s="81"/>
-      <c r="P33" s="82"/>
-      <c r="Q33" s="89"/>
-      <c r="R33" s="90"/>
-      <c r="S33" s="90"/>
-      <c r="T33" s="90"/>
-      <c r="U33" s="90"/>
-      <c r="V33" s="90"/>
-      <c r="W33" s="90"/>
-      <c r="X33" s="90"/>
-      <c r="Y33" s="90"/>
-      <c r="Z33" s="90"/>
-      <c r="AA33" s="90"/>
-      <c r="AB33" s="90"/>
-      <c r="AC33" s="90"/>
-      <c r="AD33" s="90"/>
-      <c r="AE33" s="91"/>
-      <c r="AF33" s="80"/>
-      <c r="AG33" s="81"/>
-      <c r="AH33" s="81"/>
-      <c r="AI33" s="82"/>
+      <c r="AG8" s="103"/>
+      <c r="AH8" s="103"/>
+      <c r="AI8" s="104"/>
+    </row>
+    <row r="9" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="75"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="133"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="135"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="136"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="137"/>
+      <c r="K9" s="138"/>
+      <c r="L9" s="138"/>
+      <c r="M9" s="138"/>
+      <c r="N9" s="138"/>
+      <c r="O9" s="138"/>
+      <c r="P9" s="139"/>
+      <c r="Q9" s="140"/>
+      <c r="R9" s="141"/>
+      <c r="S9" s="141"/>
+      <c r="T9" s="141"/>
+      <c r="U9" s="141"/>
+      <c r="V9" s="141"/>
+      <c r="W9" s="141"/>
+      <c r="X9" s="141"/>
+      <c r="Y9" s="141"/>
+      <c r="Z9" s="141"/>
+      <c r="AA9" s="141"/>
+      <c r="AB9" s="141"/>
+      <c r="AC9" s="141"/>
+      <c r="AD9" s="141"/>
+      <c r="AE9" s="142"/>
+      <c r="AF9" s="137"/>
+      <c r="AG9" s="138"/>
+      <c r="AH9" s="138"/>
+      <c r="AI9" s="139"/>
+    </row>
+    <row r="10" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="75"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="134"/>
+      <c r="F10" s="135"/>
+      <c r="G10" s="131"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="137"/>
+      <c r="K10" s="138"/>
+      <c r="L10" s="138"/>
+      <c r="M10" s="138"/>
+      <c r="N10" s="138"/>
+      <c r="O10" s="138"/>
+      <c r="P10" s="139"/>
+      <c r="Q10" s="140"/>
+      <c r="R10" s="141"/>
+      <c r="S10" s="141"/>
+      <c r="T10" s="141"/>
+      <c r="U10" s="141"/>
+      <c r="V10" s="141"/>
+      <c r="W10" s="141"/>
+      <c r="X10" s="141"/>
+      <c r="Y10" s="141"/>
+      <c r="Z10" s="141"/>
+      <c r="AA10" s="141"/>
+      <c r="AB10" s="141"/>
+      <c r="AC10" s="141"/>
+      <c r="AD10" s="141"/>
+      <c r="AE10" s="142"/>
+      <c r="AF10" s="137"/>
+      <c r="AG10" s="138"/>
+      <c r="AH10" s="138"/>
+      <c r="AI10" s="139"/>
+    </row>
+    <row r="11" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="75"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="134"/>
+      <c r="F11" s="135"/>
+      <c r="G11" s="131"/>
+      <c r="H11" s="136"/>
+      <c r="I11" s="132"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="138"/>
+      <c r="L11" s="138"/>
+      <c r="M11" s="138"/>
+      <c r="N11" s="138"/>
+      <c r="O11" s="138"/>
+      <c r="P11" s="139"/>
+      <c r="Q11" s="140"/>
+      <c r="R11" s="141"/>
+      <c r="S11" s="141"/>
+      <c r="T11" s="141"/>
+      <c r="U11" s="141"/>
+      <c r="V11" s="141"/>
+      <c r="W11" s="141"/>
+      <c r="X11" s="141"/>
+      <c r="Y11" s="141"/>
+      <c r="Z11" s="141"/>
+      <c r="AA11" s="141"/>
+      <c r="AB11" s="141"/>
+      <c r="AC11" s="141"/>
+      <c r="AD11" s="141"/>
+      <c r="AE11" s="142"/>
+      <c r="AF11" s="137"/>
+      <c r="AG11" s="138"/>
+      <c r="AH11" s="138"/>
+      <c r="AI11" s="139"/>
+    </row>
+    <row r="12" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="75"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="132"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="135"/>
+      <c r="G12" s="131"/>
+      <c r="H12" s="136"/>
+      <c r="I12" s="132"/>
+      <c r="J12" s="137"/>
+      <c r="K12" s="138"/>
+      <c r="L12" s="138"/>
+      <c r="M12" s="138"/>
+      <c r="N12" s="138"/>
+      <c r="O12" s="138"/>
+      <c r="P12" s="139"/>
+      <c r="Q12" s="140"/>
+      <c r="R12" s="141"/>
+      <c r="S12" s="141"/>
+      <c r="T12" s="141"/>
+      <c r="U12" s="141"/>
+      <c r="V12" s="141"/>
+      <c r="W12" s="141"/>
+      <c r="X12" s="141"/>
+      <c r="Y12" s="141"/>
+      <c r="Z12" s="141"/>
+      <c r="AA12" s="141"/>
+      <c r="AB12" s="141"/>
+      <c r="AC12" s="141"/>
+      <c r="AD12" s="141"/>
+      <c r="AE12" s="142"/>
+      <c r="AF12" s="137"/>
+      <c r="AG12" s="138"/>
+      <c r="AH12" s="138"/>
+      <c r="AI12" s="139"/>
+    </row>
+    <row r="13" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="75"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="133"/>
+      <c r="E13" s="134"/>
+      <c r="F13" s="135"/>
+      <c r="G13" s="131"/>
+      <c r="H13" s="136"/>
+      <c r="I13" s="132"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="138"/>
+      <c r="L13" s="138"/>
+      <c r="M13" s="138"/>
+      <c r="N13" s="138"/>
+      <c r="O13" s="138"/>
+      <c r="P13" s="139"/>
+      <c r="Q13" s="140"/>
+      <c r="R13" s="141"/>
+      <c r="S13" s="141"/>
+      <c r="T13" s="141"/>
+      <c r="U13" s="141"/>
+      <c r="V13" s="141"/>
+      <c r="W13" s="141"/>
+      <c r="X13" s="141"/>
+      <c r="Y13" s="141"/>
+      <c r="Z13" s="141"/>
+      <c r="AA13" s="141"/>
+      <c r="AB13" s="141"/>
+      <c r="AC13" s="141"/>
+      <c r="AD13" s="141"/>
+      <c r="AE13" s="142"/>
+      <c r="AF13" s="137"/>
+      <c r="AG13" s="138"/>
+      <c r="AH13" s="138"/>
+      <c r="AI13" s="139"/>
+    </row>
+    <row r="14" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="75"/>
+      <c r="B14" s="131"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="133"/>
+      <c r="E14" s="134"/>
+      <c r="F14" s="135"/>
+      <c r="G14" s="131"/>
+      <c r="H14" s="136"/>
+      <c r="I14" s="132"/>
+      <c r="J14" s="137"/>
+      <c r="K14" s="138"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="138"/>
+      <c r="N14" s="138"/>
+      <c r="O14" s="138"/>
+      <c r="P14" s="139"/>
+      <c r="Q14" s="140"/>
+      <c r="R14" s="141"/>
+      <c r="S14" s="141"/>
+      <c r="T14" s="141"/>
+      <c r="U14" s="141"/>
+      <c r="V14" s="141"/>
+      <c r="W14" s="141"/>
+      <c r="X14" s="141"/>
+      <c r="Y14" s="141"/>
+      <c r="Z14" s="141"/>
+      <c r="AA14" s="141"/>
+      <c r="AB14" s="141"/>
+      <c r="AC14" s="141"/>
+      <c r="AD14" s="141"/>
+      <c r="AE14" s="142"/>
+      <c r="AF14" s="137"/>
+      <c r="AG14" s="138"/>
+      <c r="AH14" s="138"/>
+      <c r="AI14" s="139"/>
+    </row>
+    <row r="15" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="75"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="132"/>
+      <c r="D15" s="133"/>
+      <c r="E15" s="134"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="131"/>
+      <c r="H15" s="136"/>
+      <c r="I15" s="132"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="138"/>
+      <c r="L15" s="138"/>
+      <c r="M15" s="138"/>
+      <c r="N15" s="138"/>
+      <c r="O15" s="138"/>
+      <c r="P15" s="139"/>
+      <c r="Q15" s="140"/>
+      <c r="R15" s="141"/>
+      <c r="S15" s="141"/>
+      <c r="T15" s="141"/>
+      <c r="U15" s="141"/>
+      <c r="V15" s="141"/>
+      <c r="W15" s="141"/>
+      <c r="X15" s="141"/>
+      <c r="Y15" s="141"/>
+      <c r="Z15" s="141"/>
+      <c r="AA15" s="141"/>
+      <c r="AB15" s="141"/>
+      <c r="AC15" s="141"/>
+      <c r="AD15" s="141"/>
+      <c r="AE15" s="142"/>
+      <c r="AF15" s="137"/>
+      <c r="AG15" s="138"/>
+      <c r="AH15" s="138"/>
+      <c r="AI15" s="139"/>
+    </row>
+    <row r="16" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="75"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="133"/>
+      <c r="E16" s="134"/>
+      <c r="F16" s="135"/>
+      <c r="G16" s="131"/>
+      <c r="H16" s="136"/>
+      <c r="I16" s="132"/>
+      <c r="J16" s="137"/>
+      <c r="K16" s="138"/>
+      <c r="L16" s="138"/>
+      <c r="M16" s="138"/>
+      <c r="N16" s="138"/>
+      <c r="O16" s="138"/>
+      <c r="P16" s="139"/>
+      <c r="Q16" s="140"/>
+      <c r="R16" s="141"/>
+      <c r="S16" s="141"/>
+      <c r="T16" s="141"/>
+      <c r="U16" s="141"/>
+      <c r="V16" s="141"/>
+      <c r="W16" s="141"/>
+      <c r="X16" s="141"/>
+      <c r="Y16" s="141"/>
+      <c r="Z16" s="141"/>
+      <c r="AA16" s="141"/>
+      <c r="AB16" s="141"/>
+      <c r="AC16" s="141"/>
+      <c r="AD16" s="141"/>
+      <c r="AE16" s="142"/>
+      <c r="AF16" s="137"/>
+      <c r="AG16" s="138"/>
+      <c r="AH16" s="138"/>
+      <c r="AI16" s="139"/>
+    </row>
+    <row r="17" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="75"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="134"/>
+      <c r="F17" s="135"/>
+      <c r="G17" s="131"/>
+      <c r="H17" s="136"/>
+      <c r="I17" s="132"/>
+      <c r="J17" s="137"/>
+      <c r="K17" s="138"/>
+      <c r="L17" s="138"/>
+      <c r="M17" s="138"/>
+      <c r="N17" s="138"/>
+      <c r="O17" s="138"/>
+      <c r="P17" s="139"/>
+      <c r="Q17" s="140"/>
+      <c r="R17" s="141"/>
+      <c r="S17" s="141"/>
+      <c r="T17" s="141"/>
+      <c r="U17" s="141"/>
+      <c r="V17" s="141"/>
+      <c r="W17" s="141"/>
+      <c r="X17" s="141"/>
+      <c r="Y17" s="141"/>
+      <c r="Z17" s="141"/>
+      <c r="AA17" s="141"/>
+      <c r="AB17" s="141"/>
+      <c r="AC17" s="141"/>
+      <c r="AD17" s="141"/>
+      <c r="AE17" s="142"/>
+      <c r="AF17" s="137"/>
+      <c r="AG17" s="138"/>
+      <c r="AH17" s="138"/>
+      <c r="AI17" s="139"/>
+    </row>
+    <row r="18" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="75"/>
+      <c r="B18" s="131"/>
+      <c r="C18" s="132"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="134"/>
+      <c r="F18" s="135"/>
+      <c r="G18" s="131"/>
+      <c r="H18" s="136"/>
+      <c r="I18" s="132"/>
+      <c r="J18" s="137"/>
+      <c r="K18" s="138"/>
+      <c r="L18" s="138"/>
+      <c r="M18" s="138"/>
+      <c r="N18" s="138"/>
+      <c r="O18" s="138"/>
+      <c r="P18" s="139"/>
+      <c r="Q18" s="140"/>
+      <c r="R18" s="141"/>
+      <c r="S18" s="141"/>
+      <c r="T18" s="141"/>
+      <c r="U18" s="141"/>
+      <c r="V18" s="141"/>
+      <c r="W18" s="141"/>
+      <c r="X18" s="141"/>
+      <c r="Y18" s="141"/>
+      <c r="Z18" s="141"/>
+      <c r="AA18" s="141"/>
+      <c r="AB18" s="141"/>
+      <c r="AC18" s="141"/>
+      <c r="AD18" s="141"/>
+      <c r="AE18" s="142"/>
+      <c r="AF18" s="137"/>
+      <c r="AG18" s="138"/>
+      <c r="AH18" s="138"/>
+      <c r="AI18" s="139"/>
+    </row>
+    <row r="19" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="75"/>
+      <c r="B19" s="131"/>
+      <c r="C19" s="132"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="135"/>
+      <c r="G19" s="131"/>
+      <c r="H19" s="136"/>
+      <c r="I19" s="132"/>
+      <c r="J19" s="137"/>
+      <c r="K19" s="138"/>
+      <c r="L19" s="138"/>
+      <c r="M19" s="138"/>
+      <c r="N19" s="138"/>
+      <c r="O19" s="138"/>
+      <c r="P19" s="139"/>
+      <c r="Q19" s="140"/>
+      <c r="R19" s="141"/>
+      <c r="S19" s="141"/>
+      <c r="T19" s="141"/>
+      <c r="U19" s="141"/>
+      <c r="V19" s="141"/>
+      <c r="W19" s="141"/>
+      <c r="X19" s="141"/>
+      <c r="Y19" s="141"/>
+      <c r="Z19" s="141"/>
+      <c r="AA19" s="141"/>
+      <c r="AB19" s="141"/>
+      <c r="AC19" s="141"/>
+      <c r="AD19" s="141"/>
+      <c r="AE19" s="142"/>
+      <c r="AF19" s="137"/>
+      <c r="AG19" s="138"/>
+      <c r="AH19" s="138"/>
+      <c r="AI19" s="139"/>
+    </row>
+    <row r="20" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="75"/>
+      <c r="B20" s="131"/>
+      <c r="C20" s="132"/>
+      <c r="D20" s="133"/>
+      <c r="E20" s="134"/>
+      <c r="F20" s="135"/>
+      <c r="G20" s="131"/>
+      <c r="H20" s="136"/>
+      <c r="I20" s="132"/>
+      <c r="J20" s="137"/>
+      <c r="K20" s="138"/>
+      <c r="L20" s="138"/>
+      <c r="M20" s="138"/>
+      <c r="N20" s="138"/>
+      <c r="O20" s="138"/>
+      <c r="P20" s="139"/>
+      <c r="Q20" s="140"/>
+      <c r="R20" s="141"/>
+      <c r="S20" s="141"/>
+      <c r="T20" s="141"/>
+      <c r="U20" s="141"/>
+      <c r="V20" s="141"/>
+      <c r="W20" s="141"/>
+      <c r="X20" s="141"/>
+      <c r="Y20" s="141"/>
+      <c r="Z20" s="141"/>
+      <c r="AA20" s="141"/>
+      <c r="AB20" s="141"/>
+      <c r="AC20" s="141"/>
+      <c r="AD20" s="141"/>
+      <c r="AE20" s="142"/>
+      <c r="AF20" s="137"/>
+      <c r="AG20" s="138"/>
+      <c r="AH20" s="138"/>
+      <c r="AI20" s="139"/>
+    </row>
+    <row r="21" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="75"/>
+      <c r="B21" s="131"/>
+      <c r="C21" s="132"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="134"/>
+      <c r="F21" s="135"/>
+      <c r="G21" s="131"/>
+      <c r="H21" s="136"/>
+      <c r="I21" s="132"/>
+      <c r="J21" s="137"/>
+      <c r="K21" s="138"/>
+      <c r="L21" s="138"/>
+      <c r="M21" s="138"/>
+      <c r="N21" s="138"/>
+      <c r="O21" s="138"/>
+      <c r="P21" s="139"/>
+      <c r="Q21" s="140"/>
+      <c r="R21" s="141"/>
+      <c r="S21" s="141"/>
+      <c r="T21" s="141"/>
+      <c r="U21" s="141"/>
+      <c r="V21" s="141"/>
+      <c r="W21" s="141"/>
+      <c r="X21" s="141"/>
+      <c r="Y21" s="141"/>
+      <c r="Z21" s="141"/>
+      <c r="AA21" s="141"/>
+      <c r="AB21" s="141"/>
+      <c r="AC21" s="141"/>
+      <c r="AD21" s="141"/>
+      <c r="AE21" s="142"/>
+      <c r="AF21" s="137"/>
+      <c r="AG21" s="138"/>
+      <c r="AH21" s="138"/>
+      <c r="AI21" s="139"/>
+    </row>
+    <row r="22" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="75"/>
+      <c r="B22" s="131"/>
+      <c r="C22" s="132"/>
+      <c r="D22" s="133"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="135"/>
+      <c r="G22" s="131"/>
+      <c r="H22" s="136"/>
+      <c r="I22" s="132"/>
+      <c r="J22" s="137"/>
+      <c r="K22" s="138"/>
+      <c r="L22" s="138"/>
+      <c r="M22" s="138"/>
+      <c r="N22" s="138"/>
+      <c r="O22" s="138"/>
+      <c r="P22" s="139"/>
+      <c r="Q22" s="140"/>
+      <c r="R22" s="141"/>
+      <c r="S22" s="141"/>
+      <c r="T22" s="141"/>
+      <c r="U22" s="141"/>
+      <c r="V22" s="141"/>
+      <c r="W22" s="141"/>
+      <c r="X22" s="141"/>
+      <c r="Y22" s="141"/>
+      <c r="Z22" s="141"/>
+      <c r="AA22" s="141"/>
+      <c r="AB22" s="141"/>
+      <c r="AC22" s="141"/>
+      <c r="AD22" s="141"/>
+      <c r="AE22" s="142"/>
+      <c r="AF22" s="137"/>
+      <c r="AG22" s="138"/>
+      <c r="AH22" s="138"/>
+      <c r="AI22" s="139"/>
+    </row>
+    <row r="23" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="75"/>
+      <c r="B23" s="131"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="133"/>
+      <c r="E23" s="134"/>
+      <c r="F23" s="135"/>
+      <c r="G23" s="131"/>
+      <c r="H23" s="136"/>
+      <c r="I23" s="132"/>
+      <c r="J23" s="137"/>
+      <c r="K23" s="138"/>
+      <c r="L23" s="138"/>
+      <c r="M23" s="138"/>
+      <c r="N23" s="138"/>
+      <c r="O23" s="138"/>
+      <c r="P23" s="139"/>
+      <c r="Q23" s="140"/>
+      <c r="R23" s="141"/>
+      <c r="S23" s="141"/>
+      <c r="T23" s="141"/>
+      <c r="U23" s="141"/>
+      <c r="V23" s="141"/>
+      <c r="W23" s="141"/>
+      <c r="X23" s="141"/>
+      <c r="Y23" s="141"/>
+      <c r="Z23" s="141"/>
+      <c r="AA23" s="141"/>
+      <c r="AB23" s="141"/>
+      <c r="AC23" s="141"/>
+      <c r="AD23" s="141"/>
+      <c r="AE23" s="142"/>
+      <c r="AF23" s="137"/>
+      <c r="AG23" s="138"/>
+      <c r="AH23" s="138"/>
+      <c r="AI23" s="139"/>
+    </row>
+    <row r="24" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="75"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="131"/>
+      <c r="H24" s="136"/>
+      <c r="I24" s="132"/>
+      <c r="J24" s="137"/>
+      <c r="K24" s="138"/>
+      <c r="L24" s="138"/>
+      <c r="M24" s="138"/>
+      <c r="N24" s="138"/>
+      <c r="O24" s="138"/>
+      <c r="P24" s="139"/>
+      <c r="Q24" s="140"/>
+      <c r="R24" s="141"/>
+      <c r="S24" s="141"/>
+      <c r="T24" s="141"/>
+      <c r="U24" s="141"/>
+      <c r="V24" s="141"/>
+      <c r="W24" s="141"/>
+      <c r="X24" s="141"/>
+      <c r="Y24" s="141"/>
+      <c r="Z24" s="141"/>
+      <c r="AA24" s="141"/>
+      <c r="AB24" s="141"/>
+      <c r="AC24" s="141"/>
+      <c r="AD24" s="141"/>
+      <c r="AE24" s="142"/>
+      <c r="AF24" s="137"/>
+      <c r="AG24" s="138"/>
+      <c r="AH24" s="138"/>
+      <c r="AI24" s="139"/>
+    </row>
+    <row r="25" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="75"/>
+      <c r="B25" s="131"/>
+      <c r="C25" s="132"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="135"/>
+      <c r="G25" s="131"/>
+      <c r="H25" s="136"/>
+      <c r="I25" s="132"/>
+      <c r="J25" s="137"/>
+      <c r="K25" s="138"/>
+      <c r="L25" s="138"/>
+      <c r="M25" s="138"/>
+      <c r="N25" s="138"/>
+      <c r="O25" s="138"/>
+      <c r="P25" s="139"/>
+      <c r="Q25" s="140"/>
+      <c r="R25" s="141"/>
+      <c r="S25" s="141"/>
+      <c r="T25" s="141"/>
+      <c r="U25" s="141"/>
+      <c r="V25" s="141"/>
+      <c r="W25" s="141"/>
+      <c r="X25" s="141"/>
+      <c r="Y25" s="141"/>
+      <c r="Z25" s="141"/>
+      <c r="AA25" s="141"/>
+      <c r="AB25" s="141"/>
+      <c r="AC25" s="141"/>
+      <c r="AD25" s="141"/>
+      <c r="AE25" s="142"/>
+      <c r="AF25" s="137"/>
+      <c r="AG25" s="138"/>
+      <c r="AH25" s="138"/>
+      <c r="AI25" s="139"/>
+    </row>
+    <row r="26" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="75"/>
+      <c r="B26" s="131"/>
+      <c r="C26" s="132"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="134"/>
+      <c r="F26" s="135"/>
+      <c r="G26" s="131"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="132"/>
+      <c r="J26" s="137"/>
+      <c r="K26" s="138"/>
+      <c r="L26" s="138"/>
+      <c r="M26" s="138"/>
+      <c r="N26" s="138"/>
+      <c r="O26" s="138"/>
+      <c r="P26" s="139"/>
+      <c r="Q26" s="140"/>
+      <c r="R26" s="141"/>
+      <c r="S26" s="141"/>
+      <c r="T26" s="141"/>
+      <c r="U26" s="141"/>
+      <c r="V26" s="141"/>
+      <c r="W26" s="141"/>
+      <c r="X26" s="141"/>
+      <c r="Y26" s="141"/>
+      <c r="Z26" s="141"/>
+      <c r="AA26" s="141"/>
+      <c r="AB26" s="141"/>
+      <c r="AC26" s="141"/>
+      <c r="AD26" s="141"/>
+      <c r="AE26" s="142"/>
+      <c r="AF26" s="137"/>
+      <c r="AG26" s="138"/>
+      <c r="AH26" s="138"/>
+      <c r="AI26" s="139"/>
+    </row>
+    <row r="27" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="75"/>
+      <c r="B27" s="131"/>
+      <c r="C27" s="132"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="134"/>
+      <c r="F27" s="135"/>
+      <c r="G27" s="131"/>
+      <c r="H27" s="136"/>
+      <c r="I27" s="132"/>
+      <c r="J27" s="137"/>
+      <c r="K27" s="138"/>
+      <c r="L27" s="138"/>
+      <c r="M27" s="138"/>
+      <c r="N27" s="138"/>
+      <c r="O27" s="138"/>
+      <c r="P27" s="139"/>
+      <c r="Q27" s="140"/>
+      <c r="R27" s="141"/>
+      <c r="S27" s="141"/>
+      <c r="T27" s="141"/>
+      <c r="U27" s="141"/>
+      <c r="V27" s="141"/>
+      <c r="W27" s="141"/>
+      <c r="X27" s="141"/>
+      <c r="Y27" s="141"/>
+      <c r="Z27" s="141"/>
+      <c r="AA27" s="141"/>
+      <c r="AB27" s="141"/>
+      <c r="AC27" s="141"/>
+      <c r="AD27" s="141"/>
+      <c r="AE27" s="142"/>
+      <c r="AF27" s="137"/>
+      <c r="AG27" s="138"/>
+      <c r="AH27" s="138"/>
+      <c r="AI27" s="139"/>
+    </row>
+    <row r="28" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="75"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="132"/>
+      <c r="D28" s="133"/>
+      <c r="E28" s="134"/>
+      <c r="F28" s="135"/>
+      <c r="G28" s="131"/>
+      <c r="H28" s="136"/>
+      <c r="I28" s="132"/>
+      <c r="J28" s="137"/>
+      <c r="K28" s="138"/>
+      <c r="L28" s="138"/>
+      <c r="M28" s="138"/>
+      <c r="N28" s="138"/>
+      <c r="O28" s="138"/>
+      <c r="P28" s="139"/>
+      <c r="Q28" s="140"/>
+      <c r="R28" s="141"/>
+      <c r="S28" s="141"/>
+      <c r="T28" s="141"/>
+      <c r="U28" s="141"/>
+      <c r="V28" s="141"/>
+      <c r="W28" s="141"/>
+      <c r="X28" s="141"/>
+      <c r="Y28" s="141"/>
+      <c r="Z28" s="141"/>
+      <c r="AA28" s="141"/>
+      <c r="AB28" s="141"/>
+      <c r="AC28" s="141"/>
+      <c r="AD28" s="141"/>
+      <c r="AE28" s="142"/>
+      <c r="AF28" s="137"/>
+      <c r="AG28" s="138"/>
+      <c r="AH28" s="138"/>
+      <c r="AI28" s="139"/>
+    </row>
+    <row r="29" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="75"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="133"/>
+      <c r="E29" s="134"/>
+      <c r="F29" s="135"/>
+      <c r="G29" s="131"/>
+      <c r="H29" s="136"/>
+      <c r="I29" s="132"/>
+      <c r="J29" s="137"/>
+      <c r="K29" s="138"/>
+      <c r="L29" s="138"/>
+      <c r="M29" s="138"/>
+      <c r="N29" s="138"/>
+      <c r="O29" s="138"/>
+      <c r="P29" s="139"/>
+      <c r="Q29" s="140"/>
+      <c r="R29" s="141"/>
+      <c r="S29" s="141"/>
+      <c r="T29" s="141"/>
+      <c r="U29" s="141"/>
+      <c r="V29" s="141"/>
+      <c r="W29" s="141"/>
+      <c r="X29" s="141"/>
+      <c r="Y29" s="141"/>
+      <c r="Z29" s="141"/>
+      <c r="AA29" s="141"/>
+      <c r="AB29" s="141"/>
+      <c r="AC29" s="141"/>
+      <c r="AD29" s="141"/>
+      <c r="AE29" s="142"/>
+      <c r="AF29" s="137"/>
+      <c r="AG29" s="138"/>
+      <c r="AH29" s="138"/>
+      <c r="AI29" s="139"/>
+    </row>
+    <row r="30" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="75"/>
+      <c r="B30" s="131"/>
+      <c r="C30" s="132"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="134"/>
+      <c r="F30" s="135"/>
+      <c r="G30" s="131"/>
+      <c r="H30" s="136"/>
+      <c r="I30" s="132"/>
+      <c r="J30" s="137"/>
+      <c r="K30" s="138"/>
+      <c r="L30" s="138"/>
+      <c r="M30" s="138"/>
+      <c r="N30" s="138"/>
+      <c r="O30" s="138"/>
+      <c r="P30" s="139"/>
+      <c r="Q30" s="140"/>
+      <c r="R30" s="141"/>
+      <c r="S30" s="141"/>
+      <c r="T30" s="141"/>
+      <c r="U30" s="141"/>
+      <c r="V30" s="141"/>
+      <c r="W30" s="141"/>
+      <c r="X30" s="141"/>
+      <c r="Y30" s="141"/>
+      <c r="Z30" s="141"/>
+      <c r="AA30" s="141"/>
+      <c r="AB30" s="141"/>
+      <c r="AC30" s="141"/>
+      <c r="AD30" s="141"/>
+      <c r="AE30" s="142"/>
+      <c r="AF30" s="137"/>
+      <c r="AG30" s="138"/>
+      <c r="AH30" s="138"/>
+      <c r="AI30" s="139"/>
+    </row>
+    <row r="31" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="75"/>
+      <c r="B31" s="131"/>
+      <c r="C31" s="132"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="134"/>
+      <c r="F31" s="135"/>
+      <c r="G31" s="131"/>
+      <c r="H31" s="136"/>
+      <c r="I31" s="132"/>
+      <c r="J31" s="137"/>
+      <c r="K31" s="138"/>
+      <c r="L31" s="138"/>
+      <c r="M31" s="138"/>
+      <c r="N31" s="138"/>
+      <c r="O31" s="138"/>
+      <c r="P31" s="139"/>
+      <c r="Q31" s="140"/>
+      <c r="R31" s="141"/>
+      <c r="S31" s="141"/>
+      <c r="T31" s="141"/>
+      <c r="U31" s="141"/>
+      <c r="V31" s="141"/>
+      <c r="W31" s="141"/>
+      <c r="X31" s="141"/>
+      <c r="Y31" s="141"/>
+      <c r="Z31" s="141"/>
+      <c r="AA31" s="141"/>
+      <c r="AB31" s="141"/>
+      <c r="AC31" s="141"/>
+      <c r="AD31" s="141"/>
+      <c r="AE31" s="142"/>
+      <c r="AF31" s="137"/>
+      <c r="AG31" s="138"/>
+      <c r="AH31" s="138"/>
+      <c r="AI31" s="139"/>
+    </row>
+    <row r="32" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="75"/>
+      <c r="B32" s="131"/>
+      <c r="C32" s="132"/>
+      <c r="D32" s="133"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="135"/>
+      <c r="G32" s="131"/>
+      <c r="H32" s="136"/>
+      <c r="I32" s="132"/>
+      <c r="J32" s="137"/>
+      <c r="K32" s="143"/>
+      <c r="L32" s="138"/>
+      <c r="M32" s="138"/>
+      <c r="N32" s="138"/>
+      <c r="O32" s="138"/>
+      <c r="P32" s="139"/>
+      <c r="Q32" s="140"/>
+      <c r="R32" s="141"/>
+      <c r="S32" s="141"/>
+      <c r="T32" s="141"/>
+      <c r="U32" s="141"/>
+      <c r="V32" s="141"/>
+      <c r="W32" s="141"/>
+      <c r="X32" s="141"/>
+      <c r="Y32" s="141"/>
+      <c r="Z32" s="141"/>
+      <c r="AA32" s="141"/>
+      <c r="AB32" s="141"/>
+      <c r="AC32" s="141"/>
+      <c r="AD32" s="141"/>
+      <c r="AE32" s="142"/>
+      <c r="AF32" s="137"/>
+      <c r="AG32" s="138"/>
+      <c r="AH32" s="138"/>
+      <c r="AI32" s="139"/>
+    </row>
+    <row r="33" spans="1:35" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="75"/>
+      <c r="B33" s="131"/>
+      <c r="C33" s="132"/>
+      <c r="D33" s="133"/>
+      <c r="E33" s="134"/>
+      <c r="F33" s="135"/>
+      <c r="G33" s="131"/>
+      <c r="H33" s="136"/>
+      <c r="I33" s="132"/>
+      <c r="J33" s="137"/>
+      <c r="K33" s="138"/>
+      <c r="L33" s="138"/>
+      <c r="M33" s="138"/>
+      <c r="N33" s="138"/>
+      <c r="O33" s="138"/>
+      <c r="P33" s="139"/>
+      <c r="Q33" s="140"/>
+      <c r="R33" s="141"/>
+      <c r="S33" s="141"/>
+      <c r="T33" s="141"/>
+      <c r="U33" s="141"/>
+      <c r="V33" s="141"/>
+      <c r="W33" s="141"/>
+      <c r="X33" s="141"/>
+      <c r="Y33" s="141"/>
+      <c r="Z33" s="141"/>
+      <c r="AA33" s="141"/>
+      <c r="AB33" s="141"/>
+      <c r="AC33" s="141"/>
+      <c r="AD33" s="141"/>
+      <c r="AE33" s="142"/>
+      <c r="AF33" s="137"/>
+      <c r="AG33" s="138"/>
+      <c r="AH33" s="138"/>
+      <c r="AI33" s="139"/>
     </row>
     <row r="34" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="K34" s="170"/>
+      <c r="K34" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="179">
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:P33"/>
+    <mergeCell ref="Q33:AE33"/>
+    <mergeCell ref="AF33:AI33"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:P32"/>
+    <mergeCell ref="Q32:AE32"/>
+    <mergeCell ref="AF32:AI32"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="Q31:AE31"/>
+    <mergeCell ref="AF31:AI31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:P30"/>
+    <mergeCell ref="Q30:AE30"/>
+    <mergeCell ref="AF30:AI30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:P29"/>
+    <mergeCell ref="Q29:AE29"/>
+    <mergeCell ref="AF29:AI29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:P28"/>
+    <mergeCell ref="Q28:AE28"/>
+    <mergeCell ref="AF28:AI28"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:P27"/>
+    <mergeCell ref="Q27:AE27"/>
+    <mergeCell ref="AF27:AI27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:P26"/>
+    <mergeCell ref="Q26:AE26"/>
+    <mergeCell ref="AF26:AI26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:P25"/>
+    <mergeCell ref="Q25:AE25"/>
+    <mergeCell ref="AF25:AI25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:P24"/>
+    <mergeCell ref="Q24:AE24"/>
+    <mergeCell ref="AF24:AI24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:P23"/>
+    <mergeCell ref="Q23:AE23"/>
+    <mergeCell ref="AF23:AI23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:P22"/>
+    <mergeCell ref="Q22:AE22"/>
+    <mergeCell ref="AF22:AI22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="Q21:AE21"/>
+    <mergeCell ref="AF21:AI21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:P20"/>
+    <mergeCell ref="Q20:AE20"/>
+    <mergeCell ref="AF20:AI20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:P19"/>
+    <mergeCell ref="Q19:AE19"/>
+    <mergeCell ref="AF19:AI19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:P18"/>
+    <mergeCell ref="Q18:AE18"/>
+    <mergeCell ref="AF18:AI18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:P17"/>
+    <mergeCell ref="Q17:AE17"/>
+    <mergeCell ref="AF17:AI17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:P16"/>
+    <mergeCell ref="Q16:AE16"/>
+    <mergeCell ref="AF16:AI16"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:P15"/>
+    <mergeCell ref="Q15:AE15"/>
+    <mergeCell ref="AF15:AI15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:P14"/>
+    <mergeCell ref="Q14:AE14"/>
+    <mergeCell ref="AF14:AI14"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:P13"/>
+    <mergeCell ref="Q13:AE13"/>
+    <mergeCell ref="AF13:AI13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:P12"/>
+    <mergeCell ref="Q12:AE12"/>
+    <mergeCell ref="AF12:AI12"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:P7"/>
+    <mergeCell ref="Q7:AE7"/>
+    <mergeCell ref="AF7:AI7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="Q11:AE11"/>
+    <mergeCell ref="AF11:AI11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:P10"/>
+    <mergeCell ref="Q10:AE10"/>
+    <mergeCell ref="AF10:AI10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:P9"/>
+    <mergeCell ref="Q9:AE9"/>
+    <mergeCell ref="AF9:AI9"/>
     <mergeCell ref="S1:Z3"/>
     <mergeCell ref="AG3:AI3"/>
     <mergeCell ref="B8:C8"/>
@@ -4313,161 +4469,6 @@
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AC3:AF3"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:P7"/>
-    <mergeCell ref="Q7:AE7"/>
-    <mergeCell ref="AF7:AI7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:P11"/>
-    <mergeCell ref="Q11:AE11"/>
-    <mergeCell ref="AF11:AI11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="J10:P10"/>
-    <mergeCell ref="Q10:AE10"/>
-    <mergeCell ref="AF10:AI10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:P9"/>
-    <mergeCell ref="Q9:AE9"/>
-    <mergeCell ref="AF9:AI9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:P13"/>
-    <mergeCell ref="Q13:AE13"/>
-    <mergeCell ref="AF13:AI13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:P12"/>
-    <mergeCell ref="Q12:AE12"/>
-    <mergeCell ref="AF12:AI12"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:P15"/>
-    <mergeCell ref="Q15:AE15"/>
-    <mergeCell ref="AF15:AI15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:P14"/>
-    <mergeCell ref="Q14:AE14"/>
-    <mergeCell ref="AF14:AI14"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:P17"/>
-    <mergeCell ref="Q17:AE17"/>
-    <mergeCell ref="AF17:AI17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:P16"/>
-    <mergeCell ref="Q16:AE16"/>
-    <mergeCell ref="AF16:AI16"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:P19"/>
-    <mergeCell ref="Q19:AE19"/>
-    <mergeCell ref="AF19:AI19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:P18"/>
-    <mergeCell ref="Q18:AE18"/>
-    <mergeCell ref="AF18:AI18"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="Q21:AE21"/>
-    <mergeCell ref="AF21:AI21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:P20"/>
-    <mergeCell ref="Q20:AE20"/>
-    <mergeCell ref="AF20:AI20"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:P23"/>
-    <mergeCell ref="Q23:AE23"/>
-    <mergeCell ref="AF23:AI23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:P22"/>
-    <mergeCell ref="Q22:AE22"/>
-    <mergeCell ref="AF22:AI22"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:P25"/>
-    <mergeCell ref="Q25:AE25"/>
-    <mergeCell ref="AF25:AI25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:P24"/>
-    <mergeCell ref="Q24:AE24"/>
-    <mergeCell ref="AF24:AI24"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:P27"/>
-    <mergeCell ref="Q27:AE27"/>
-    <mergeCell ref="AF27:AI27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:P26"/>
-    <mergeCell ref="Q26:AE26"/>
-    <mergeCell ref="AF26:AI26"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:P29"/>
-    <mergeCell ref="Q29:AE29"/>
-    <mergeCell ref="AF29:AI29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:P28"/>
-    <mergeCell ref="Q28:AE28"/>
-    <mergeCell ref="AF28:AI28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="Q31:AE31"/>
-    <mergeCell ref="AF31:AI31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:P30"/>
-    <mergeCell ref="Q30:AE30"/>
-    <mergeCell ref="AF30:AI30"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:P33"/>
-    <mergeCell ref="Q33:AE33"/>
-    <mergeCell ref="AF33:AI33"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:P32"/>
-    <mergeCell ref="Q32:AE32"/>
-    <mergeCell ref="AF32:AI32"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <printOptions horizontalCentered="1"/>
@@ -4623,163 +4624,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="171" t="str">
+      <c r="A1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A1")&lt;&gt;"",INDIRECT("'Revision history'!A1"),"")</f>
         <v>Project name</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="71" t="str">
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="108" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E1")&lt;&gt;"",INDIRECT("'Revision history'!E1"),"")</f>
         <v>Sample Project</v>
       </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="174" t="str">
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="153" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!O1")&lt;&gt;"",INDIRECT("'Revision history'!O1"),"")</f>
         <v>Deliverable name</v>
       </c>
-      <c r="P1" s="175"/>
-      <c r="Q1" s="175"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="113" t="str">
+      <c r="P1" s="154"/>
+      <c r="Q1" s="154"/>
+      <c r="R1" s="155"/>
+      <c r="S1" s="79" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!S1")&lt;&gt;"",INDIRECT("'Revision history'!S1"),"")</f>
         <v>Web Service API List</v>
       </c>
-      <c r="T1" s="114"/>
-      <c r="U1" s="114"/>
-      <c r="V1" s="114"/>
-      <c r="W1" s="114"/>
-      <c r="X1" s="114"/>
-      <c r="Y1" s="114"/>
-      <c r="Z1" s="115"/>
-      <c r="AA1" s="171" t="str">
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA1")&lt;&gt;"",INDIRECT("'Revision history'!AA1"),"")</f>
         <v>Prepared by</v>
       </c>
-      <c r="AB1" s="173"/>
-      <c r="AC1" s="177" t="str">
+      <c r="AB1" s="145"/>
+      <c r="AC1" s="146" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC1")&lt;&gt;"",INDIRECT("'Revision history'!AC1"),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD1" s="178"/>
-      <c r="AE1" s="178"/>
-      <c r="AF1" s="179"/>
-      <c r="AG1" s="77">
+      <c r="AD1" s="147"/>
+      <c r="AE1" s="147"/>
+      <c r="AF1" s="148"/>
+      <c r="AG1" s="149">
         <f ca="1">IF(INDIRECT("'Revision history'!AG1")&lt;&gt;"",INDIRECT("'Revision history'!AG1"),"")</f>
         <v>43404</v>
       </c>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="79"/>
+      <c r="AH1" s="150"/>
+      <c r="AI1" s="151"/>
     </row>
     <row r="2" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="171" t="str">
+      <c r="A2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A2")&lt;&gt;"",INDIRECT("'Revision history'!A2"),"")</f>
         <v>System name</v>
       </c>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="71" t="str">
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="108" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E2")&lt;&gt;"",INDIRECT("'Revision history'!E2"),"")</f>
         <v>Sample System</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="180"/>
-      <c r="P2" s="181"/>
-      <c r="Q2" s="181"/>
-      <c r="R2" s="182"/>
-      <c r="S2" s="119"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="120"/>
-      <c r="X2" s="120"/>
-      <c r="Y2" s="120"/>
-      <c r="Z2" s="121"/>
-      <c r="AA2" s="171" t="str">
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="156"/>
+      <c r="P2" s="157"/>
+      <c r="Q2" s="157"/>
+      <c r="R2" s="158"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA2")&lt;&gt;"",INDIRECT("'Revision history'!AA2"),"")</f>
         <v>Changes</v>
       </c>
-      <c r="AB2" s="173"/>
-      <c r="AC2" s="177" t="str">
+      <c r="AB2" s="145"/>
+      <c r="AC2" s="146" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC2")&lt;&gt;"",INDIRECT("'Revision history'!AC2"),"")</f>
         <v/>
       </c>
-      <c r="AD2" s="178"/>
-      <c r="AE2" s="178"/>
-      <c r="AF2" s="179"/>
-      <c r="AG2" s="77" t="str">
+      <c r="AD2" s="147"/>
+      <c r="AE2" s="147"/>
+      <c r="AF2" s="148"/>
+      <c r="AG2" s="149" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG2")&lt;&gt;"",INDIRECT("'Revision history'!AG2"),"")</f>
         <v/>
       </c>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="79"/>
+      <c r="AH2" s="150"/>
+      <c r="AI2" s="151"/>
     </row>
     <row r="3" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="171" t="str">
+      <c r="A3" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A3")&lt;&gt;"",INDIRECT("'Revision history'!A3"),"")</f>
         <v>Sub-system name</v>
       </c>
-      <c r="B3" s="172"/>
-      <c r="C3" s="172"/>
-      <c r="D3" s="173"/>
-      <c r="E3" s="71" t="str">
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="145"/>
+      <c r="E3" s="108" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E3")&lt;&gt;"",INDIRECT("'Revision history'!E3"),"")</f>
         <v>Client Management System</v>
       </c>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="183"/>
-      <c r="P3" s="184"/>
-      <c r="Q3" s="184"/>
-      <c r="R3" s="185"/>
-      <c r="S3" s="125"/>
-      <c r="T3" s="126"/>
-      <c r="U3" s="126"/>
-      <c r="V3" s="126"/>
-      <c r="W3" s="126"/>
-      <c r="X3" s="126"/>
-      <c r="Y3" s="126"/>
-      <c r="Z3" s="127"/>
-      <c r="AA3" s="171"/>
-      <c r="AB3" s="173"/>
-      <c r="AC3" s="177" t="str">
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="110"/>
+      <c r="O3" s="159"/>
+      <c r="P3" s="160"/>
+      <c r="Q3" s="160"/>
+      <c r="R3" s="161"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="86"/>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="86"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="144"/>
+      <c r="AB3" s="145"/>
+      <c r="AC3" s="146" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC3")&lt;&gt;"",INDIRECT("'Revision history'!AC3"),"")</f>
         <v/>
       </c>
-      <c r="AD3" s="178"/>
-      <c r="AE3" s="178"/>
-      <c r="AF3" s="179"/>
-      <c r="AG3" s="77" t="str">
+      <c r="AD3" s="147"/>
+      <c r="AE3" s="147"/>
+      <c r="AF3" s="148"/>
+      <c r="AG3" s="149" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG3")&lt;&gt;"",INDIRECT("'Revision history'!AG3"),"")</f>
         <v/>
       </c>
-      <c r="AH3" s="78"/>
-      <c r="AI3" s="79"/>
+      <c r="AH3" s="150"/>
+      <c r="AI3" s="151"/>
     </row>
     <row r="4" spans="1:35" s="28" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26"/>
@@ -4836,7 +4837,7 @@
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R5" s="26"/>
       <c r="S5" s="26"/>
@@ -6241,6 +6242,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="S1:Z3"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:N1"/>
+    <mergeCell ref="O1:R3"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:N2"/>
+    <mergeCell ref="E3:N3"/>
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AC3:AF3"/>
     <mergeCell ref="AG3:AI3"/>
@@ -6250,14 +6259,6 @@
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="AC2:AF2"/>
     <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:N1"/>
-    <mergeCell ref="O1:R3"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:N2"/>
-    <mergeCell ref="E3:N3"/>
-    <mergeCell ref="S1:Z3"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <printOptions horizontalCentered="1"/>
@@ -6273,8 +6274,8 @@
   </sheetPr>
   <dimension ref="A1:BF27"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -6287,163 +6288,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" s="19" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="171" t="str">
+      <c r="A1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A1")&lt;&gt;"",INDIRECT("'Revision history'!A1"),"")</f>
         <v>Project name</v>
       </c>
-      <c r="B1" s="172"/>
-      <c r="C1" s="172"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="71" t="str">
+      <c r="B1" s="152"/>
+      <c r="C1" s="152"/>
+      <c r="D1" s="145"/>
+      <c r="E1" s="108" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E1")&lt;&gt;"",INDIRECT("'Revision history'!E1"),"")</f>
         <v>Sample Project</v>
       </c>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="174" t="str">
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="110"/>
+      <c r="O1" s="153" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!O1")&lt;&gt;"",INDIRECT("'Revision history'!O1"),"")</f>
         <v>Deliverable name</v>
       </c>
-      <c r="P1" s="175"/>
-      <c r="Q1" s="175"/>
-      <c r="R1" s="176"/>
-      <c r="S1" s="113" t="str">
+      <c r="P1" s="154"/>
+      <c r="Q1" s="154"/>
+      <c r="R1" s="155"/>
+      <c r="S1" s="79" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!S1")&lt;&gt;"",INDIRECT("'Revision history'!S1"),"")</f>
         <v>Web Service API List</v>
       </c>
-      <c r="T1" s="114"/>
-      <c r="U1" s="114"/>
-      <c r="V1" s="114"/>
-      <c r="W1" s="114"/>
-      <c r="X1" s="114"/>
-      <c r="Y1" s="114"/>
-      <c r="Z1" s="115"/>
-      <c r="AA1" s="171" t="str">
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA1")&lt;&gt;"",INDIRECT("'Revision history'!AA1"),"")</f>
         <v>Prepared by</v>
       </c>
-      <c r="AB1" s="173"/>
-      <c r="AC1" s="177" t="str">
+      <c r="AB1" s="145"/>
+      <c r="AC1" s="146" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC1")&lt;&gt;"",INDIRECT("'Revision history'!AC1"),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD1" s="178"/>
-      <c r="AE1" s="178"/>
-      <c r="AF1" s="179"/>
-      <c r="AG1" s="77">
+      <c r="AD1" s="147"/>
+      <c r="AE1" s="147"/>
+      <c r="AF1" s="148"/>
+      <c r="AG1" s="149">
         <f ca="1">IF(INDIRECT("'Revision history'!AG1")&lt;&gt;"",INDIRECT("'Revision history'!AG1"),"")</f>
         <v>43404</v>
       </c>
-      <c r="AH1" s="78"/>
-      <c r="AI1" s="79"/>
+      <c r="AH1" s="150"/>
+      <c r="AI1" s="151"/>
     </row>
     <row r="2" spans="1:58" s="19" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="171" t="str">
+      <c r="A2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A2")&lt;&gt;"",INDIRECT("'Revision history'!A2"),"")</f>
         <v>System name</v>
       </c>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="71" t="str">
+      <c r="B2" s="152"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="108" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E2")&lt;&gt;"",INDIRECT("'Revision history'!E2"),"")</f>
         <v>Sample System</v>
       </c>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="180"/>
-      <c r="P2" s="181"/>
-      <c r="Q2" s="181"/>
-      <c r="R2" s="182"/>
-      <c r="S2" s="119"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="120"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="120"/>
-      <c r="X2" s="120"/>
-      <c r="Y2" s="120"/>
-      <c r="Z2" s="121"/>
-      <c r="AA2" s="171" t="str">
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="110"/>
+      <c r="O2" s="156"/>
+      <c r="P2" s="157"/>
+      <c r="Q2" s="157"/>
+      <c r="R2" s="158"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA2")&lt;&gt;"",INDIRECT("'Revision history'!AA2"),"")</f>
         <v>Changes</v>
       </c>
-      <c r="AB2" s="173"/>
-      <c r="AC2" s="177" t="str">
+      <c r="AB2" s="145"/>
+      <c r="AC2" s="146" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC2")&lt;&gt;"",INDIRECT("'Revision history'!AC2"),"")</f>
         <v/>
       </c>
-      <c r="AD2" s="178"/>
-      <c r="AE2" s="178"/>
-      <c r="AF2" s="179"/>
-      <c r="AG2" s="77" t="str">
+      <c r="AD2" s="147"/>
+      <c r="AE2" s="147"/>
+      <c r="AF2" s="148"/>
+      <c r="AG2" s="149" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG2")&lt;&gt;"",INDIRECT("'Revision history'!AG2"),"")</f>
         <v/>
       </c>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="79"/>
+      <c r="AH2" s="150"/>
+      <c r="AI2" s="151"/>
     </row>
     <row r="3" spans="1:58" s="19" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="171" t="str">
+      <c r="A3" s="144" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A3")&lt;&gt;"",INDIRECT("'Revision history'!A3"),"")</f>
         <v>Sub-system name</v>
       </c>
-      <c r="B3" s="172"/>
-      <c r="C3" s="172"/>
-      <c r="D3" s="173"/>
-      <c r="E3" s="71" t="str">
+      <c r="B3" s="152"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="145"/>
+      <c r="E3" s="108" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E3")&lt;&gt;"",INDIRECT("'Revision history'!E3"),"")</f>
         <v>Client Management System</v>
       </c>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="183"/>
-      <c r="P3" s="184"/>
-      <c r="Q3" s="184"/>
-      <c r="R3" s="185"/>
-      <c r="S3" s="125"/>
-      <c r="T3" s="126"/>
-      <c r="U3" s="126"/>
-      <c r="V3" s="126"/>
-      <c r="W3" s="126"/>
-      <c r="X3" s="126"/>
-      <c r="Y3" s="126"/>
-      <c r="Z3" s="127"/>
-      <c r="AA3" s="171"/>
-      <c r="AB3" s="173"/>
-      <c r="AC3" s="177" t="str">
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="110"/>
+      <c r="O3" s="159"/>
+      <c r="P3" s="160"/>
+      <c r="Q3" s="160"/>
+      <c r="R3" s="161"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="86"/>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="86"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="144"/>
+      <c r="AB3" s="145"/>
+      <c r="AC3" s="146" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC3")&lt;&gt;"",INDIRECT("'Revision history'!AC3"),"")</f>
         <v/>
       </c>
-      <c r="AD3" s="178"/>
-      <c r="AE3" s="178"/>
-      <c r="AF3" s="179"/>
-      <c r="AG3" s="77" t="str">
+      <c r="AD3" s="147"/>
+      <c r="AE3" s="147"/>
+      <c r="AF3" s="148"/>
+      <c r="AG3" s="149" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG3")&lt;&gt;"",INDIRECT("'Revision history'!AG3"),"")</f>
         <v/>
       </c>
-      <c r="AH3" s="78"/>
-      <c r="AI3" s="79"/>
+      <c r="AH3" s="150"/>
+      <c r="AI3" s="151"/>
     </row>
     <row r="4" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="17"/>
@@ -6814,26 +6815,26 @@
     <row r="10" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
-      <c r="C10" s="92" t="s">
+      <c r="C10" s="165" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="93"/>
-      <c r="E10" s="93"/>
-      <c r="F10" s="93"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="80" t="s">
+      <c r="D10" s="166"/>
+      <c r="E10" s="166"/>
+      <c r="F10" s="166"/>
+      <c r="G10" s="167"/>
+      <c r="H10" s="137" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
-      <c r="N10" s="81"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="82"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="138"/>
+      <c r="K10" s="138"/>
+      <c r="L10" s="138"/>
+      <c r="M10" s="138"/>
+      <c r="N10" s="138"/>
+      <c r="O10" s="138"/>
+      <c r="P10" s="138"/>
+      <c r="Q10" s="138"/>
+      <c r="R10" s="139"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
       <c r="U10" s="17"/>
@@ -6878,26 +6879,26 @@
     <row r="11" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
-      <c r="C11" s="92" t="s">
+      <c r="C11" s="165" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="93"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="93"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="95" t="s">
+      <c r="D11" s="166"/>
+      <c r="E11" s="166"/>
+      <c r="F11" s="166"/>
+      <c r="G11" s="167"/>
+      <c r="H11" s="180" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="82"/>
+      <c r="I11" s="138"/>
+      <c r="J11" s="138"/>
+      <c r="K11" s="138"/>
+      <c r="L11" s="138"/>
+      <c r="M11" s="138"/>
+      <c r="N11" s="138"/>
+      <c r="O11" s="138"/>
+      <c r="P11" s="138"/>
+      <c r="Q11" s="138"/>
+      <c r="R11" s="139"/>
       <c r="S11" s="17"/>
       <c r="T11" s="17"/>
       <c r="U11" s="17"/>
@@ -7184,155 +7185,155 @@
     <row r="16" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
-      <c r="C16" s="96" t="s">
+      <c r="C16" s="181" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="83" t="s">
+      <c r="D16" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="84"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="83" t="s">
+      <c r="E16" s="184"/>
+      <c r="F16" s="172"/>
+      <c r="G16" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="85"/>
-      <c r="L16" s="83" t="s">
+      <c r="H16" s="184"/>
+      <c r="I16" s="184"/>
+      <c r="J16" s="184"/>
+      <c r="K16" s="172"/>
+      <c r="L16" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="M16" s="84"/>
-      <c r="N16" s="84"/>
-      <c r="O16" s="84"/>
-      <c r="P16" s="84"/>
-      <c r="Q16" s="84"/>
-      <c r="R16" s="84"/>
-      <c r="S16" s="84"/>
-      <c r="T16" s="84"/>
-      <c r="U16" s="84"/>
-      <c r="V16" s="85"/>
-      <c r="W16" s="83" t="s">
+      <c r="M16" s="184"/>
+      <c r="N16" s="184"/>
+      <c r="O16" s="184"/>
+      <c r="P16" s="184"/>
+      <c r="Q16" s="184"/>
+      <c r="R16" s="184"/>
+      <c r="S16" s="184"/>
+      <c r="T16" s="184"/>
+      <c r="U16" s="184"/>
+      <c r="V16" s="172"/>
+      <c r="W16" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="X16" s="84"/>
-      <c r="Y16" s="85"/>
-      <c r="Z16" s="98" t="s">
+      <c r="X16" s="184"/>
+      <c r="Y16" s="172"/>
+      <c r="Z16" s="171" t="s">
         <v>16</v>
       </c>
-      <c r="AA16" s="85"/>
-      <c r="AB16" s="98" t="s">
+      <c r="AA16" s="172"/>
+      <c r="AB16" s="171" t="s">
         <v>17</v>
       </c>
-      <c r="AC16" s="99"/>
-      <c r="AD16" s="99"/>
-      <c r="AE16" s="99"/>
-      <c r="AF16" s="99"/>
-      <c r="AG16" s="99"/>
-      <c r="AH16" s="99"/>
-      <c r="AI16" s="99"/>
-      <c r="AJ16" s="99"/>
-      <c r="AK16" s="100"/>
-      <c r="AL16" s="92" t="s">
+      <c r="AC16" s="175"/>
+      <c r="AD16" s="175"/>
+      <c r="AE16" s="175"/>
+      <c r="AF16" s="175"/>
+      <c r="AG16" s="175"/>
+      <c r="AH16" s="175"/>
+      <c r="AI16" s="175"/>
+      <c r="AJ16" s="175"/>
+      <c r="AK16" s="176"/>
+      <c r="AL16" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="AM16" s="93"/>
-      <c r="AN16" s="93"/>
-      <c r="AO16" s="93"/>
-      <c r="AP16" s="93"/>
-      <c r="AQ16" s="93"/>
-      <c r="AR16" s="94"/>
-      <c r="AS16" s="92" t="s">
+      <c r="AM16" s="166"/>
+      <c r="AN16" s="166"/>
+      <c r="AO16" s="166"/>
+      <c r="AP16" s="166"/>
+      <c r="AQ16" s="166"/>
+      <c r="AR16" s="167"/>
+      <c r="AS16" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="AT16" s="93"/>
-      <c r="AU16" s="93"/>
-      <c r="AV16" s="93"/>
-      <c r="AW16" s="93"/>
-      <c r="AX16" s="94"/>
-      <c r="AY16" s="104" t="s">
-        <v>46</v>
-      </c>
-      <c r="AZ16" s="105"/>
-      <c r="BA16" s="105"/>
-      <c r="BB16" s="105"/>
-      <c r="BC16" s="105"/>
-      <c r="BD16" s="105"/>
-      <c r="BE16" s="106"/>
+      <c r="AT16" s="166"/>
+      <c r="AU16" s="166"/>
+      <c r="AV16" s="166"/>
+      <c r="AW16" s="166"/>
+      <c r="AX16" s="167"/>
+      <c r="AY16" s="162" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ16" s="163"/>
+      <c r="BA16" s="163"/>
+      <c r="BB16" s="163"/>
+      <c r="BC16" s="163"/>
+      <c r="BD16" s="163"/>
+      <c r="BE16" s="164"/>
       <c r="BF16" s="17"/>
     </row>
     <row r="17" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
-      <c r="C17" s="97"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="86"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="87"/>
-      <c r="K17" s="88"/>
-      <c r="L17" s="86"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="87"/>
-      <c r="O17" s="87"/>
-      <c r="P17" s="87"/>
-      <c r="Q17" s="87"/>
-      <c r="R17" s="87"/>
-      <c r="S17" s="87"/>
-      <c r="T17" s="87"/>
-      <c r="U17" s="87"/>
-      <c r="V17" s="88"/>
-      <c r="W17" s="86"/>
-      <c r="X17" s="87"/>
-      <c r="Y17" s="88"/>
-      <c r="Z17" s="86"/>
-      <c r="AA17" s="88"/>
-      <c r="AB17" s="101"/>
-      <c r="AC17" s="102"/>
-      <c r="AD17" s="102"/>
-      <c r="AE17" s="102"/>
-      <c r="AF17" s="102"/>
-      <c r="AG17" s="102"/>
-      <c r="AH17" s="102"/>
-      <c r="AI17" s="102"/>
-      <c r="AJ17" s="102"/>
-      <c r="AK17" s="103"/>
-      <c r="AL17" s="92" t="s">
+      <c r="C17" s="182"/>
+      <c r="D17" s="173"/>
+      <c r="E17" s="185"/>
+      <c r="F17" s="174"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="185"/>
+      <c r="I17" s="185"/>
+      <c r="J17" s="185"/>
+      <c r="K17" s="174"/>
+      <c r="L17" s="173"/>
+      <c r="M17" s="185"/>
+      <c r="N17" s="185"/>
+      <c r="O17" s="185"/>
+      <c r="P17" s="185"/>
+      <c r="Q17" s="185"/>
+      <c r="R17" s="185"/>
+      <c r="S17" s="185"/>
+      <c r="T17" s="185"/>
+      <c r="U17" s="185"/>
+      <c r="V17" s="174"/>
+      <c r="W17" s="173"/>
+      <c r="X17" s="185"/>
+      <c r="Y17" s="174"/>
+      <c r="Z17" s="173"/>
+      <c r="AA17" s="174"/>
+      <c r="AB17" s="177"/>
+      <c r="AC17" s="178"/>
+      <c r="AD17" s="178"/>
+      <c r="AE17" s="178"/>
+      <c r="AF17" s="178"/>
+      <c r="AG17" s="178"/>
+      <c r="AH17" s="178"/>
+      <c r="AI17" s="178"/>
+      <c r="AJ17" s="178"/>
+      <c r="AK17" s="179"/>
+      <c r="AL17" s="165" t="s">
         <v>20</v>
       </c>
-      <c r="AM17" s="93"/>
-      <c r="AN17" s="92" t="s">
+      <c r="AM17" s="166"/>
+      <c r="AN17" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="AO17" s="93"/>
-      <c r="AP17" s="92" t="s">
+      <c r="AO17" s="166"/>
+      <c r="AP17" s="165" t="s">
         <v>22</v>
       </c>
-      <c r="AQ17" s="93"/>
-      <c r="AR17" s="94"/>
-      <c r="AS17" s="92" t="s">
+      <c r="AQ17" s="166"/>
+      <c r="AR17" s="167"/>
+      <c r="AS17" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="AT17" s="93"/>
-      <c r="AU17" s="94"/>
-      <c r="AV17" s="93" t="s">
+      <c r="AT17" s="166"/>
+      <c r="AU17" s="167"/>
+      <c r="AV17" s="166" t="s">
         <v>24</v>
       </c>
-      <c r="AW17" s="93"/>
-      <c r="AX17" s="94"/>
-      <c r="AY17" s="104" t="s">
+      <c r="AW17" s="166"/>
+      <c r="AX17" s="167"/>
+      <c r="AY17" s="162" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ17" s="163"/>
+      <c r="BA17" s="164"/>
+      <c r="BB17" s="168" t="s">
         <v>47</v>
       </c>
-      <c r="AZ17" s="105"/>
-      <c r="BA17" s="106"/>
-      <c r="BB17" s="107" t="s">
-        <v>48</v>
-      </c>
-      <c r="BC17" s="108"/>
-      <c r="BD17" s="108"/>
-      <c r="BE17" s="109"/>
+      <c r="BC17" s="169"/>
+      <c r="BD17" s="169"/>
+      <c r="BE17" s="170"/>
       <c r="BF17" s="17"/>
     </row>
     <row r="18" spans="1:58" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7341,86 +7342,86 @@
       <c r="C18" s="21">
         <v>1</v>
       </c>
-      <c r="D18" s="80" t="s">
+      <c r="D18" s="137" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="81"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="80" t="s">
+      <c r="E18" s="138"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="137" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="81"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="89" t="s">
+      <c r="H18" s="138"/>
+      <c r="I18" s="138"/>
+      <c r="J18" s="138"/>
+      <c r="K18" s="139"/>
+      <c r="L18" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="M18" s="90"/>
-      <c r="N18" s="90"/>
-      <c r="O18" s="90"/>
-      <c r="P18" s="90"/>
-      <c r="Q18" s="90"/>
-      <c r="R18" s="90"/>
-      <c r="S18" s="90"/>
-      <c r="T18" s="90"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="91"/>
-      <c r="W18" s="80" t="s">
+      <c r="M18" s="141"/>
+      <c r="N18" s="141"/>
+      <c r="O18" s="141"/>
+      <c r="P18" s="141"/>
+      <c r="Q18" s="141"/>
+      <c r="R18" s="141"/>
+      <c r="S18" s="141"/>
+      <c r="T18" s="141"/>
+      <c r="U18" s="141"/>
+      <c r="V18" s="142"/>
+      <c r="W18" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="X18" s="81"/>
-      <c r="Y18" s="82"/>
-      <c r="Z18" s="80" t="s">
+      <c r="X18" s="138"/>
+      <c r="Y18" s="139"/>
+      <c r="Z18" s="137" t="s">
         <v>29</v>
       </c>
-      <c r="AA18" s="82"/>
-      <c r="AB18" s="89" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC18" s="90"/>
-      <c r="AD18" s="90"/>
-      <c r="AE18" s="90"/>
-      <c r="AF18" s="90"/>
-      <c r="AG18" s="90"/>
-      <c r="AH18" s="90"/>
-      <c r="AI18" s="90"/>
-      <c r="AJ18" s="90"/>
-      <c r="AK18" s="91"/>
+      <c r="AA18" s="139"/>
+      <c r="AB18" s="140" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC18" s="141"/>
+      <c r="AD18" s="141"/>
+      <c r="AE18" s="141"/>
+      <c r="AF18" s="141"/>
+      <c r="AG18" s="141"/>
+      <c r="AH18" s="141"/>
+      <c r="AI18" s="141"/>
+      <c r="AJ18" s="141"/>
+      <c r="AK18" s="142"/>
       <c r="AL18" s="22" t="s">
         <v>2</v>
       </c>
       <c r="AM18" s="23"/>
       <c r="AN18" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO18" s="23"/>
+      <c r="AP18" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="AO18" s="23"/>
-      <c r="AP18" s="89" t="s">
+      <c r="AQ18" s="141"/>
+      <c r="AR18" s="142"/>
+      <c r="AS18" s="137" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT18" s="138"/>
+      <c r="AU18" s="139"/>
+      <c r="AV18" s="137" t="s">
         <v>32</v>
       </c>
-      <c r="AQ18" s="90"/>
-      <c r="AR18" s="91"/>
-      <c r="AS18" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT18" s="81"/>
-      <c r="AU18" s="82"/>
-      <c r="AV18" s="80" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW18" s="81"/>
-      <c r="AX18" s="82"/>
-      <c r="AY18" s="80" t="s">
+      <c r="AW18" s="138"/>
+      <c r="AX18" s="139"/>
+      <c r="AY18" s="137" t="s">
         <v>25</v>
       </c>
-      <c r="AZ18" s="81"/>
-      <c r="BA18" s="82"/>
-      <c r="BB18" s="80" t="s">
+      <c r="AZ18" s="138"/>
+      <c r="BA18" s="139"/>
+      <c r="BB18" s="137" t="s">
         <v>26</v>
       </c>
-      <c r="BC18" s="81"/>
-      <c r="BD18" s="81"/>
-      <c r="BE18" s="82"/>
+      <c r="BC18" s="138"/>
+      <c r="BD18" s="138"/>
+      <c r="BE18" s="139"/>
       <c r="BF18" s="20"/>
     </row>
     <row r="19" spans="1:58" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7429,86 +7430,86 @@
       <c r="C19" s="21">
         <v>2</v>
       </c>
-      <c r="D19" s="80" t="s">
+      <c r="D19" s="137" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="138"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="81"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="80" t="s">
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="138"/>
+      <c r="K19" s="139"/>
+      <c r="L19" s="140" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="89" t="s">
+      <c r="M19" s="141"/>
+      <c r="N19" s="141"/>
+      <c r="O19" s="141"/>
+      <c r="P19" s="141"/>
+      <c r="Q19" s="141"/>
+      <c r="R19" s="141"/>
+      <c r="S19" s="141"/>
+      <c r="T19" s="141"/>
+      <c r="U19" s="141"/>
+      <c r="V19" s="142"/>
+      <c r="W19" s="137" t="s">
+        <v>28</v>
+      </c>
+      <c r="X19" s="138"/>
+      <c r="Y19" s="139"/>
+      <c r="Z19" s="137" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA19" s="139"/>
+      <c r="AB19" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="M19" s="90"/>
-      <c r="N19" s="90"/>
-      <c r="O19" s="90"/>
-      <c r="P19" s="90"/>
-      <c r="Q19" s="90"/>
-      <c r="R19" s="90"/>
-      <c r="S19" s="90"/>
-      <c r="T19" s="90"/>
-      <c r="U19" s="90"/>
-      <c r="V19" s="91"/>
-      <c r="W19" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="X19" s="81"/>
-      <c r="Y19" s="82"/>
-      <c r="Z19" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA19" s="82"/>
-      <c r="AB19" s="89" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC19" s="90"/>
-      <c r="AD19" s="90"/>
-      <c r="AE19" s="90"/>
-      <c r="AF19" s="90"/>
-      <c r="AG19" s="90"/>
-      <c r="AH19" s="90"/>
-      <c r="AI19" s="90"/>
-      <c r="AJ19" s="90"/>
-      <c r="AK19" s="91"/>
+      <c r="AC19" s="141"/>
+      <c r="AD19" s="141"/>
+      <c r="AE19" s="141"/>
+      <c r="AF19" s="141"/>
+      <c r="AG19" s="141"/>
+      <c r="AH19" s="141"/>
+      <c r="AI19" s="141"/>
+      <c r="AJ19" s="141"/>
+      <c r="AK19" s="142"/>
       <c r="AL19" s="22" t="s">
         <v>2</v>
       </c>
       <c r="AM19" s="23"/>
       <c r="AN19" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO19" s="23"/>
+      <c r="AP19" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="AO19" s="23"/>
-      <c r="AP19" s="89" t="s">
-        <v>32</v>
-      </c>
-      <c r="AQ19" s="90"/>
-      <c r="AR19" s="91"/>
-      <c r="AS19" s="80" t="s">
+      <c r="AQ19" s="141"/>
+      <c r="AR19" s="142"/>
+      <c r="AS19" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="AT19" s="81"/>
-      <c r="AU19" s="82"/>
-      <c r="AV19" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW19" s="81"/>
-      <c r="AX19" s="82"/>
-      <c r="AY19" s="80" t="s">
+      <c r="AT19" s="138"/>
+      <c r="AU19" s="139"/>
+      <c r="AV19" s="137" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW19" s="138"/>
+      <c r="AX19" s="139"/>
+      <c r="AY19" s="137" t="s">
+        <v>33</v>
+      </c>
+      <c r="AZ19" s="138"/>
+      <c r="BA19" s="139"/>
+      <c r="BB19" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="AZ19" s="81"/>
-      <c r="BA19" s="82"/>
-      <c r="BB19" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="BC19" s="81"/>
-      <c r="BD19" s="81"/>
-      <c r="BE19" s="82"/>
+      <c r="BC19" s="138"/>
+      <c r="BD19" s="138"/>
+      <c r="BE19" s="139"/>
       <c r="BF19" s="20"/>
     </row>
     <row r="20" spans="1:58" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7517,86 +7518,86 @@
       <c r="C20" s="21">
         <v>3</v>
       </c>
-      <c r="D20" s="80" t="s">
+      <c r="D20" s="137" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="138"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="81"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="80" t="s">
+      <c r="H20" s="138"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="138"/>
+      <c r="K20" s="139"/>
+      <c r="L20" s="140" t="s">
         <v>40</v>
       </c>
-      <c r="H20" s="81"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="82"/>
-      <c r="L20" s="89" t="s">
+      <c r="M20" s="141"/>
+      <c r="N20" s="141"/>
+      <c r="O20" s="141"/>
+      <c r="P20" s="141"/>
+      <c r="Q20" s="141"/>
+      <c r="R20" s="141"/>
+      <c r="S20" s="141"/>
+      <c r="T20" s="141"/>
+      <c r="U20" s="141"/>
+      <c r="V20" s="142"/>
+      <c r="W20" s="137" t="s">
+        <v>28</v>
+      </c>
+      <c r="X20" s="138"/>
+      <c r="Y20" s="139"/>
+      <c r="Z20" s="137" t="s">
         <v>41</v>
       </c>
-      <c r="M20" s="90"/>
-      <c r="N20" s="90"/>
-      <c r="O20" s="90"/>
-      <c r="P20" s="90"/>
-      <c r="Q20" s="90"/>
-      <c r="R20" s="90"/>
-      <c r="S20" s="90"/>
-      <c r="T20" s="90"/>
-      <c r="U20" s="90"/>
-      <c r="V20" s="91"/>
-      <c r="W20" s="80" t="s">
-        <v>28</v>
-      </c>
-      <c r="X20" s="81"/>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="80" t="s">
+      <c r="AA20" s="139"/>
+      <c r="AB20" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="AA20" s="82"/>
-      <c r="AB20" s="89" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC20" s="90"/>
-      <c r="AD20" s="90"/>
-      <c r="AE20" s="90"/>
-      <c r="AF20" s="90"/>
-      <c r="AG20" s="90"/>
-      <c r="AH20" s="90"/>
-      <c r="AI20" s="90"/>
-      <c r="AJ20" s="90"/>
-      <c r="AK20" s="91"/>
+      <c r="AC20" s="141"/>
+      <c r="AD20" s="141"/>
+      <c r="AE20" s="141"/>
+      <c r="AF20" s="141"/>
+      <c r="AG20" s="141"/>
+      <c r="AH20" s="141"/>
+      <c r="AI20" s="141"/>
+      <c r="AJ20" s="141"/>
+      <c r="AK20" s="142"/>
       <c r="AL20" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AM20" s="23"/>
       <c r="AN20" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO20" s="23"/>
+      <c r="AP20" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="AO20" s="23"/>
-      <c r="AP20" s="89" t="s">
-        <v>32</v>
-      </c>
-      <c r="AQ20" s="90"/>
-      <c r="AR20" s="91"/>
-      <c r="AS20" s="80" t="s">
+      <c r="AQ20" s="141"/>
+      <c r="AR20" s="142"/>
+      <c r="AS20" s="137" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT20" s="138"/>
+      <c r="AU20" s="139"/>
+      <c r="AV20" s="137" t="s">
         <v>44</v>
       </c>
-      <c r="AT20" s="81"/>
-      <c r="AU20" s="82"/>
-      <c r="AV20" s="80" t="s">
-        <v>45</v>
-      </c>
-      <c r="AW20" s="81"/>
-      <c r="AX20" s="82"/>
-      <c r="AY20" s="80" t="s">
+      <c r="AW20" s="138"/>
+      <c r="AX20" s="139"/>
+      <c r="AY20" s="137" t="s">
+        <v>38</v>
+      </c>
+      <c r="AZ20" s="138"/>
+      <c r="BA20" s="139"/>
+      <c r="BB20" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="AZ20" s="81"/>
-      <c r="BA20" s="82"/>
-      <c r="BB20" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="BC20" s="81"/>
-      <c r="BD20" s="81"/>
-      <c r="BE20" s="82"/>
+      <c r="BC20" s="138"/>
+      <c r="BD20" s="138"/>
+      <c r="BE20" s="139"/>
       <c r="BF20" s="20"/>
     </row>
     <row r="21" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7667,49 +7668,18 @@
     <row r="27" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="AY16:BE16"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AN17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AY17:BA17"/>
-    <mergeCell ref="BB17:BE17"/>
-    <mergeCell ref="AL16:AR16"/>
-    <mergeCell ref="AS16:AX16"/>
-    <mergeCell ref="AV17:AX17"/>
-    <mergeCell ref="AS17:AU17"/>
-    <mergeCell ref="BB18:BE18"/>
-    <mergeCell ref="BB19:BE19"/>
-    <mergeCell ref="BB20:BE20"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AY18:BA18"/>
-    <mergeCell ref="AY19:BA19"/>
-    <mergeCell ref="AY20:BA20"/>
-    <mergeCell ref="AV18:AX18"/>
-    <mergeCell ref="AV19:AX19"/>
-    <mergeCell ref="AV20:AX20"/>
-    <mergeCell ref="AS18:AU18"/>
-    <mergeCell ref="AS19:AU19"/>
-    <mergeCell ref="AS20:AU20"/>
-    <mergeCell ref="AB18:AK18"/>
-    <mergeCell ref="AB19:AK19"/>
-    <mergeCell ref="AB20:AK20"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="AG3:AI3"/>
-    <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="Z16:AA17"/>
-    <mergeCell ref="AB16:AK17"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AC3:AF3"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="S1:Z3"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="W19:Y19"/>
+    <mergeCell ref="W20:Y20"/>
+    <mergeCell ref="W16:Y17"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="L19:V19"/>
+    <mergeCell ref="L20:V20"/>
+    <mergeCell ref="L16:V17"/>
+    <mergeCell ref="L18:V18"/>
+    <mergeCell ref="G16:K17"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G20:K20"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D19:F19"/>
@@ -7726,18 +7696,49 @@
     <mergeCell ref="D16:F17"/>
     <mergeCell ref="H10:R10"/>
     <mergeCell ref="O1:R3"/>
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="W19:Y19"/>
-    <mergeCell ref="W20:Y20"/>
-    <mergeCell ref="W16:Y17"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="L19:V19"/>
-    <mergeCell ref="L20:V20"/>
-    <mergeCell ref="L16:V17"/>
-    <mergeCell ref="L18:V18"/>
-    <mergeCell ref="G16:K17"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="AG3:AI3"/>
+    <mergeCell ref="AG1:AI1"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="Z16:AA17"/>
+    <mergeCell ref="AB16:AK17"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AC3:AF3"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="S1:Z3"/>
+    <mergeCell ref="AB18:AK18"/>
+    <mergeCell ref="AB19:AK19"/>
+    <mergeCell ref="AB20:AK20"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="BB18:BE18"/>
+    <mergeCell ref="BB19:BE19"/>
+    <mergeCell ref="BB20:BE20"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AY18:BA18"/>
+    <mergeCell ref="AY19:BA19"/>
+    <mergeCell ref="AY20:BA20"/>
+    <mergeCell ref="AV18:AX18"/>
+    <mergeCell ref="AV19:AX19"/>
+    <mergeCell ref="AV20:AX20"/>
+    <mergeCell ref="AS18:AU18"/>
+    <mergeCell ref="AS19:AU19"/>
+    <mergeCell ref="AS20:AU20"/>
+    <mergeCell ref="AY16:BE16"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AN17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AY17:BA17"/>
+    <mergeCell ref="BB17:BE17"/>
+    <mergeCell ref="AL16:AR16"/>
+    <mergeCell ref="AS16:AX16"/>
+    <mergeCell ref="AV17:AX17"/>
+    <mergeCell ref="AS17:AU17"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Nab 458 criteria check (#137)
* 設計書最終調整

* 開発ガイド最終調整（PGUT工程）

* リリースに向けた体裁調整

* デグレを復旧
</commit_message>
<xml_diff>
--- a/en/Sample_Project/Design_Document/B1_Client_Management_System/030_Application_Design/030_Interface_Design/Web_Service_API_List_B1_Client_Management_System.xlsx
+++ b/en/Sample_Project/Design_Document/B1_Client_Management_System/030_Application_Design/030_Interface_Design/Web_Service_API_List_B1_Client_Management_System.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B5776C-730D-4D05-A5B4-9FCA7C59CE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB5BDA8-A939-458F-9150-FDF9452E4DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="28" r:id="rId1"/>
@@ -1338,6 +1338,60 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="32" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="41" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1485,66 +1539,42 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="32" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="11" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="24" borderId="12" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="13" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="14" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="15" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="24" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" xfId="41" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="25" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="16" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="17" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="18" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="177" fontId="32" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1554,35 +1584,59 @@
     <xf numFmtId="177" fontId="32" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="11" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="13" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="14" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="15" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="24" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" xfId="41" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="25" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="16" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="17" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="18" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1593,15 +1647,6 @@
     <xf numFmtId="0" fontId="32" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1609,51 +1654,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="24" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3061,145 +3061,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="84" t="s">
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="90" t="s">
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="55" t="s">
+      <c r="P1" s="109"/>
+      <c r="Q1" s="109"/>
+      <c r="R1" s="110"/>
+      <c r="S1" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="81" t="s">
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="AB1" s="83"/>
-      <c r="AC1" s="99" t="s">
+      <c r="AB1" s="101"/>
+      <c r="AC1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="AD1" s="100"/>
-      <c r="AE1" s="100"/>
-      <c r="AF1" s="101"/>
-      <c r="AG1" s="64">
+      <c r="AD1" s="118"/>
+      <c r="AE1" s="118"/>
+      <c r="AF1" s="119"/>
+      <c r="AG1" s="82">
         <v>43404</v>
       </c>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="66"/>
+      <c r="AH1" s="83"/>
+      <c r="AI1" s="84"/>
     </row>
     <row r="2" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="99" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="84" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="102" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="93"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
-      <c r="R2" s="95"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="81" t="s">
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="112"/>
+      <c r="Q2" s="112"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
+      <c r="X2" s="77"/>
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="AB2" s="83"/>
-      <c r="AC2" s="87" t="str">
+      <c r="AB2" s="101"/>
+      <c r="AC2" s="105" t="str">
         <f ca="1">IF(COUNTA(AF9:AF33)&lt;&gt;0,INDIRECT("AF"&amp;(COUNTA(AF9:AF33)+8)),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD2" s="88"/>
-      <c r="AE2" s="88"/>
-      <c r="AF2" s="89"/>
-      <c r="AG2" s="64">
+      <c r="AD2" s="106"/>
+      <c r="AE2" s="106"/>
+      <c r="AF2" s="107"/>
+      <c r="AG2" s="82">
         <f>IF(D9="","",MAX(D9:F33))</f>
         <v>44833</v>
       </c>
-      <c r="AH2" s="65"/>
-      <c r="AI2" s="66"/>
+      <c r="AH2" s="83"/>
+      <c r="AI2" s="84"/>
     </row>
     <row r="3" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="84" t="s">
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="96"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="62"/>
-      <c r="U3" s="62"/>
-      <c r="V3" s="62"/>
-      <c r="W3" s="62"/>
-      <c r="X3" s="62"/>
-      <c r="Y3" s="62"/>
-      <c r="Z3" s="63"/>
-      <c r="AA3" s="81"/>
-      <c r="AB3" s="83"/>
-      <c r="AC3" s="99"/>
-      <c r="AD3" s="100"/>
-      <c r="AE3" s="100"/>
-      <c r="AF3" s="101"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="65"/>
-      <c r="AI3" s="66"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="114"/>
+      <c r="P3" s="115"/>
+      <c r="Q3" s="115"/>
+      <c r="R3" s="116"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="81"/>
+      <c r="AA3" s="99"/>
+      <c r="AB3" s="101"/>
+      <c r="AC3" s="117"/>
+      <c r="AD3" s="118"/>
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="119"/>
+      <c r="AG3" s="82"/>
+      <c r="AH3" s="83"/>
+      <c r="AI3" s="84"/>
     </row>
     <row r="5" spans="1:35" s="25" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N5" s="46" t="s">
@@ -3231,1203 +3231,1048 @@
       <c r="A7" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="102" t="s">
+      <c r="B7" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="103"/>
-      <c r="D7" s="104" t="s">
+      <c r="C7" s="121"/>
+      <c r="D7" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="105"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="104" t="s">
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="105"/>
-      <c r="I7" s="106"/>
-      <c r="J7" s="104" t="s">
+      <c r="H7" s="71"/>
+      <c r="I7" s="72"/>
+      <c r="J7" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="105"/>
-      <c r="L7" s="105"/>
-      <c r="M7" s="105"/>
-      <c r="N7" s="105"/>
-      <c r="O7" s="105"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="104" t="s">
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="R7" s="105"/>
-      <c r="S7" s="105"/>
-      <c r="T7" s="105"/>
-      <c r="U7" s="105"/>
-      <c r="V7" s="105"/>
-      <c r="W7" s="105"/>
-      <c r="X7" s="105"/>
-      <c r="Y7" s="105"/>
-      <c r="Z7" s="105"/>
-      <c r="AA7" s="105"/>
-      <c r="AB7" s="105"/>
-      <c r="AC7" s="105"/>
-      <c r="AD7" s="105"/>
-      <c r="AE7" s="106"/>
-      <c r="AF7" s="104" t="s">
+      <c r="R7" s="71"/>
+      <c r="S7" s="71"/>
+      <c r="T7" s="71"/>
+      <c r="U7" s="71"/>
+      <c r="V7" s="71"/>
+      <c r="W7" s="71"/>
+      <c r="X7" s="71"/>
+      <c r="Y7" s="71"/>
+      <c r="Z7" s="71"/>
+      <c r="AA7" s="71"/>
+      <c r="AB7" s="71"/>
+      <c r="AC7" s="71"/>
+      <c r="AD7" s="71"/>
+      <c r="AE7" s="72"/>
+      <c r="AF7" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="AG7" s="105"/>
-      <c r="AH7" s="105"/>
-      <c r="AI7" s="106"/>
+      <c r="AG7" s="71"/>
+      <c r="AH7" s="71"/>
+      <c r="AI7" s="72"/>
     </row>
     <row r="8" spans="1:35" s="50" customFormat="1" ht="26.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A8" s="51">
         <v>1</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="69">
+      <c r="C8" s="86"/>
+      <c r="D8" s="87">
         <v>43404</v>
       </c>
-      <c r="E8" s="70"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="72" t="s">
+      <c r="E8" s="88"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="H8" s="73"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="75" t="s">
+      <c r="H8" s="91"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="76"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="77"/>
-      <c r="Q8" s="75" t="s">
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="94"/>
+      <c r="O8" s="94"/>
+      <c r="P8" s="95"/>
+      <c r="Q8" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="76"/>
-      <c r="W8" s="76"/>
-      <c r="X8" s="76"/>
-      <c r="Y8" s="76"/>
-      <c r="Z8" s="76"/>
-      <c r="AA8" s="76"/>
-      <c r="AB8" s="76"/>
-      <c r="AC8" s="76"/>
-      <c r="AD8" s="76"/>
-      <c r="AE8" s="77"/>
-      <c r="AF8" s="78" t="s">
+      <c r="R8" s="94"/>
+      <c r="S8" s="94"/>
+      <c r="T8" s="94"/>
+      <c r="U8" s="94"/>
+      <c r="V8" s="94"/>
+      <c r="W8" s="94"/>
+      <c r="X8" s="94"/>
+      <c r="Y8" s="94"/>
+      <c r="Z8" s="94"/>
+      <c r="AA8" s="94"/>
+      <c r="AB8" s="94"/>
+      <c r="AC8" s="94"/>
+      <c r="AD8" s="94"/>
+      <c r="AE8" s="95"/>
+      <c r="AF8" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="AG8" s="79"/>
-      <c r="AH8" s="79"/>
-      <c r="AI8" s="80"/>
+      <c r="AG8" s="97"/>
+      <c r="AH8" s="97"/>
+      <c r="AI8" s="98"/>
     </row>
     <row r="9" spans="1:35" s="50" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="52">
         <v>2</v>
       </c>
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="108"/>
-      <c r="D9" s="109">
+      <c r="C9" s="56"/>
+      <c r="D9" s="57">
         <v>44833</v>
       </c>
-      <c r="E9" s="110"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="109" t="s">
+      <c r="E9" s="58"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="113"/>
-      <c r="I9" s="114"/>
-      <c r="J9" s="115" t="s">
+      <c r="H9" s="61"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
-      <c r="M9" s="116"/>
-      <c r="N9" s="116"/>
-      <c r="O9" s="116"/>
-      <c r="P9" s="117"/>
-      <c r="Q9" s="118" t="s">
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="64"/>
+      <c r="O9" s="64"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="R9" s="119"/>
-      <c r="S9" s="119"/>
-      <c r="T9" s="119"/>
-      <c r="U9" s="119"/>
-      <c r="V9" s="119"/>
-      <c r="W9" s="119"/>
-      <c r="X9" s="119"/>
-      <c r="Y9" s="119"/>
-      <c r="Z9" s="119"/>
-      <c r="AA9" s="119"/>
-      <c r="AB9" s="119"/>
-      <c r="AC9" s="119"/>
-      <c r="AD9" s="119"/>
-      <c r="AE9" s="120"/>
-      <c r="AF9" s="115" t="s">
+      <c r="R9" s="67"/>
+      <c r="S9" s="67"/>
+      <c r="T9" s="67"/>
+      <c r="U9" s="67"/>
+      <c r="V9" s="67"/>
+      <c r="W9" s="67"/>
+      <c r="X9" s="67"/>
+      <c r="Y9" s="67"/>
+      <c r="Z9" s="67"/>
+      <c r="AA9" s="67"/>
+      <c r="AB9" s="67"/>
+      <c r="AC9" s="67"/>
+      <c r="AD9" s="67"/>
+      <c r="AE9" s="68"/>
+      <c r="AF9" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="AG9" s="116"/>
-      <c r="AH9" s="116"/>
-      <c r="AI9" s="117"/>
+      <c r="AG9" s="64"/>
+      <c r="AH9" s="64"/>
+      <c r="AI9" s="65"/>
     </row>
     <row r="10" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="52"/>
-      <c r="B10" s="107"/>
-      <c r="C10" s="108"/>
-      <c r="D10" s="109"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="111"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="113"/>
-      <c r="I10" s="114"/>
-      <c r="J10" s="115"/>
-      <c r="K10" s="116"/>
-      <c r="L10" s="116"/>
-      <c r="M10" s="116"/>
-      <c r="N10" s="116"/>
-      <c r="O10" s="116"/>
-      <c r="P10" s="117"/>
-      <c r="Q10" s="118"/>
-      <c r="R10" s="119"/>
-      <c r="S10" s="119"/>
-      <c r="T10" s="119"/>
-      <c r="U10" s="119"/>
-      <c r="V10" s="119"/>
-      <c r="W10" s="119"/>
-      <c r="X10" s="119"/>
-      <c r="Y10" s="119"/>
-      <c r="Z10" s="119"/>
-      <c r="AA10" s="119"/>
-      <c r="AB10" s="119"/>
-      <c r="AC10" s="119"/>
-      <c r="AD10" s="119"/>
-      <c r="AE10" s="120"/>
-      <c r="AF10" s="115"/>
-      <c r="AG10" s="116"/>
-      <c r="AH10" s="116"/>
-      <c r="AI10" s="117"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="67"/>
+      <c r="S10" s="67"/>
+      <c r="T10" s="67"/>
+      <c r="U10" s="67"/>
+      <c r="V10" s="67"/>
+      <c r="W10" s="67"/>
+      <c r="X10" s="67"/>
+      <c r="Y10" s="67"/>
+      <c r="Z10" s="67"/>
+      <c r="AA10" s="67"/>
+      <c r="AB10" s="67"/>
+      <c r="AC10" s="67"/>
+      <c r="AD10" s="67"/>
+      <c r="AE10" s="68"/>
+      <c r="AF10" s="63"/>
+      <c r="AG10" s="64"/>
+      <c r="AH10" s="64"/>
+      <c r="AI10" s="65"/>
     </row>
     <row r="11" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="52"/>
-      <c r="B11" s="107"/>
-      <c r="C11" s="108"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="112"/>
-      <c r="H11" s="113"/>
-      <c r="I11" s="114"/>
-      <c r="J11" s="115"/>
-      <c r="K11" s="116"/>
-      <c r="L11" s="116"/>
-      <c r="M11" s="116"/>
-      <c r="N11" s="116"/>
-      <c r="O11" s="116"/>
-      <c r="P11" s="117"/>
-      <c r="Q11" s="118"/>
-      <c r="R11" s="119"/>
-      <c r="S11" s="119"/>
-      <c r="T11" s="119"/>
-      <c r="U11" s="119"/>
-      <c r="V11" s="119"/>
-      <c r="W11" s="119"/>
-      <c r="X11" s="119"/>
-      <c r="Y11" s="119"/>
-      <c r="Z11" s="119"/>
-      <c r="AA11" s="119"/>
-      <c r="AB11" s="119"/>
-      <c r="AC11" s="119"/>
-      <c r="AD11" s="119"/>
-      <c r="AE11" s="120"/>
-      <c r="AF11" s="115"/>
-      <c r="AG11" s="116"/>
-      <c r="AH11" s="116"/>
-      <c r="AI11" s="117"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="62"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="67"/>
+      <c r="S11" s="67"/>
+      <c r="T11" s="67"/>
+      <c r="U11" s="67"/>
+      <c r="V11" s="67"/>
+      <c r="W11" s="67"/>
+      <c r="X11" s="67"/>
+      <c r="Y11" s="67"/>
+      <c r="Z11" s="67"/>
+      <c r="AA11" s="67"/>
+      <c r="AB11" s="67"/>
+      <c r="AC11" s="67"/>
+      <c r="AD11" s="67"/>
+      <c r="AE11" s="68"/>
+      <c r="AF11" s="63"/>
+      <c r="AG11" s="64"/>
+      <c r="AH11" s="64"/>
+      <c r="AI11" s="65"/>
     </row>
     <row r="12" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="52"/>
-      <c r="B12" s="107"/>
-      <c r="C12" s="108"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="112"/>
-      <c r="H12" s="113"/>
-      <c r="I12" s="114"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="116"/>
-      <c r="L12" s="116"/>
-      <c r="M12" s="116"/>
-      <c r="N12" s="116"/>
-      <c r="O12" s="116"/>
-      <c r="P12" s="117"/>
-      <c r="Q12" s="118"/>
-      <c r="R12" s="119"/>
-      <c r="S12" s="119"/>
-      <c r="T12" s="119"/>
-      <c r="U12" s="119"/>
-      <c r="V12" s="119"/>
-      <c r="W12" s="119"/>
-      <c r="X12" s="119"/>
-      <c r="Y12" s="119"/>
-      <c r="Z12" s="119"/>
-      <c r="AA12" s="119"/>
-      <c r="AB12" s="119"/>
-      <c r="AC12" s="119"/>
-      <c r="AD12" s="119"/>
-      <c r="AE12" s="120"/>
-      <c r="AF12" s="115"/>
-      <c r="AG12" s="116"/>
-      <c r="AH12" s="116"/>
-      <c r="AI12" s="117"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="67"/>
+      <c r="T12" s="67"/>
+      <c r="U12" s="67"/>
+      <c r="V12" s="67"/>
+      <c r="W12" s="67"/>
+      <c r="X12" s="67"/>
+      <c r="Y12" s="67"/>
+      <c r="Z12" s="67"/>
+      <c r="AA12" s="67"/>
+      <c r="AB12" s="67"/>
+      <c r="AC12" s="67"/>
+      <c r="AD12" s="67"/>
+      <c r="AE12" s="68"/>
+      <c r="AF12" s="63"/>
+      <c r="AG12" s="64"/>
+      <c r="AH12" s="64"/>
+      <c r="AI12" s="65"/>
     </row>
     <row r="13" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="52"/>
-      <c r="B13" s="107"/>
-      <c r="C13" s="108"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="110"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="114"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="116"/>
-      <c r="L13" s="116"/>
-      <c r="M13" s="116"/>
-      <c r="N13" s="116"/>
-      <c r="O13" s="116"/>
-      <c r="P13" s="117"/>
-      <c r="Q13" s="118"/>
-      <c r="R13" s="119"/>
-      <c r="S13" s="119"/>
-      <c r="T13" s="119"/>
-      <c r="U13" s="119"/>
-      <c r="V13" s="119"/>
-      <c r="W13" s="119"/>
-      <c r="X13" s="119"/>
-      <c r="Y13" s="119"/>
-      <c r="Z13" s="119"/>
-      <c r="AA13" s="119"/>
-      <c r="AB13" s="119"/>
-      <c r="AC13" s="119"/>
-      <c r="AD13" s="119"/>
-      <c r="AE13" s="120"/>
-      <c r="AF13" s="115"/>
-      <c r="AG13" s="116"/>
-      <c r="AH13" s="116"/>
-      <c r="AI13" s="117"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="67"/>
+      <c r="S13" s="67"/>
+      <c r="T13" s="67"/>
+      <c r="U13" s="67"/>
+      <c r="V13" s="67"/>
+      <c r="W13" s="67"/>
+      <c r="X13" s="67"/>
+      <c r="Y13" s="67"/>
+      <c r="Z13" s="67"/>
+      <c r="AA13" s="67"/>
+      <c r="AB13" s="67"/>
+      <c r="AC13" s="67"/>
+      <c r="AD13" s="67"/>
+      <c r="AE13" s="68"/>
+      <c r="AF13" s="63"/>
+      <c r="AG13" s="64"/>
+      <c r="AH13" s="64"/>
+      <c r="AI13" s="65"/>
     </row>
     <row r="14" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="52"/>
-      <c r="B14" s="107"/>
-      <c r="C14" s="108"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="110"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="112"/>
-      <c r="H14" s="113"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="115"/>
-      <c r="K14" s="116"/>
-      <c r="L14" s="116"/>
-      <c r="M14" s="116"/>
-      <c r="N14" s="116"/>
-      <c r="O14" s="116"/>
-      <c r="P14" s="117"/>
-      <c r="Q14" s="118"/>
-      <c r="R14" s="119"/>
-      <c r="S14" s="119"/>
-      <c r="T14" s="119"/>
-      <c r="U14" s="119"/>
-      <c r="V14" s="119"/>
-      <c r="W14" s="119"/>
-      <c r="X14" s="119"/>
-      <c r="Y14" s="119"/>
-      <c r="Z14" s="119"/>
-      <c r="AA14" s="119"/>
-      <c r="AB14" s="119"/>
-      <c r="AC14" s="119"/>
-      <c r="AD14" s="119"/>
-      <c r="AE14" s="120"/>
-      <c r="AF14" s="115"/>
-      <c r="AG14" s="116"/>
-      <c r="AH14" s="116"/>
-      <c r="AI14" s="117"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="64"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="67"/>
+      <c r="S14" s="67"/>
+      <c r="T14" s="67"/>
+      <c r="U14" s="67"/>
+      <c r="V14" s="67"/>
+      <c r="W14" s="67"/>
+      <c r="X14" s="67"/>
+      <c r="Y14" s="67"/>
+      <c r="Z14" s="67"/>
+      <c r="AA14" s="67"/>
+      <c r="AB14" s="67"/>
+      <c r="AC14" s="67"/>
+      <c r="AD14" s="67"/>
+      <c r="AE14" s="68"/>
+      <c r="AF14" s="63"/>
+      <c r="AG14" s="64"/>
+      <c r="AH14" s="64"/>
+      <c r="AI14" s="65"/>
     </row>
     <row r="15" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="52"/>
-      <c r="B15" s="107"/>
-      <c r="C15" s="108"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="111"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="114"/>
-      <c r="J15" s="115"/>
-      <c r="K15" s="116"/>
-      <c r="L15" s="116"/>
-      <c r="M15" s="116"/>
-      <c r="N15" s="116"/>
-      <c r="O15" s="116"/>
-      <c r="P15" s="117"/>
-      <c r="Q15" s="118"/>
-      <c r="R15" s="119"/>
-      <c r="S15" s="119"/>
-      <c r="T15" s="119"/>
-      <c r="U15" s="119"/>
-      <c r="V15" s="119"/>
-      <c r="W15" s="119"/>
-      <c r="X15" s="119"/>
-      <c r="Y15" s="119"/>
-      <c r="Z15" s="119"/>
-      <c r="AA15" s="119"/>
-      <c r="AB15" s="119"/>
-      <c r="AC15" s="119"/>
-      <c r="AD15" s="119"/>
-      <c r="AE15" s="120"/>
-      <c r="AF15" s="115"/>
-      <c r="AG15" s="116"/>
-      <c r="AH15" s="116"/>
-      <c r="AI15" s="117"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="65"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="67"/>
+      <c r="S15" s="67"/>
+      <c r="T15" s="67"/>
+      <c r="U15" s="67"/>
+      <c r="V15" s="67"/>
+      <c r="W15" s="67"/>
+      <c r="X15" s="67"/>
+      <c r="Y15" s="67"/>
+      <c r="Z15" s="67"/>
+      <c r="AA15" s="67"/>
+      <c r="AB15" s="67"/>
+      <c r="AC15" s="67"/>
+      <c r="AD15" s="67"/>
+      <c r="AE15" s="68"/>
+      <c r="AF15" s="63"/>
+      <c r="AG15" s="64"/>
+      <c r="AH15" s="64"/>
+      <c r="AI15" s="65"/>
     </row>
     <row r="16" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="52"/>
-      <c r="B16" s="107"/>
-      <c r="C16" s="108"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="112"/>
-      <c r="H16" s="113"/>
-      <c r="I16" s="114"/>
-      <c r="J16" s="115"/>
-      <c r="K16" s="116"/>
-      <c r="L16" s="116"/>
-      <c r="M16" s="116"/>
-      <c r="N16" s="116"/>
-      <c r="O16" s="116"/>
-      <c r="P16" s="117"/>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="119"/>
-      <c r="S16" s="119"/>
-      <c r="T16" s="119"/>
-      <c r="U16" s="119"/>
-      <c r="V16" s="119"/>
-      <c r="W16" s="119"/>
-      <c r="X16" s="119"/>
-      <c r="Y16" s="119"/>
-      <c r="Z16" s="119"/>
-      <c r="AA16" s="119"/>
-      <c r="AB16" s="119"/>
-      <c r="AC16" s="119"/>
-      <c r="AD16" s="119"/>
-      <c r="AE16" s="120"/>
-      <c r="AF16" s="115"/>
-      <c r="AG16" s="116"/>
-      <c r="AH16" s="116"/>
-      <c r="AI16" s="117"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="63"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="64"/>
+      <c r="P16" s="65"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="67"/>
+      <c r="S16" s="67"/>
+      <c r="T16" s="67"/>
+      <c r="U16" s="67"/>
+      <c r="V16" s="67"/>
+      <c r="W16" s="67"/>
+      <c r="X16" s="67"/>
+      <c r="Y16" s="67"/>
+      <c r="Z16" s="67"/>
+      <c r="AA16" s="67"/>
+      <c r="AB16" s="67"/>
+      <c r="AC16" s="67"/>
+      <c r="AD16" s="67"/>
+      <c r="AE16" s="68"/>
+      <c r="AF16" s="63"/>
+      <c r="AG16" s="64"/>
+      <c r="AH16" s="64"/>
+      <c r="AI16" s="65"/>
     </row>
     <row r="17" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="52"/>
-      <c r="B17" s="107"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="111"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="113"/>
-      <c r="I17" s="114"/>
-      <c r="J17" s="115"/>
-      <c r="K17" s="116"/>
-      <c r="L17" s="116"/>
-      <c r="M17" s="116"/>
-      <c r="N17" s="116"/>
-      <c r="O17" s="116"/>
-      <c r="P17" s="117"/>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="119"/>
-      <c r="S17" s="119"/>
-      <c r="T17" s="119"/>
-      <c r="U17" s="119"/>
-      <c r="V17" s="119"/>
-      <c r="W17" s="119"/>
-      <c r="X17" s="119"/>
-      <c r="Y17" s="119"/>
-      <c r="Z17" s="119"/>
-      <c r="AA17" s="119"/>
-      <c r="AB17" s="119"/>
-      <c r="AC17" s="119"/>
-      <c r="AD17" s="119"/>
-      <c r="AE17" s="120"/>
-      <c r="AF17" s="115"/>
-      <c r="AG17" s="116"/>
-      <c r="AH17" s="116"/>
-      <c r="AI17" s="117"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="64"/>
+      <c r="P17" s="65"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="67"/>
+      <c r="S17" s="67"/>
+      <c r="T17" s="67"/>
+      <c r="U17" s="67"/>
+      <c r="V17" s="67"/>
+      <c r="W17" s="67"/>
+      <c r="X17" s="67"/>
+      <c r="Y17" s="67"/>
+      <c r="Z17" s="67"/>
+      <c r="AA17" s="67"/>
+      <c r="AB17" s="67"/>
+      <c r="AC17" s="67"/>
+      <c r="AD17" s="67"/>
+      <c r="AE17" s="68"/>
+      <c r="AF17" s="63"/>
+      <c r="AG17" s="64"/>
+      <c r="AH17" s="64"/>
+      <c r="AI17" s="65"/>
     </row>
     <row r="18" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="52"/>
-      <c r="B18" s="107"/>
-      <c r="C18" s="108"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="110"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="113"/>
-      <c r="I18" s="114"/>
-      <c r="J18" s="115"/>
-      <c r="K18" s="116"/>
-      <c r="L18" s="116"/>
-      <c r="M18" s="116"/>
-      <c r="N18" s="116"/>
-      <c r="O18" s="116"/>
-      <c r="P18" s="117"/>
-      <c r="Q18" s="118"/>
-      <c r="R18" s="119"/>
-      <c r="S18" s="119"/>
-      <c r="T18" s="119"/>
-      <c r="U18" s="119"/>
-      <c r="V18" s="119"/>
-      <c r="W18" s="119"/>
-      <c r="X18" s="119"/>
-      <c r="Y18" s="119"/>
-      <c r="Z18" s="119"/>
-      <c r="AA18" s="119"/>
-      <c r="AB18" s="119"/>
-      <c r="AC18" s="119"/>
-      <c r="AD18" s="119"/>
-      <c r="AE18" s="120"/>
-      <c r="AF18" s="115"/>
-      <c r="AG18" s="116"/>
-      <c r="AH18" s="116"/>
-      <c r="AI18" s="117"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="62"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="64"/>
+      <c r="O18" s="64"/>
+      <c r="P18" s="65"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="67"/>
+      <c r="S18" s="67"/>
+      <c r="T18" s="67"/>
+      <c r="U18" s="67"/>
+      <c r="V18" s="67"/>
+      <c r="W18" s="67"/>
+      <c r="X18" s="67"/>
+      <c r="Y18" s="67"/>
+      <c r="Z18" s="67"/>
+      <c r="AA18" s="67"/>
+      <c r="AB18" s="67"/>
+      <c r="AC18" s="67"/>
+      <c r="AD18" s="67"/>
+      <c r="AE18" s="68"/>
+      <c r="AF18" s="63"/>
+      <c r="AG18" s="64"/>
+      <c r="AH18" s="64"/>
+      <c r="AI18" s="65"/>
     </row>
     <row r="19" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="52"/>
-      <c r="B19" s="107"/>
-      <c r="C19" s="108"/>
-      <c r="D19" s="109"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="111"/>
-      <c r="G19" s="112"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="114"/>
-      <c r="J19" s="115"/>
-      <c r="K19" s="116"/>
-      <c r="L19" s="116"/>
-      <c r="M19" s="116"/>
-      <c r="N19" s="116"/>
-      <c r="O19" s="116"/>
-      <c r="P19" s="117"/>
-      <c r="Q19" s="118"/>
-      <c r="R19" s="119"/>
-      <c r="S19" s="119"/>
-      <c r="T19" s="119"/>
-      <c r="U19" s="119"/>
-      <c r="V19" s="119"/>
-      <c r="W19" s="119"/>
-      <c r="X19" s="119"/>
-      <c r="Y19" s="119"/>
-      <c r="Z19" s="119"/>
-      <c r="AA19" s="119"/>
-      <c r="AB19" s="119"/>
-      <c r="AC19" s="119"/>
-      <c r="AD19" s="119"/>
-      <c r="AE19" s="120"/>
-      <c r="AF19" s="115"/>
-      <c r="AG19" s="116"/>
-      <c r="AH19" s="116"/>
-      <c r="AI19" s="117"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="64"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="67"/>
+      <c r="S19" s="67"/>
+      <c r="T19" s="67"/>
+      <c r="U19" s="67"/>
+      <c r="V19" s="67"/>
+      <c r="W19" s="67"/>
+      <c r="X19" s="67"/>
+      <c r="Y19" s="67"/>
+      <c r="Z19" s="67"/>
+      <c r="AA19" s="67"/>
+      <c r="AB19" s="67"/>
+      <c r="AC19" s="67"/>
+      <c r="AD19" s="67"/>
+      <c r="AE19" s="68"/>
+      <c r="AF19" s="63"/>
+      <c r="AG19" s="64"/>
+      <c r="AH19" s="64"/>
+      <c r="AI19" s="65"/>
     </row>
     <row r="20" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="52"/>
-      <c r="B20" s="107"/>
-      <c r="C20" s="108"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="113"/>
-      <c r="I20" s="114"/>
-      <c r="J20" s="115"/>
-      <c r="K20" s="116"/>
-      <c r="L20" s="116"/>
-      <c r="M20" s="116"/>
-      <c r="N20" s="116"/>
-      <c r="O20" s="116"/>
-      <c r="P20" s="117"/>
-      <c r="Q20" s="118"/>
-      <c r="R20" s="119"/>
-      <c r="S20" s="119"/>
-      <c r="T20" s="119"/>
-      <c r="U20" s="119"/>
-      <c r="V20" s="119"/>
-      <c r="W20" s="119"/>
-      <c r="X20" s="119"/>
-      <c r="Y20" s="119"/>
-      <c r="Z20" s="119"/>
-      <c r="AA20" s="119"/>
-      <c r="AB20" s="119"/>
-      <c r="AC20" s="119"/>
-      <c r="AD20" s="119"/>
-      <c r="AE20" s="120"/>
-      <c r="AF20" s="115"/>
-      <c r="AG20" s="116"/>
-      <c r="AH20" s="116"/>
-      <c r="AI20" s="117"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="64"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="66"/>
+      <c r="R20" s="67"/>
+      <c r="S20" s="67"/>
+      <c r="T20" s="67"/>
+      <c r="U20" s="67"/>
+      <c r="V20" s="67"/>
+      <c r="W20" s="67"/>
+      <c r="X20" s="67"/>
+      <c r="Y20" s="67"/>
+      <c r="Z20" s="67"/>
+      <c r="AA20" s="67"/>
+      <c r="AB20" s="67"/>
+      <c r="AC20" s="67"/>
+      <c r="AD20" s="67"/>
+      <c r="AE20" s="68"/>
+      <c r="AF20" s="63"/>
+      <c r="AG20" s="64"/>
+      <c r="AH20" s="64"/>
+      <c r="AI20" s="65"/>
     </row>
     <row r="21" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="52"/>
-      <c r="B21" s="107"/>
-      <c r="C21" s="108"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="110"/>
-      <c r="F21" s="111"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="113"/>
-      <c r="I21" s="114"/>
-      <c r="J21" s="115"/>
-      <c r="K21" s="116"/>
-      <c r="L21" s="116"/>
-      <c r="M21" s="116"/>
-      <c r="N21" s="116"/>
-      <c r="O21" s="116"/>
-      <c r="P21" s="117"/>
-      <c r="Q21" s="118"/>
-      <c r="R21" s="119"/>
-      <c r="S21" s="119"/>
-      <c r="T21" s="119"/>
-      <c r="U21" s="119"/>
-      <c r="V21" s="119"/>
-      <c r="W21" s="119"/>
-      <c r="X21" s="119"/>
-      <c r="Y21" s="119"/>
-      <c r="Z21" s="119"/>
-      <c r="AA21" s="119"/>
-      <c r="AB21" s="119"/>
-      <c r="AC21" s="119"/>
-      <c r="AD21" s="119"/>
-      <c r="AE21" s="120"/>
-      <c r="AF21" s="115"/>
-      <c r="AG21" s="116"/>
-      <c r="AH21" s="116"/>
-      <c r="AI21" s="117"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="64"/>
+      <c r="P21" s="65"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="67"/>
+      <c r="S21" s="67"/>
+      <c r="T21" s="67"/>
+      <c r="U21" s="67"/>
+      <c r="V21" s="67"/>
+      <c r="W21" s="67"/>
+      <c r="X21" s="67"/>
+      <c r="Y21" s="67"/>
+      <c r="Z21" s="67"/>
+      <c r="AA21" s="67"/>
+      <c r="AB21" s="67"/>
+      <c r="AC21" s="67"/>
+      <c r="AD21" s="67"/>
+      <c r="AE21" s="68"/>
+      <c r="AF21" s="63"/>
+      <c r="AG21" s="64"/>
+      <c r="AH21" s="64"/>
+      <c r="AI21" s="65"/>
     </row>
     <row r="22" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="52"/>
-      <c r="B22" s="107"/>
-      <c r="C22" s="108"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="111"/>
-      <c r="G22" s="112"/>
-      <c r="H22" s="113"/>
-      <c r="I22" s="114"/>
-      <c r="J22" s="115"/>
-      <c r="K22" s="116"/>
-      <c r="L22" s="116"/>
-      <c r="M22" s="116"/>
-      <c r="N22" s="116"/>
-      <c r="O22" s="116"/>
-      <c r="P22" s="117"/>
-      <c r="Q22" s="118"/>
-      <c r="R22" s="119"/>
-      <c r="S22" s="119"/>
-      <c r="T22" s="119"/>
-      <c r="U22" s="119"/>
-      <c r="V22" s="119"/>
-      <c r="W22" s="119"/>
-      <c r="X22" s="119"/>
-      <c r="Y22" s="119"/>
-      <c r="Z22" s="119"/>
-      <c r="AA22" s="119"/>
-      <c r="AB22" s="119"/>
-      <c r="AC22" s="119"/>
-      <c r="AD22" s="119"/>
-      <c r="AE22" s="120"/>
-      <c r="AF22" s="115"/>
-      <c r="AG22" s="116"/>
-      <c r="AH22" s="116"/>
-      <c r="AI22" s="117"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="64"/>
+      <c r="P22" s="65"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="67"/>
+      <c r="S22" s="67"/>
+      <c r="T22" s="67"/>
+      <c r="U22" s="67"/>
+      <c r="V22" s="67"/>
+      <c r="W22" s="67"/>
+      <c r="X22" s="67"/>
+      <c r="Y22" s="67"/>
+      <c r="Z22" s="67"/>
+      <c r="AA22" s="67"/>
+      <c r="AB22" s="67"/>
+      <c r="AC22" s="67"/>
+      <c r="AD22" s="67"/>
+      <c r="AE22" s="68"/>
+      <c r="AF22" s="63"/>
+      <c r="AG22" s="64"/>
+      <c r="AH22" s="64"/>
+      <c r="AI22" s="65"/>
     </row>
     <row r="23" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="52"/>
-      <c r="B23" s="107"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="112"/>
-      <c r="H23" s="113"/>
-      <c r="I23" s="114"/>
-      <c r="J23" s="115"/>
-      <c r="K23" s="116"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="116"/>
-      <c r="N23" s="116"/>
-      <c r="O23" s="116"/>
-      <c r="P23" s="117"/>
-      <c r="Q23" s="118"/>
-      <c r="R23" s="119"/>
-      <c r="S23" s="119"/>
-      <c r="T23" s="119"/>
-      <c r="U23" s="119"/>
-      <c r="V23" s="119"/>
-      <c r="W23" s="119"/>
-      <c r="X23" s="119"/>
-      <c r="Y23" s="119"/>
-      <c r="Z23" s="119"/>
-      <c r="AA23" s="119"/>
-      <c r="AB23" s="119"/>
-      <c r="AC23" s="119"/>
-      <c r="AD23" s="119"/>
-      <c r="AE23" s="120"/>
-      <c r="AF23" s="115"/>
-      <c r="AG23" s="116"/>
-      <c r="AH23" s="116"/>
-      <c r="AI23" s="117"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="65"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="67"/>
+      <c r="S23" s="67"/>
+      <c r="T23" s="67"/>
+      <c r="U23" s="67"/>
+      <c r="V23" s="67"/>
+      <c r="W23" s="67"/>
+      <c r="X23" s="67"/>
+      <c r="Y23" s="67"/>
+      <c r="Z23" s="67"/>
+      <c r="AA23" s="67"/>
+      <c r="AB23" s="67"/>
+      <c r="AC23" s="67"/>
+      <c r="AD23" s="67"/>
+      <c r="AE23" s="68"/>
+      <c r="AF23" s="63"/>
+      <c r="AG23" s="64"/>
+      <c r="AH23" s="64"/>
+      <c r="AI23" s="65"/>
     </row>
     <row r="24" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="52"/>
-      <c r="B24" s="107"/>
-      <c r="C24" s="108"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="110"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="112"/>
-      <c r="H24" s="113"/>
-      <c r="I24" s="114"/>
-      <c r="J24" s="115"/>
-      <c r="K24" s="116"/>
-      <c r="L24" s="116"/>
-      <c r="M24" s="116"/>
-      <c r="N24" s="116"/>
-      <c r="O24" s="116"/>
-      <c r="P24" s="117"/>
-      <c r="Q24" s="118"/>
-      <c r="R24" s="119"/>
-      <c r="S24" s="119"/>
-      <c r="T24" s="119"/>
-      <c r="U24" s="119"/>
-      <c r="V24" s="119"/>
-      <c r="W24" s="119"/>
-      <c r="X24" s="119"/>
-      <c r="Y24" s="119"/>
-      <c r="Z24" s="119"/>
-      <c r="AA24" s="119"/>
-      <c r="AB24" s="119"/>
-      <c r="AC24" s="119"/>
-      <c r="AD24" s="119"/>
-      <c r="AE24" s="120"/>
-      <c r="AF24" s="115"/>
-      <c r="AG24" s="116"/>
-      <c r="AH24" s="116"/>
-      <c r="AI24" s="117"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="65"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="67"/>
+      <c r="S24" s="67"/>
+      <c r="T24" s="67"/>
+      <c r="U24" s="67"/>
+      <c r="V24" s="67"/>
+      <c r="W24" s="67"/>
+      <c r="X24" s="67"/>
+      <c r="Y24" s="67"/>
+      <c r="Z24" s="67"/>
+      <c r="AA24" s="67"/>
+      <c r="AB24" s="67"/>
+      <c r="AC24" s="67"/>
+      <c r="AD24" s="67"/>
+      <c r="AE24" s="68"/>
+      <c r="AF24" s="63"/>
+      <c r="AG24" s="64"/>
+      <c r="AH24" s="64"/>
+      <c r="AI24" s="65"/>
     </row>
     <row r="25" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="52"/>
-      <c r="B25" s="107"/>
-      <c r="C25" s="108"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="110"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="112"/>
-      <c r="H25" s="113"/>
-      <c r="I25" s="114"/>
-      <c r="J25" s="115"/>
-      <c r="K25" s="116"/>
-      <c r="L25" s="116"/>
-      <c r="M25" s="116"/>
-      <c r="N25" s="116"/>
-      <c r="O25" s="116"/>
-      <c r="P25" s="117"/>
-      <c r="Q25" s="118"/>
-      <c r="R25" s="119"/>
-      <c r="S25" s="119"/>
-      <c r="T25" s="119"/>
-      <c r="U25" s="119"/>
-      <c r="V25" s="119"/>
-      <c r="W25" s="119"/>
-      <c r="X25" s="119"/>
-      <c r="Y25" s="119"/>
-      <c r="Z25" s="119"/>
-      <c r="AA25" s="119"/>
-      <c r="AB25" s="119"/>
-      <c r="AC25" s="119"/>
-      <c r="AD25" s="119"/>
-      <c r="AE25" s="120"/>
-      <c r="AF25" s="115"/>
-      <c r="AG25" s="116"/>
-      <c r="AH25" s="116"/>
-      <c r="AI25" s="117"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="66"/>
+      <c r="R25" s="67"/>
+      <c r="S25" s="67"/>
+      <c r="T25" s="67"/>
+      <c r="U25" s="67"/>
+      <c r="V25" s="67"/>
+      <c r="W25" s="67"/>
+      <c r="X25" s="67"/>
+      <c r="Y25" s="67"/>
+      <c r="Z25" s="67"/>
+      <c r="AA25" s="67"/>
+      <c r="AB25" s="67"/>
+      <c r="AC25" s="67"/>
+      <c r="AD25" s="67"/>
+      <c r="AE25" s="68"/>
+      <c r="AF25" s="63"/>
+      <c r="AG25" s="64"/>
+      <c r="AH25" s="64"/>
+      <c r="AI25" s="65"/>
     </row>
     <row r="26" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="52"/>
-      <c r="B26" s="107"/>
-      <c r="C26" s="108"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="110"/>
-      <c r="F26" s="111"/>
-      <c r="G26" s="112"/>
-      <c r="H26" s="113"/>
-      <c r="I26" s="114"/>
-      <c r="J26" s="115"/>
-      <c r="K26" s="116"/>
-      <c r="L26" s="116"/>
-      <c r="M26" s="116"/>
-      <c r="N26" s="116"/>
-      <c r="O26" s="116"/>
-      <c r="P26" s="117"/>
-      <c r="Q26" s="118"/>
-      <c r="R26" s="119"/>
-      <c r="S26" s="119"/>
-      <c r="T26" s="119"/>
-      <c r="U26" s="119"/>
-      <c r="V26" s="119"/>
-      <c r="W26" s="119"/>
-      <c r="X26" s="119"/>
-      <c r="Y26" s="119"/>
-      <c r="Z26" s="119"/>
-      <c r="AA26" s="119"/>
-      <c r="AB26" s="119"/>
-      <c r="AC26" s="119"/>
-      <c r="AD26" s="119"/>
-      <c r="AE26" s="120"/>
-      <c r="AF26" s="115"/>
-      <c r="AG26" s="116"/>
-      <c r="AH26" s="116"/>
-      <c r="AI26" s="117"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="64"/>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="66"/>
+      <c r="R26" s="67"/>
+      <c r="S26" s="67"/>
+      <c r="T26" s="67"/>
+      <c r="U26" s="67"/>
+      <c r="V26" s="67"/>
+      <c r="W26" s="67"/>
+      <c r="X26" s="67"/>
+      <c r="Y26" s="67"/>
+      <c r="Z26" s="67"/>
+      <c r="AA26" s="67"/>
+      <c r="AB26" s="67"/>
+      <c r="AC26" s="67"/>
+      <c r="AD26" s="67"/>
+      <c r="AE26" s="68"/>
+      <c r="AF26" s="63"/>
+      <c r="AG26" s="64"/>
+      <c r="AH26" s="64"/>
+      <c r="AI26" s="65"/>
     </row>
     <row r="27" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="52"/>
-      <c r="B27" s="107"/>
-      <c r="C27" s="108"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="112"/>
-      <c r="H27" s="113"/>
-      <c r="I27" s="114"/>
-      <c r="J27" s="115"/>
-      <c r="K27" s="116"/>
-      <c r="L27" s="116"/>
-      <c r="M27" s="116"/>
-      <c r="N27" s="116"/>
-      <c r="O27" s="116"/>
-      <c r="P27" s="117"/>
-      <c r="Q27" s="118"/>
-      <c r="R27" s="119"/>
-      <c r="S27" s="119"/>
-      <c r="T27" s="119"/>
-      <c r="U27" s="119"/>
-      <c r="V27" s="119"/>
-      <c r="W27" s="119"/>
-      <c r="X27" s="119"/>
-      <c r="Y27" s="119"/>
-      <c r="Z27" s="119"/>
-      <c r="AA27" s="119"/>
-      <c r="AB27" s="119"/>
-      <c r="AC27" s="119"/>
-      <c r="AD27" s="119"/>
-      <c r="AE27" s="120"/>
-      <c r="AF27" s="115"/>
-      <c r="AG27" s="116"/>
-      <c r="AH27" s="116"/>
-      <c r="AI27" s="117"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="64"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="66"/>
+      <c r="R27" s="67"/>
+      <c r="S27" s="67"/>
+      <c r="T27" s="67"/>
+      <c r="U27" s="67"/>
+      <c r="V27" s="67"/>
+      <c r="W27" s="67"/>
+      <c r="X27" s="67"/>
+      <c r="Y27" s="67"/>
+      <c r="Z27" s="67"/>
+      <c r="AA27" s="67"/>
+      <c r="AB27" s="67"/>
+      <c r="AC27" s="67"/>
+      <c r="AD27" s="67"/>
+      <c r="AE27" s="68"/>
+      <c r="AF27" s="63"/>
+      <c r="AG27" s="64"/>
+      <c r="AH27" s="64"/>
+      <c r="AI27" s="65"/>
     </row>
     <row r="28" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="52"/>
-      <c r="B28" s="107"/>
-      <c r="C28" s="108"/>
-      <c r="D28" s="109"/>
-      <c r="E28" s="110"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="112"/>
-      <c r="H28" s="113"/>
-      <c r="I28" s="114"/>
-      <c r="J28" s="115"/>
-      <c r="K28" s="116"/>
-      <c r="L28" s="116"/>
-      <c r="M28" s="116"/>
-      <c r="N28" s="116"/>
-      <c r="O28" s="116"/>
-      <c r="P28" s="117"/>
-      <c r="Q28" s="118"/>
-      <c r="R28" s="119"/>
-      <c r="S28" s="119"/>
-      <c r="T28" s="119"/>
-      <c r="U28" s="119"/>
-      <c r="V28" s="119"/>
-      <c r="W28" s="119"/>
-      <c r="X28" s="119"/>
-      <c r="Y28" s="119"/>
-      <c r="Z28" s="119"/>
-      <c r="AA28" s="119"/>
-      <c r="AB28" s="119"/>
-      <c r="AC28" s="119"/>
-      <c r="AD28" s="119"/>
-      <c r="AE28" s="120"/>
-      <c r="AF28" s="115"/>
-      <c r="AG28" s="116"/>
-      <c r="AH28" s="116"/>
-      <c r="AI28" s="117"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="63"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="64"/>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="67"/>
+      <c r="S28" s="67"/>
+      <c r="T28" s="67"/>
+      <c r="U28" s="67"/>
+      <c r="V28" s="67"/>
+      <c r="W28" s="67"/>
+      <c r="X28" s="67"/>
+      <c r="Y28" s="67"/>
+      <c r="Z28" s="67"/>
+      <c r="AA28" s="67"/>
+      <c r="AB28" s="67"/>
+      <c r="AC28" s="67"/>
+      <c r="AD28" s="67"/>
+      <c r="AE28" s="68"/>
+      <c r="AF28" s="63"/>
+      <c r="AG28" s="64"/>
+      <c r="AH28" s="64"/>
+      <c r="AI28" s="65"/>
     </row>
     <row r="29" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="52"/>
-      <c r="B29" s="107"/>
-      <c r="C29" s="108"/>
-      <c r="D29" s="109"/>
-      <c r="E29" s="110"/>
-      <c r="F29" s="111"/>
-      <c r="G29" s="112"/>
-      <c r="H29" s="113"/>
-      <c r="I29" s="114"/>
-      <c r="J29" s="115"/>
-      <c r="K29" s="116"/>
-      <c r="L29" s="116"/>
-      <c r="M29" s="116"/>
-      <c r="N29" s="116"/>
-      <c r="O29" s="116"/>
-      <c r="P29" s="117"/>
-      <c r="Q29" s="118"/>
-      <c r="R29" s="119"/>
-      <c r="S29" s="119"/>
-      <c r="T29" s="119"/>
-      <c r="U29" s="119"/>
-      <c r="V29" s="119"/>
-      <c r="W29" s="119"/>
-      <c r="X29" s="119"/>
-      <c r="Y29" s="119"/>
-      <c r="Z29" s="119"/>
-      <c r="AA29" s="119"/>
-      <c r="AB29" s="119"/>
-      <c r="AC29" s="119"/>
-      <c r="AD29" s="119"/>
-      <c r="AE29" s="120"/>
-      <c r="AF29" s="115"/>
-      <c r="AG29" s="116"/>
-      <c r="AH29" s="116"/>
-      <c r="AI29" s="117"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="65"/>
+      <c r="Q29" s="66"/>
+      <c r="R29" s="67"/>
+      <c r="S29" s="67"/>
+      <c r="T29" s="67"/>
+      <c r="U29" s="67"/>
+      <c r="V29" s="67"/>
+      <c r="W29" s="67"/>
+      <c r="X29" s="67"/>
+      <c r="Y29" s="67"/>
+      <c r="Z29" s="67"/>
+      <c r="AA29" s="67"/>
+      <c r="AB29" s="67"/>
+      <c r="AC29" s="67"/>
+      <c r="AD29" s="67"/>
+      <c r="AE29" s="68"/>
+      <c r="AF29" s="63"/>
+      <c r="AG29" s="64"/>
+      <c r="AH29" s="64"/>
+      <c r="AI29" s="65"/>
     </row>
     <row r="30" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="52"/>
-      <c r="B30" s="107"/>
-      <c r="C30" s="108"/>
-      <c r="D30" s="109"/>
-      <c r="E30" s="110"/>
-      <c r="F30" s="111"/>
-      <c r="G30" s="112"/>
-      <c r="H30" s="113"/>
-      <c r="I30" s="114"/>
-      <c r="J30" s="115"/>
-      <c r="K30" s="116"/>
-      <c r="L30" s="116"/>
-      <c r="M30" s="116"/>
-      <c r="N30" s="116"/>
-      <c r="O30" s="116"/>
-      <c r="P30" s="117"/>
-      <c r="Q30" s="118"/>
-      <c r="R30" s="119"/>
-      <c r="S30" s="119"/>
-      <c r="T30" s="119"/>
-      <c r="U30" s="119"/>
-      <c r="V30" s="119"/>
-      <c r="W30" s="119"/>
-      <c r="X30" s="119"/>
-      <c r="Y30" s="119"/>
-      <c r="Z30" s="119"/>
-      <c r="AA30" s="119"/>
-      <c r="AB30" s="119"/>
-      <c r="AC30" s="119"/>
-      <c r="AD30" s="119"/>
-      <c r="AE30" s="120"/>
-      <c r="AF30" s="115"/>
-      <c r="AG30" s="116"/>
-      <c r="AH30" s="116"/>
-      <c r="AI30" s="117"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="67"/>
+      <c r="S30" s="67"/>
+      <c r="T30" s="67"/>
+      <c r="U30" s="67"/>
+      <c r="V30" s="67"/>
+      <c r="W30" s="67"/>
+      <c r="X30" s="67"/>
+      <c r="Y30" s="67"/>
+      <c r="Z30" s="67"/>
+      <c r="AA30" s="67"/>
+      <c r="AB30" s="67"/>
+      <c r="AC30" s="67"/>
+      <c r="AD30" s="67"/>
+      <c r="AE30" s="68"/>
+      <c r="AF30" s="63"/>
+      <c r="AG30" s="64"/>
+      <c r="AH30" s="64"/>
+      <c r="AI30" s="65"/>
     </row>
     <row r="31" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="52"/>
-      <c r="B31" s="107"/>
-      <c r="C31" s="108"/>
-      <c r="D31" s="109"/>
-      <c r="E31" s="110"/>
-      <c r="F31" s="111"/>
-      <c r="G31" s="112"/>
-      <c r="H31" s="113"/>
-      <c r="I31" s="114"/>
-      <c r="J31" s="115"/>
-      <c r="K31" s="116"/>
-      <c r="L31" s="116"/>
-      <c r="M31" s="116"/>
-      <c r="N31" s="116"/>
-      <c r="O31" s="116"/>
-      <c r="P31" s="117"/>
-      <c r="Q31" s="118"/>
-      <c r="R31" s="119"/>
-      <c r="S31" s="119"/>
-      <c r="T31" s="119"/>
-      <c r="U31" s="119"/>
-      <c r="V31" s="119"/>
-      <c r="W31" s="119"/>
-      <c r="X31" s="119"/>
-      <c r="Y31" s="119"/>
-      <c r="Z31" s="119"/>
-      <c r="AA31" s="119"/>
-      <c r="AB31" s="119"/>
-      <c r="AC31" s="119"/>
-      <c r="AD31" s="119"/>
-      <c r="AE31" s="120"/>
-      <c r="AF31" s="115"/>
-      <c r="AG31" s="116"/>
-      <c r="AH31" s="116"/>
-      <c r="AI31" s="117"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="63"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="64"/>
+      <c r="O31" s="64"/>
+      <c r="P31" s="65"/>
+      <c r="Q31" s="66"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="67"/>
+      <c r="T31" s="67"/>
+      <c r="U31" s="67"/>
+      <c r="V31" s="67"/>
+      <c r="W31" s="67"/>
+      <c r="X31" s="67"/>
+      <c r="Y31" s="67"/>
+      <c r="Z31" s="67"/>
+      <c r="AA31" s="67"/>
+      <c r="AB31" s="67"/>
+      <c r="AC31" s="67"/>
+      <c r="AD31" s="67"/>
+      <c r="AE31" s="68"/>
+      <c r="AF31" s="63"/>
+      <c r="AG31" s="64"/>
+      <c r="AH31" s="64"/>
+      <c r="AI31" s="65"/>
     </row>
     <row r="32" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="52"/>
-      <c r="B32" s="107"/>
-      <c r="C32" s="108"/>
-      <c r="D32" s="109"/>
-      <c r="E32" s="110"/>
-      <c r="F32" s="111"/>
-      <c r="G32" s="112"/>
-      <c r="H32" s="113"/>
-      <c r="I32" s="114"/>
-      <c r="J32" s="115"/>
-      <c r="K32" s="121"/>
-      <c r="L32" s="116"/>
-      <c r="M32" s="116"/>
-      <c r="N32" s="116"/>
-      <c r="O32" s="116"/>
-      <c r="P32" s="117"/>
-      <c r="Q32" s="118"/>
-      <c r="R32" s="119"/>
-      <c r="S32" s="119"/>
-      <c r="T32" s="119"/>
-      <c r="U32" s="119"/>
-      <c r="V32" s="119"/>
-      <c r="W32" s="119"/>
-      <c r="X32" s="119"/>
-      <c r="Y32" s="119"/>
-      <c r="Z32" s="119"/>
-      <c r="AA32" s="119"/>
-      <c r="AB32" s="119"/>
-      <c r="AC32" s="119"/>
-      <c r="AD32" s="119"/>
-      <c r="AE32" s="120"/>
-      <c r="AF32" s="115"/>
-      <c r="AG32" s="116"/>
-      <c r="AH32" s="116"/>
-      <c r="AI32" s="117"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="66"/>
+      <c r="R32" s="67"/>
+      <c r="S32" s="67"/>
+      <c r="T32" s="67"/>
+      <c r="U32" s="67"/>
+      <c r="V32" s="67"/>
+      <c r="W32" s="67"/>
+      <c r="X32" s="67"/>
+      <c r="Y32" s="67"/>
+      <c r="Z32" s="67"/>
+      <c r="AA32" s="67"/>
+      <c r="AB32" s="67"/>
+      <c r="AC32" s="67"/>
+      <c r="AD32" s="67"/>
+      <c r="AE32" s="68"/>
+      <c r="AF32" s="63"/>
+      <c r="AG32" s="64"/>
+      <c r="AH32" s="64"/>
+      <c r="AI32" s="65"/>
     </row>
     <row r="33" spans="1:35" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="52"/>
-      <c r="B33" s="107"/>
-      <c r="C33" s="108"/>
-      <c r="D33" s="109"/>
-      <c r="E33" s="110"/>
-      <c r="F33" s="111"/>
-      <c r="G33" s="112"/>
-      <c r="H33" s="113"/>
-      <c r="I33" s="114"/>
-      <c r="J33" s="115"/>
-      <c r="K33" s="116"/>
-      <c r="L33" s="116"/>
-      <c r="M33" s="116"/>
-      <c r="N33" s="116"/>
-      <c r="O33" s="116"/>
-      <c r="P33" s="117"/>
-      <c r="Q33" s="118"/>
-      <c r="R33" s="119"/>
-      <c r="S33" s="119"/>
-      <c r="T33" s="119"/>
-      <c r="U33" s="119"/>
-      <c r="V33" s="119"/>
-      <c r="W33" s="119"/>
-      <c r="X33" s="119"/>
-      <c r="Y33" s="119"/>
-      <c r="Z33" s="119"/>
-      <c r="AA33" s="119"/>
-      <c r="AB33" s="119"/>
-      <c r="AC33" s="119"/>
-      <c r="AD33" s="119"/>
-      <c r="AE33" s="120"/>
-      <c r="AF33" s="115"/>
-      <c r="AG33" s="116"/>
-      <c r="AH33" s="116"/>
-      <c r="AI33" s="117"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="64"/>
+      <c r="N33" s="64"/>
+      <c r="O33" s="64"/>
+      <c r="P33" s="65"/>
+      <c r="Q33" s="66"/>
+      <c r="R33" s="67"/>
+      <c r="S33" s="67"/>
+      <c r="T33" s="67"/>
+      <c r="U33" s="67"/>
+      <c r="V33" s="67"/>
+      <c r="W33" s="67"/>
+      <c r="X33" s="67"/>
+      <c r="Y33" s="67"/>
+      <c r="Z33" s="67"/>
+      <c r="AA33" s="67"/>
+      <c r="AB33" s="67"/>
+      <c r="AC33" s="67"/>
+      <c r="AD33" s="67"/>
+      <c r="AE33" s="68"/>
+      <c r="AF33" s="63"/>
+      <c r="AG33" s="64"/>
+      <c r="AH33" s="64"/>
+      <c r="AI33" s="65"/>
     </row>
     <row r="34" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="K34" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="179">
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:P33"/>
-    <mergeCell ref="Q33:AE33"/>
-    <mergeCell ref="AF33:AI33"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:P32"/>
-    <mergeCell ref="Q32:AE32"/>
-    <mergeCell ref="AF32:AI32"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="Q31:AE31"/>
-    <mergeCell ref="AF31:AI31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:P30"/>
-    <mergeCell ref="Q30:AE30"/>
-    <mergeCell ref="AF30:AI30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:P29"/>
-    <mergeCell ref="Q29:AE29"/>
-    <mergeCell ref="AF29:AI29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:P28"/>
-    <mergeCell ref="Q28:AE28"/>
-    <mergeCell ref="AF28:AI28"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:P27"/>
-    <mergeCell ref="Q27:AE27"/>
-    <mergeCell ref="AF27:AI27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:P26"/>
-    <mergeCell ref="Q26:AE26"/>
-    <mergeCell ref="AF26:AI26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:P25"/>
-    <mergeCell ref="Q25:AE25"/>
-    <mergeCell ref="AF25:AI25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:P24"/>
-    <mergeCell ref="Q24:AE24"/>
-    <mergeCell ref="AF24:AI24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:P23"/>
-    <mergeCell ref="Q23:AE23"/>
-    <mergeCell ref="AF23:AI23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:P22"/>
-    <mergeCell ref="Q22:AE22"/>
-    <mergeCell ref="AF22:AI22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:P21"/>
-    <mergeCell ref="Q21:AE21"/>
-    <mergeCell ref="AF21:AI21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:P20"/>
-    <mergeCell ref="Q20:AE20"/>
-    <mergeCell ref="AF20:AI20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:P19"/>
-    <mergeCell ref="Q19:AE19"/>
-    <mergeCell ref="AF19:AI19"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:P18"/>
-    <mergeCell ref="Q18:AE18"/>
-    <mergeCell ref="AF18:AI18"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:P17"/>
-    <mergeCell ref="Q17:AE17"/>
-    <mergeCell ref="AF17:AI17"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:P16"/>
-    <mergeCell ref="Q16:AE16"/>
-    <mergeCell ref="AF16:AI16"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:P15"/>
-    <mergeCell ref="Q15:AE15"/>
-    <mergeCell ref="AF15:AI15"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:P14"/>
-    <mergeCell ref="Q14:AE14"/>
-    <mergeCell ref="AF14:AI14"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:P13"/>
-    <mergeCell ref="Q13:AE13"/>
-    <mergeCell ref="AF13:AI13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:P12"/>
-    <mergeCell ref="Q12:AE12"/>
-    <mergeCell ref="AF12:AI12"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:P7"/>
-    <mergeCell ref="Q7:AE7"/>
-    <mergeCell ref="AF7:AI7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:P11"/>
-    <mergeCell ref="Q11:AE11"/>
-    <mergeCell ref="AF11:AI11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="J10:P10"/>
-    <mergeCell ref="Q10:AE10"/>
-    <mergeCell ref="AF10:AI10"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:P9"/>
-    <mergeCell ref="Q9:AE9"/>
-    <mergeCell ref="AF9:AI9"/>
     <mergeCell ref="S1:Z3"/>
     <mergeCell ref="AG3:AI3"/>
     <mergeCell ref="B8:C8"/>
@@ -4452,6 +4297,161 @@
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AC3:AF3"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:P7"/>
+    <mergeCell ref="Q7:AE7"/>
+    <mergeCell ref="AF7:AI7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:P11"/>
+    <mergeCell ref="Q11:AE11"/>
+    <mergeCell ref="AF11:AI11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:P10"/>
+    <mergeCell ref="Q10:AE10"/>
+    <mergeCell ref="AF10:AI10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:P9"/>
+    <mergeCell ref="Q9:AE9"/>
+    <mergeCell ref="AF9:AI9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:P13"/>
+    <mergeCell ref="Q13:AE13"/>
+    <mergeCell ref="AF13:AI13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:P12"/>
+    <mergeCell ref="Q12:AE12"/>
+    <mergeCell ref="AF12:AI12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:P15"/>
+    <mergeCell ref="Q15:AE15"/>
+    <mergeCell ref="AF15:AI15"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:P14"/>
+    <mergeCell ref="Q14:AE14"/>
+    <mergeCell ref="AF14:AI14"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:P17"/>
+    <mergeCell ref="Q17:AE17"/>
+    <mergeCell ref="AF17:AI17"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:P16"/>
+    <mergeCell ref="Q16:AE16"/>
+    <mergeCell ref="AF16:AI16"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:P19"/>
+    <mergeCell ref="Q19:AE19"/>
+    <mergeCell ref="AF19:AI19"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:P18"/>
+    <mergeCell ref="Q18:AE18"/>
+    <mergeCell ref="AF18:AI18"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:P21"/>
+    <mergeCell ref="Q21:AE21"/>
+    <mergeCell ref="AF21:AI21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:P20"/>
+    <mergeCell ref="Q20:AE20"/>
+    <mergeCell ref="AF20:AI20"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:P23"/>
+    <mergeCell ref="Q23:AE23"/>
+    <mergeCell ref="AF23:AI23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:P22"/>
+    <mergeCell ref="Q22:AE22"/>
+    <mergeCell ref="AF22:AI22"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:P25"/>
+    <mergeCell ref="Q25:AE25"/>
+    <mergeCell ref="AF25:AI25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:P24"/>
+    <mergeCell ref="Q24:AE24"/>
+    <mergeCell ref="AF24:AI24"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:P27"/>
+    <mergeCell ref="Q27:AE27"/>
+    <mergeCell ref="AF27:AI27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:P26"/>
+    <mergeCell ref="Q26:AE26"/>
+    <mergeCell ref="AF26:AI26"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:P29"/>
+    <mergeCell ref="Q29:AE29"/>
+    <mergeCell ref="AF29:AI29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:P28"/>
+    <mergeCell ref="Q28:AE28"/>
+    <mergeCell ref="AF28:AI28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="Q31:AE31"/>
+    <mergeCell ref="AF31:AI31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:P30"/>
+    <mergeCell ref="Q30:AE30"/>
+    <mergeCell ref="AF30:AI30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:P33"/>
+    <mergeCell ref="Q33:AE33"/>
+    <mergeCell ref="AF33:AI33"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:P32"/>
+    <mergeCell ref="Q32:AE32"/>
+    <mergeCell ref="AF32:AI32"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <printOptions horizontalCentered="1"/>
@@ -4468,7 +4468,7 @@
   <dimension ref="A1:AI49"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4611,159 +4611,159 @@
         <f ca="1">IF(INDIRECT("'Revision history'!A1")&lt;&gt;"",INDIRECT("'Revision history'!A1"),"")</f>
         <v>Project name</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="84" t="str">
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="102" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E1")&lt;&gt;"",INDIRECT("'Revision history'!E1"),"")</f>
         <v>Sample Project</v>
       </c>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="128" t="str">
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="125" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!O1")&lt;&gt;"",INDIRECT("'Revision history'!O1"),"")</f>
         <v>Deliverable name</v>
       </c>
-      <c r="P1" s="129"/>
-      <c r="Q1" s="129"/>
-      <c r="R1" s="130"/>
-      <c r="S1" s="55" t="str">
+      <c r="P1" s="126"/>
+      <c r="Q1" s="126"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="73" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!S1")&lt;&gt;"",INDIRECT("'Revision history'!S1"),"")</f>
         <v>Web Service API List</v>
       </c>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="57"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="75"/>
       <c r="AA1" s="122" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA1")&lt;&gt;"",INDIRECT("'Revision history'!AA1"),"")</f>
         <v>Prepared by</v>
       </c>
-      <c r="AB1" s="123"/>
-      <c r="AC1" s="99" t="str">
+      <c r="AB1" s="124"/>
+      <c r="AC1" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC1")&lt;&gt;"",INDIRECT("'Revision history'!AC1"),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD1" s="100"/>
-      <c r="AE1" s="100"/>
-      <c r="AF1" s="101"/>
-      <c r="AG1" s="124">
+      <c r="AD1" s="118"/>
+      <c r="AE1" s="118"/>
+      <c r="AF1" s="119"/>
+      <c r="AG1" s="134">
         <f ca="1">IF(INDIRECT("'Revision history'!AG1")&lt;&gt;"",INDIRECT("'Revision history'!AG1"),"")</f>
         <v>43404</v>
       </c>
-      <c r="AH1" s="125"/>
-      <c r="AI1" s="126"/>
+      <c r="AH1" s="135"/>
+      <c r="AI1" s="136"/>
     </row>
     <row r="2" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="122" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A2")&lt;&gt;"",INDIRECT("'Revision history'!A2"),"")</f>
         <v>System name</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="84" t="str">
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="102" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E2")&lt;&gt;"",INDIRECT("'Revision history'!E2"),"")</f>
         <v>Sample System</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="131"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="132"/>
-      <c r="R2" s="133"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="60"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="128"/>
+      <c r="P2" s="129"/>
+      <c r="Q2" s="129"/>
+      <c r="R2" s="130"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
+      <c r="X2" s="77"/>
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="78"/>
       <c r="AA2" s="122" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA2")&lt;&gt;"",INDIRECT("'Revision history'!AA2"),"")</f>
         <v>Changes</v>
       </c>
-      <c r="AB2" s="123"/>
-      <c r="AC2" s="99" t="str">
+      <c r="AB2" s="124"/>
+      <c r="AC2" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC2")&lt;&gt;"",INDIRECT("'Revision history'!AC2"),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD2" s="100"/>
-      <c r="AE2" s="100"/>
-      <c r="AF2" s="101"/>
-      <c r="AG2" s="124">
+      <c r="AD2" s="118"/>
+      <c r="AE2" s="118"/>
+      <c r="AF2" s="119"/>
+      <c r="AG2" s="134">
         <f ca="1">IF(INDIRECT("'Revision history'!AG2")&lt;&gt;"",INDIRECT("'Revision history'!AG2"),"")</f>
         <v>44833</v>
       </c>
-      <c r="AH2" s="125"/>
-      <c r="AI2" s="126"/>
+      <c r="AH2" s="135"/>
+      <c r="AI2" s="136"/>
     </row>
     <row r="3" spans="1:35" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="122" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A3")&lt;&gt;"",INDIRECT("'Revision history'!A3"),"")</f>
         <v>Sub-system name</v>
       </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="84" t="str">
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="102" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E3")&lt;&gt;"",INDIRECT("'Revision history'!E3"),"")</f>
         <v>Client Management System</v>
       </c>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="136"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="62"/>
-      <c r="U3" s="62"/>
-      <c r="V3" s="62"/>
-      <c r="W3" s="62"/>
-      <c r="X3" s="62"/>
-      <c r="Y3" s="62"/>
-      <c r="Z3" s="63"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="132"/>
+      <c r="Q3" s="132"/>
+      <c r="R3" s="133"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="81"/>
       <c r="AA3" s="122"/>
-      <c r="AB3" s="123"/>
-      <c r="AC3" s="99" t="str">
+      <c r="AB3" s="124"/>
+      <c r="AC3" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC3")&lt;&gt;"",INDIRECT("'Revision history'!AC3"),"")</f>
         <v/>
       </c>
-      <c r="AD3" s="100"/>
-      <c r="AE3" s="100"/>
-      <c r="AF3" s="101"/>
-      <c r="AG3" s="124" t="str">
+      <c r="AD3" s="118"/>
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="119"/>
+      <c r="AG3" s="134" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG3")&lt;&gt;"",INDIRECT("'Revision history'!AG3"),"")</f>
         <v/>
       </c>
-      <c r="AH3" s="125"/>
-      <c r="AI3" s="126"/>
+      <c r="AH3" s="135"/>
+      <c r="AI3" s="136"/>
     </row>
     <row r="4" spans="1:35" s="28" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26"/>
@@ -6040,14 +6040,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="S1:Z3"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:N1"/>
-    <mergeCell ref="O1:R3"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:N2"/>
-    <mergeCell ref="E3:N3"/>
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AC3:AF3"/>
     <mergeCell ref="AG3:AI3"/>
@@ -6057,6 +6049,14 @@
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="AC2:AF2"/>
     <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="S1:Z3"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:N1"/>
+    <mergeCell ref="O1:R3"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:N2"/>
+    <mergeCell ref="E3:N3"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <printOptions horizontalCentered="1"/>
@@ -6090,159 +6090,159 @@
         <f ca="1">IF(INDIRECT("'Revision history'!A1")&lt;&gt;"",INDIRECT("'Revision history'!A1"),"")</f>
         <v>Project name</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="84" t="str">
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="102" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E1")&lt;&gt;"",INDIRECT("'Revision history'!E1"),"")</f>
         <v>Sample Project</v>
       </c>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="128" t="str">
+      <c r="F1" s="103"/>
+      <c r="G1" s="103"/>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="125" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!O1")&lt;&gt;"",INDIRECT("'Revision history'!O1"),"")</f>
         <v>Deliverable name</v>
       </c>
-      <c r="P1" s="129"/>
-      <c r="Q1" s="129"/>
-      <c r="R1" s="130"/>
-      <c r="S1" s="55" t="str">
+      <c r="P1" s="126"/>
+      <c r="Q1" s="126"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="73" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!S1")&lt;&gt;"",INDIRECT("'Revision history'!S1"),"")</f>
         <v>Web Service API List</v>
       </c>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="57"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="75"/>
       <c r="AA1" s="122" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA1")&lt;&gt;"",INDIRECT("'Revision history'!AA1"),"")</f>
         <v>Prepared by</v>
       </c>
-      <c r="AB1" s="123"/>
-      <c r="AC1" s="99" t="str">
+      <c r="AB1" s="124"/>
+      <c r="AC1" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC1")&lt;&gt;"",INDIRECT("'Revision history'!AC1"),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD1" s="100"/>
-      <c r="AE1" s="100"/>
-      <c r="AF1" s="101"/>
-      <c r="AG1" s="124">
+      <c r="AD1" s="118"/>
+      <c r="AE1" s="118"/>
+      <c r="AF1" s="119"/>
+      <c r="AG1" s="134">
         <f ca="1">IF(INDIRECT("'Revision history'!AG1")&lt;&gt;"",INDIRECT("'Revision history'!AG1"),"")</f>
         <v>43404</v>
       </c>
-      <c r="AH1" s="125"/>
-      <c r="AI1" s="126"/>
+      <c r="AH1" s="135"/>
+      <c r="AI1" s="136"/>
     </row>
     <row r="2" spans="1:58" s="19" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="122" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A2")&lt;&gt;"",INDIRECT("'Revision history'!A2"),"")</f>
         <v>System name</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="84" t="str">
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="102" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E2")&lt;&gt;"",INDIRECT("'Revision history'!E2"),"")</f>
         <v>Sample System</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="131"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="132"/>
-      <c r="R2" s="133"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="60"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="128"/>
+      <c r="P2" s="129"/>
+      <c r="Q2" s="129"/>
+      <c r="R2" s="130"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
+      <c r="X2" s="77"/>
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="78"/>
       <c r="AA2" s="122" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AA2")&lt;&gt;"",INDIRECT("'Revision history'!AA2"),"")</f>
         <v>Changes</v>
       </c>
-      <c r="AB2" s="123"/>
-      <c r="AC2" s="99" t="str">
+      <c r="AB2" s="124"/>
+      <c r="AC2" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC2")&lt;&gt;"",INDIRECT("'Revision history'!AC2"),"")</f>
         <v>TIS</v>
       </c>
-      <c r="AD2" s="100"/>
-      <c r="AE2" s="100"/>
-      <c r="AF2" s="101"/>
-      <c r="AG2" s="124">
+      <c r="AD2" s="118"/>
+      <c r="AE2" s="118"/>
+      <c r="AF2" s="119"/>
+      <c r="AG2" s="134">
         <f ca="1">IF(INDIRECT("'Revision history'!AG2")&lt;&gt;"",INDIRECT("'Revision history'!AG2"),"")</f>
         <v>44833</v>
       </c>
-      <c r="AH2" s="125"/>
-      <c r="AI2" s="126"/>
+      <c r="AH2" s="135"/>
+      <c r="AI2" s="136"/>
     </row>
     <row r="3" spans="1:58" s="19" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="122" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!A3")&lt;&gt;"",INDIRECT("'Revision history'!A3"),"")</f>
         <v>Sub-system name</v>
       </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="84" t="str">
+      <c r="B3" s="123"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="102" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!E3")&lt;&gt;"",INDIRECT("'Revision history'!E3"),"")</f>
         <v>Client Management System</v>
       </c>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="136"/>
-      <c r="S3" s="61"/>
-      <c r="T3" s="62"/>
-      <c r="U3" s="62"/>
-      <c r="V3" s="62"/>
-      <c r="W3" s="62"/>
-      <c r="X3" s="62"/>
-      <c r="Y3" s="62"/>
-      <c r="Z3" s="63"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="132"/>
+      <c r="Q3" s="132"/>
+      <c r="R3" s="133"/>
+      <c r="S3" s="79"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="80"/>
+      <c r="X3" s="80"/>
+      <c r="Y3" s="80"/>
+      <c r="Z3" s="81"/>
       <c r="AA3" s="122"/>
-      <c r="AB3" s="123"/>
-      <c r="AC3" s="99" t="str">
+      <c r="AB3" s="124"/>
+      <c r="AC3" s="117" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AC3")&lt;&gt;"",INDIRECT("'Revision history'!AC3"),"")</f>
         <v/>
       </c>
-      <c r="AD3" s="100"/>
-      <c r="AE3" s="100"/>
-      <c r="AF3" s="101"/>
-      <c r="AG3" s="124" t="str">
+      <c r="AD3" s="118"/>
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="119"/>
+      <c r="AG3" s="134" t="str">
         <f ca="1">IF(INDIRECT("'Revision history'!AG3")&lt;&gt;"",INDIRECT("'Revision history'!AG3"),"")</f>
         <v/>
       </c>
-      <c r="AH3" s="125"/>
-      <c r="AI3" s="126"/>
+      <c r="AH3" s="135"/>
+      <c r="AI3" s="136"/>
     </row>
     <row r="4" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="17"/>
@@ -6613,26 +6613,26 @@
     <row r="10" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
-      <c r="C10" s="140" t="s">
+      <c r="C10" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="141"/>
-      <c r="E10" s="141"/>
-      <c r="F10" s="141"/>
-      <c r="G10" s="142"/>
-      <c r="H10" s="115" t="s">
+      <c r="D10" s="144"/>
+      <c r="E10" s="144"/>
+      <c r="F10" s="144"/>
+      <c r="G10" s="145"/>
+      <c r="H10" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="116"/>
-      <c r="J10" s="116"/>
-      <c r="K10" s="116"/>
-      <c r="L10" s="116"/>
-      <c r="M10" s="116"/>
-      <c r="N10" s="116"/>
-      <c r="O10" s="116"/>
-      <c r="P10" s="116"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="117"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="64"/>
+      <c r="Q10" s="64"/>
+      <c r="R10" s="65"/>
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
       <c r="U10" s="17"/>
@@ -6677,26 +6677,26 @@
     <row r="11" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
-      <c r="C11" s="140" t="s">
+      <c r="C11" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="141"/>
-      <c r="E11" s="141"/>
-      <c r="F11" s="141"/>
-      <c r="G11" s="142"/>
-      <c r="H11" s="155" t="s">
+      <c r="D11" s="144"/>
+      <c r="E11" s="144"/>
+      <c r="F11" s="144"/>
+      <c r="G11" s="145"/>
+      <c r="H11" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="116"/>
-      <c r="J11" s="116"/>
-      <c r="K11" s="116"/>
-      <c r="L11" s="116"/>
-      <c r="M11" s="116"/>
-      <c r="N11" s="116"/>
-      <c r="O11" s="116"/>
-      <c r="P11" s="116"/>
-      <c r="Q11" s="116"/>
-      <c r="R11" s="117"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="65"/>
       <c r="S11" s="17"/>
       <c r="T11" s="17"/>
       <c r="U11" s="17"/>
@@ -6983,44 +6983,44 @@
     <row r="16" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
-      <c r="C16" s="156" t="s">
+      <c r="C16" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="158" t="s">
+      <c r="D16" s="137" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="159"/>
-      <c r="F16" s="147"/>
-      <c r="G16" s="158" t="s">
+      <c r="E16" s="138"/>
+      <c r="F16" s="139"/>
+      <c r="G16" s="137" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="147"/>
-      <c r="L16" s="158" t="s">
+      <c r="H16" s="138"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="138"/>
+      <c r="K16" s="139"/>
+      <c r="L16" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="M16" s="159"/>
-      <c r="N16" s="159"/>
-      <c r="O16" s="159"/>
-      <c r="P16" s="159"/>
-      <c r="Q16" s="159"/>
-      <c r="R16" s="159"/>
-      <c r="S16" s="159"/>
-      <c r="T16" s="159"/>
-      <c r="U16" s="159"/>
-      <c r="V16" s="147"/>
-      <c r="W16" s="158" t="s">
+      <c r="M16" s="138"/>
+      <c r="N16" s="138"/>
+      <c r="O16" s="138"/>
+      <c r="P16" s="138"/>
+      <c r="Q16" s="138"/>
+      <c r="R16" s="138"/>
+      <c r="S16" s="138"/>
+      <c r="T16" s="138"/>
+      <c r="U16" s="138"/>
+      <c r="V16" s="139"/>
+      <c r="W16" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="X16" s="159"/>
-      <c r="Y16" s="147"/>
-      <c r="Z16" s="146" t="s">
+      <c r="X16" s="138"/>
+      <c r="Y16" s="139"/>
+      <c r="Z16" s="149" t="s">
         <v>16</v>
       </c>
-      <c r="AA16" s="147"/>
-      <c r="AB16" s="146" t="s">
+      <c r="AA16" s="139"/>
+      <c r="AB16" s="149" t="s">
         <v>17</v>
       </c>
       <c r="AC16" s="150"/>
@@ -7032,62 +7032,62 @@
       <c r="AI16" s="150"/>
       <c r="AJ16" s="150"/>
       <c r="AK16" s="151"/>
-      <c r="AL16" s="140" t="s">
+      <c r="AL16" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="AM16" s="141"/>
-      <c r="AN16" s="141"/>
-      <c r="AO16" s="141"/>
-      <c r="AP16" s="141"/>
-      <c r="AQ16" s="141"/>
-      <c r="AR16" s="142"/>
-      <c r="AS16" s="140" t="s">
+      <c r="AM16" s="144"/>
+      <c r="AN16" s="144"/>
+      <c r="AO16" s="144"/>
+      <c r="AP16" s="144"/>
+      <c r="AQ16" s="144"/>
+      <c r="AR16" s="145"/>
+      <c r="AS16" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="AT16" s="141"/>
-      <c r="AU16" s="141"/>
-      <c r="AV16" s="141"/>
-      <c r="AW16" s="141"/>
-      <c r="AX16" s="142"/>
-      <c r="AY16" s="137" t="s">
+      <c r="AT16" s="144"/>
+      <c r="AU16" s="144"/>
+      <c r="AV16" s="144"/>
+      <c r="AW16" s="144"/>
+      <c r="AX16" s="145"/>
+      <c r="AY16" s="155" t="s">
         <v>44</v>
       </c>
-      <c r="AZ16" s="138"/>
-      <c r="BA16" s="138"/>
-      <c r="BB16" s="138"/>
-      <c r="BC16" s="138"/>
-      <c r="BD16" s="138"/>
-      <c r="BE16" s="139"/>
+      <c r="AZ16" s="156"/>
+      <c r="BA16" s="156"/>
+      <c r="BB16" s="156"/>
+      <c r="BC16" s="156"/>
+      <c r="BD16" s="156"/>
+      <c r="BE16" s="157"/>
       <c r="BF16" s="17"/>
     </row>
     <row r="17" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
-      <c r="C17" s="157"/>
-      <c r="D17" s="148"/>
-      <c r="E17" s="160"/>
-      <c r="F17" s="149"/>
-      <c r="G17" s="148"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="160"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="149"/>
-      <c r="L17" s="148"/>
-      <c r="M17" s="160"/>
-      <c r="N17" s="160"/>
-      <c r="O17" s="160"/>
-      <c r="P17" s="160"/>
-      <c r="Q17" s="160"/>
-      <c r="R17" s="160"/>
-      <c r="S17" s="160"/>
-      <c r="T17" s="160"/>
-      <c r="U17" s="160"/>
-      <c r="V17" s="149"/>
-      <c r="W17" s="148"/>
-      <c r="X17" s="160"/>
-      <c r="Y17" s="149"/>
-      <c r="Z17" s="148"/>
-      <c r="AA17" s="149"/>
+      <c r="C17" s="148"/>
+      <c r="D17" s="140"/>
+      <c r="E17" s="141"/>
+      <c r="F17" s="142"/>
+      <c r="G17" s="140"/>
+      <c r="H17" s="141"/>
+      <c r="I17" s="141"/>
+      <c r="J17" s="141"/>
+      <c r="K17" s="142"/>
+      <c r="L17" s="140"/>
+      <c r="M17" s="141"/>
+      <c r="N17" s="141"/>
+      <c r="O17" s="141"/>
+      <c r="P17" s="141"/>
+      <c r="Q17" s="141"/>
+      <c r="R17" s="141"/>
+      <c r="S17" s="141"/>
+      <c r="T17" s="141"/>
+      <c r="U17" s="141"/>
+      <c r="V17" s="142"/>
+      <c r="W17" s="140"/>
+      <c r="X17" s="141"/>
+      <c r="Y17" s="142"/>
+      <c r="Z17" s="140"/>
+      <c r="AA17" s="142"/>
       <c r="AB17" s="152"/>
       <c r="AC17" s="153"/>
       <c r="AD17" s="153"/>
@@ -7098,40 +7098,40 @@
       <c r="AI17" s="153"/>
       <c r="AJ17" s="153"/>
       <c r="AK17" s="154"/>
-      <c r="AL17" s="140" t="s">
+      <c r="AL17" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="AM17" s="141"/>
-      <c r="AN17" s="140" t="s">
+      <c r="AM17" s="144"/>
+      <c r="AN17" s="143" t="s">
         <v>21</v>
       </c>
-      <c r="AO17" s="141"/>
-      <c r="AP17" s="140" t="s">
+      <c r="AO17" s="144"/>
+      <c r="AP17" s="143" t="s">
         <v>22</v>
       </c>
-      <c r="AQ17" s="141"/>
-      <c r="AR17" s="142"/>
-      <c r="AS17" s="140" t="s">
+      <c r="AQ17" s="144"/>
+      <c r="AR17" s="145"/>
+      <c r="AS17" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="AT17" s="141"/>
-      <c r="AU17" s="142"/>
-      <c r="AV17" s="141" t="s">
+      <c r="AT17" s="144"/>
+      <c r="AU17" s="145"/>
+      <c r="AV17" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="AW17" s="141"/>
-      <c r="AX17" s="142"/>
-      <c r="AY17" s="137" t="s">
+      <c r="AW17" s="144"/>
+      <c r="AX17" s="145"/>
+      <c r="AY17" s="155" t="s">
         <v>45</v>
       </c>
-      <c r="AZ17" s="138"/>
-      <c r="BA17" s="139"/>
-      <c r="BB17" s="143" t="s">
+      <c r="AZ17" s="156"/>
+      <c r="BA17" s="157"/>
+      <c r="BB17" s="158" t="s">
         <v>46</v>
       </c>
-      <c r="BC17" s="144"/>
-      <c r="BD17" s="144"/>
-      <c r="BE17" s="145"/>
+      <c r="BC17" s="159"/>
+      <c r="BD17" s="159"/>
+      <c r="BE17" s="160"/>
       <c r="BF17" s="17"/>
     </row>
     <row r="18" spans="1:58" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7140,52 +7140,52 @@
       <c r="C18" s="21">
         <v>1</v>
       </c>
-      <c r="D18" s="115" t="s">
+      <c r="D18" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="116"/>
-      <c r="F18" s="117"/>
-      <c r="G18" s="115" t="s">
+      <c r="E18" s="64"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="116"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="116"/>
-      <c r="K18" s="117"/>
-      <c r="L18" s="118" t="s">
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="M18" s="119"/>
-      <c r="N18" s="119"/>
-      <c r="O18" s="119"/>
-      <c r="P18" s="119"/>
-      <c r="Q18" s="119"/>
-      <c r="R18" s="119"/>
-      <c r="S18" s="119"/>
-      <c r="T18" s="119"/>
-      <c r="U18" s="119"/>
-      <c r="V18" s="120"/>
-      <c r="W18" s="115" t="s">
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="67"/>
+      <c r="P18" s="67"/>
+      <c r="Q18" s="67"/>
+      <c r="R18" s="67"/>
+      <c r="S18" s="67"/>
+      <c r="T18" s="67"/>
+      <c r="U18" s="67"/>
+      <c r="V18" s="68"/>
+      <c r="W18" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="X18" s="116"/>
-      <c r="Y18" s="117"/>
-      <c r="Z18" s="115" t="s">
+      <c r="X18" s="64"/>
+      <c r="Y18" s="65"/>
+      <c r="Z18" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="AA18" s="117"/>
-      <c r="AB18" s="118" t="s">
+      <c r="AA18" s="65"/>
+      <c r="AB18" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="AC18" s="119"/>
-      <c r="AD18" s="119"/>
-      <c r="AE18" s="119"/>
-      <c r="AF18" s="119"/>
-      <c r="AG18" s="119"/>
-      <c r="AH18" s="119"/>
-      <c r="AI18" s="119"/>
-      <c r="AJ18" s="119"/>
-      <c r="AK18" s="120"/>
+      <c r="AC18" s="67"/>
+      <c r="AD18" s="67"/>
+      <c r="AE18" s="67"/>
+      <c r="AF18" s="67"/>
+      <c r="AG18" s="67"/>
+      <c r="AH18" s="67"/>
+      <c r="AI18" s="67"/>
+      <c r="AJ18" s="67"/>
+      <c r="AK18" s="68"/>
       <c r="AL18" s="22" t="s">
         <v>2</v>
       </c>
@@ -7194,32 +7194,32 @@
         <v>30</v>
       </c>
       <c r="AO18" s="23"/>
-      <c r="AP18" s="118" t="s">
+      <c r="AP18" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AQ18" s="119"/>
-      <c r="AR18" s="120"/>
-      <c r="AS18" s="115" t="s">
+      <c r="AQ18" s="67"/>
+      <c r="AR18" s="68"/>
+      <c r="AS18" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="AT18" s="116"/>
-      <c r="AU18" s="117"/>
-      <c r="AV18" s="115" t="s">
+      <c r="AT18" s="64"/>
+      <c r="AU18" s="65"/>
+      <c r="AV18" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="AW18" s="116"/>
-      <c r="AX18" s="117"/>
-      <c r="AY18" s="115" t="s">
+      <c r="AW18" s="64"/>
+      <c r="AX18" s="65"/>
+      <c r="AY18" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="AZ18" s="116"/>
-      <c r="BA18" s="117"/>
-      <c r="BB18" s="115" t="s">
+      <c r="AZ18" s="64"/>
+      <c r="BA18" s="65"/>
+      <c r="BB18" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="BC18" s="116"/>
-      <c r="BD18" s="116"/>
-      <c r="BE18" s="117"/>
+      <c r="BC18" s="64"/>
+      <c r="BD18" s="64"/>
+      <c r="BE18" s="65"/>
       <c r="BF18" s="20"/>
     </row>
     <row r="19" spans="1:58" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7228,52 +7228,52 @@
       <c r="C19" s="21">
         <v>2</v>
       </c>
-      <c r="D19" s="115" t="s">
+      <c r="D19" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="116"/>
-      <c r="F19" s="117"/>
-      <c r="G19" s="115" t="s">
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="116"/>
-      <c r="I19" s="116"/>
-      <c r="J19" s="116"/>
-      <c r="K19" s="117"/>
-      <c r="L19" s="118" t="s">
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="M19" s="119"/>
-      <c r="N19" s="119"/>
-      <c r="O19" s="119"/>
-      <c r="P19" s="119"/>
-      <c r="Q19" s="119"/>
-      <c r="R19" s="119"/>
-      <c r="S19" s="119"/>
-      <c r="T19" s="119"/>
-      <c r="U19" s="119"/>
-      <c r="V19" s="120"/>
-      <c r="W19" s="115" t="s">
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="67"/>
+      <c r="P19" s="67"/>
+      <c r="Q19" s="67"/>
+      <c r="R19" s="67"/>
+      <c r="S19" s="67"/>
+      <c r="T19" s="67"/>
+      <c r="U19" s="67"/>
+      <c r="V19" s="68"/>
+      <c r="W19" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="X19" s="116"/>
-      <c r="Y19" s="117"/>
-      <c r="Z19" s="115" t="s">
+      <c r="X19" s="64"/>
+      <c r="Y19" s="65"/>
+      <c r="Z19" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="AA19" s="117"/>
-      <c r="AB19" s="118" t="s">
+      <c r="AA19" s="65"/>
+      <c r="AB19" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="AC19" s="119"/>
-      <c r="AD19" s="119"/>
-      <c r="AE19" s="119"/>
-      <c r="AF19" s="119"/>
-      <c r="AG19" s="119"/>
-      <c r="AH19" s="119"/>
-      <c r="AI19" s="119"/>
-      <c r="AJ19" s="119"/>
-      <c r="AK19" s="120"/>
+      <c r="AC19" s="67"/>
+      <c r="AD19" s="67"/>
+      <c r="AE19" s="67"/>
+      <c r="AF19" s="67"/>
+      <c r="AG19" s="67"/>
+      <c r="AH19" s="67"/>
+      <c r="AI19" s="67"/>
+      <c r="AJ19" s="67"/>
+      <c r="AK19" s="68"/>
       <c r="AL19" s="22" t="s">
         <v>2</v>
       </c>
@@ -7282,32 +7282,32 @@
         <v>30</v>
       </c>
       <c r="AO19" s="23"/>
-      <c r="AP19" s="118" t="s">
+      <c r="AP19" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AQ19" s="119"/>
-      <c r="AR19" s="120"/>
-      <c r="AS19" s="115" t="s">
+      <c r="AQ19" s="67"/>
+      <c r="AR19" s="68"/>
+      <c r="AS19" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="AT19" s="116"/>
-      <c r="AU19" s="117"/>
-      <c r="AV19" s="115" t="s">
+      <c r="AT19" s="64"/>
+      <c r="AU19" s="65"/>
+      <c r="AV19" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="AW19" s="116"/>
-      <c r="AX19" s="117"/>
-      <c r="AY19" s="115" t="s">
+      <c r="AW19" s="64"/>
+      <c r="AX19" s="65"/>
+      <c r="AY19" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="AZ19" s="116"/>
-      <c r="BA19" s="117"/>
-      <c r="BB19" s="115" t="s">
+      <c r="AZ19" s="64"/>
+      <c r="BA19" s="65"/>
+      <c r="BB19" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="BC19" s="116"/>
-      <c r="BD19" s="116"/>
-      <c r="BE19" s="117"/>
+      <c r="BC19" s="64"/>
+      <c r="BD19" s="64"/>
+      <c r="BE19" s="65"/>
       <c r="BF19" s="20"/>
     </row>
     <row r="20" spans="1:58" s="24" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -7316,52 +7316,52 @@
       <c r="C20" s="21">
         <v>3</v>
       </c>
-      <c r="D20" s="115" t="s">
+      <c r="D20" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="116"/>
-      <c r="F20" s="117"/>
-      <c r="G20" s="115" t="s">
+      <c r="E20" s="64"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="H20" s="116"/>
-      <c r="I20" s="116"/>
-      <c r="J20" s="116"/>
-      <c r="K20" s="117"/>
-      <c r="L20" s="118" t="s">
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="M20" s="119"/>
-      <c r="N20" s="119"/>
-      <c r="O20" s="119"/>
-      <c r="P20" s="119"/>
-      <c r="Q20" s="119"/>
-      <c r="R20" s="119"/>
-      <c r="S20" s="119"/>
-      <c r="T20" s="119"/>
-      <c r="U20" s="119"/>
-      <c r="V20" s="120"/>
-      <c r="W20" s="115" t="s">
+      <c r="M20" s="67"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="67"/>
+      <c r="S20" s="67"/>
+      <c r="T20" s="67"/>
+      <c r="U20" s="67"/>
+      <c r="V20" s="68"/>
+      <c r="W20" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="X20" s="116"/>
-      <c r="Y20" s="117"/>
-      <c r="Z20" s="115" t="s">
+      <c r="X20" s="64"/>
+      <c r="Y20" s="65"/>
+      <c r="Z20" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="AA20" s="117"/>
-      <c r="AB20" s="118" t="s">
+      <c r="AA20" s="65"/>
+      <c r="AB20" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="AC20" s="119"/>
-      <c r="AD20" s="119"/>
-      <c r="AE20" s="119"/>
-      <c r="AF20" s="119"/>
-      <c r="AG20" s="119"/>
-      <c r="AH20" s="119"/>
-      <c r="AI20" s="119"/>
-      <c r="AJ20" s="119"/>
-      <c r="AK20" s="120"/>
+      <c r="AC20" s="67"/>
+      <c r="AD20" s="67"/>
+      <c r="AE20" s="67"/>
+      <c r="AF20" s="67"/>
+      <c r="AG20" s="67"/>
+      <c r="AH20" s="67"/>
+      <c r="AI20" s="67"/>
+      <c r="AJ20" s="67"/>
+      <c r="AK20" s="68"/>
       <c r="AL20" s="22" t="s">
         <v>30</v>
       </c>
@@ -7370,32 +7370,32 @@
         <v>30</v>
       </c>
       <c r="AO20" s="23"/>
-      <c r="AP20" s="118" t="s">
+      <c r="AP20" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AQ20" s="119"/>
-      <c r="AR20" s="120"/>
-      <c r="AS20" s="115" t="s">
+      <c r="AQ20" s="67"/>
+      <c r="AR20" s="68"/>
+      <c r="AS20" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="AT20" s="116"/>
-      <c r="AU20" s="117"/>
-      <c r="AV20" s="115" t="s">
+      <c r="AT20" s="64"/>
+      <c r="AU20" s="65"/>
+      <c r="AV20" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="AW20" s="116"/>
-      <c r="AX20" s="117"/>
-      <c r="AY20" s="115" t="s">
+      <c r="AW20" s="64"/>
+      <c r="AX20" s="65"/>
+      <c r="AY20" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="AZ20" s="116"/>
-      <c r="BA20" s="117"/>
-      <c r="BB20" s="115" t="s">
+      <c r="AZ20" s="64"/>
+      <c r="BA20" s="65"/>
+      <c r="BB20" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="BC20" s="116"/>
-      <c r="BD20" s="116"/>
-      <c r="BE20" s="117"/>
+      <c r="BC20" s="64"/>
+      <c r="BD20" s="64"/>
+      <c r="BE20" s="65"/>
       <c r="BF20" s="20"/>
     </row>
     <row r="21" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -7466,18 +7466,49 @@
     <row r="27" spans="1:58" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="W19:Y19"/>
-    <mergeCell ref="W20:Y20"/>
-    <mergeCell ref="W16:Y17"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="L19:V19"/>
-    <mergeCell ref="L20:V20"/>
-    <mergeCell ref="L16:V17"/>
-    <mergeCell ref="L18:V18"/>
-    <mergeCell ref="G16:K17"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="AY16:BE16"/>
+    <mergeCell ref="AL17:AM17"/>
+    <mergeCell ref="AN17:AO17"/>
+    <mergeCell ref="AP17:AR17"/>
+    <mergeCell ref="AY17:BA17"/>
+    <mergeCell ref="BB17:BE17"/>
+    <mergeCell ref="AL16:AR16"/>
+    <mergeCell ref="AS16:AX16"/>
+    <mergeCell ref="AV17:AX17"/>
+    <mergeCell ref="AS17:AU17"/>
+    <mergeCell ref="BB18:BE18"/>
+    <mergeCell ref="BB19:BE19"/>
+    <mergeCell ref="BB20:BE20"/>
+    <mergeCell ref="AP18:AR18"/>
+    <mergeCell ref="AP19:AR19"/>
+    <mergeCell ref="AP20:AR20"/>
+    <mergeCell ref="AY18:BA18"/>
+    <mergeCell ref="AY19:BA19"/>
+    <mergeCell ref="AY20:BA20"/>
+    <mergeCell ref="AV18:AX18"/>
+    <mergeCell ref="AV19:AX19"/>
+    <mergeCell ref="AV20:AX20"/>
+    <mergeCell ref="AS18:AU18"/>
+    <mergeCell ref="AS19:AU19"/>
+    <mergeCell ref="AS20:AU20"/>
+    <mergeCell ref="AB18:AK18"/>
+    <mergeCell ref="AB19:AK19"/>
+    <mergeCell ref="AB20:AK20"/>
+    <mergeCell ref="Z18:AA18"/>
+    <mergeCell ref="Z19:AA19"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="AG3:AI3"/>
+    <mergeCell ref="AG1:AI1"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="Z16:AA17"/>
+    <mergeCell ref="AB16:AK17"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AC3:AF3"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="S1:Z3"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D19:F19"/>
@@ -7494,52 +7525,21 @@
     <mergeCell ref="D16:F17"/>
     <mergeCell ref="H10:R10"/>
     <mergeCell ref="O1:R3"/>
-    <mergeCell ref="AG3:AI3"/>
-    <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="Z16:AA17"/>
-    <mergeCell ref="AB16:AK17"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AC3:AF3"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="S1:Z3"/>
-    <mergeCell ref="AB18:AK18"/>
-    <mergeCell ref="AB19:AK19"/>
-    <mergeCell ref="AB20:AK20"/>
-    <mergeCell ref="Z18:AA18"/>
-    <mergeCell ref="Z19:AA19"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="BB18:BE18"/>
-    <mergeCell ref="BB19:BE19"/>
-    <mergeCell ref="BB20:BE20"/>
-    <mergeCell ref="AP18:AR18"/>
-    <mergeCell ref="AP19:AR19"/>
-    <mergeCell ref="AP20:AR20"/>
-    <mergeCell ref="AY18:BA18"/>
-    <mergeCell ref="AY19:BA19"/>
-    <mergeCell ref="AY20:BA20"/>
-    <mergeCell ref="AV18:AX18"/>
-    <mergeCell ref="AV19:AX19"/>
-    <mergeCell ref="AV20:AX20"/>
-    <mergeCell ref="AS18:AU18"/>
-    <mergeCell ref="AS19:AU19"/>
-    <mergeCell ref="AS20:AU20"/>
-    <mergeCell ref="AY16:BE16"/>
-    <mergeCell ref="AL17:AM17"/>
-    <mergeCell ref="AN17:AO17"/>
-    <mergeCell ref="AP17:AR17"/>
-    <mergeCell ref="AY17:BA17"/>
-    <mergeCell ref="BB17:BE17"/>
-    <mergeCell ref="AL16:AR16"/>
-    <mergeCell ref="AS16:AX16"/>
-    <mergeCell ref="AV17:AX17"/>
-    <mergeCell ref="AS17:AU17"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="W19:Y19"/>
+    <mergeCell ref="W20:Y20"/>
+    <mergeCell ref="W16:Y17"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="L19:V19"/>
+    <mergeCell ref="L20:V20"/>
+    <mergeCell ref="L16:V17"/>
+    <mergeCell ref="L18:V18"/>
+    <mergeCell ref="G16:K17"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G20:K20"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="W18:W20" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"HTTP,HTTPS"</formula1>
     </dataValidation>
@@ -7549,7 +7549,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C- &amp;P -</oddFooter>
   </headerFooter>

</xml_diff>